<commit_message>
V 0.40-B36 partial update - Add Flight Recorder to create a KML and JSON flight logfile - Add Mouse wheel Inc/Dec for ERA-Trims (also extend to 0.1% readout) - Add Spoilers Voice Out - Update Spoilers and Flaps indication for the End position (out) is now Blue - Fix Spoiler indication (was not active)
</commit_message>
<xml_diff>
--- a/Config/EngineMerge.xlsx
+++ b/Config/EngineMerge.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2987" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3063" uniqueCount="246">
   <si>
     <t>ACFT</t>
   </si>
@@ -750,6 +750,12 @@
   </si>
   <si>
     <t>XPDR</t>
+  </si>
+  <si>
+    <t>SWS Kodiak 100 II</t>
+  </si>
+  <si>
+    <t>Kodiak 100 II Wheel</t>
   </si>
 </sst>
 </file>
@@ -1203,7 +1209,7 @@
   <dimension ref="A1:AK42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5548,6 +5554,117 @@
         <v>65</v>
       </c>
     </row>
+    <row r="39" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C39" s="5">
+        <v>1</v>
+      </c>
+      <c r="D39" s="5">
+        <v>750</v>
+      </c>
+      <c r="E39" s="9">
+        <f t="shared" ref="E39" si="4">D39/C39</f>
+        <v>750</v>
+      </c>
+      <c r="F39" s="16">
+        <v>0</v>
+      </c>
+      <c r="G39" s="3">
+        <v>1</v>
+      </c>
+      <c r="H39" s="3">
+        <v>1</v>
+      </c>
+      <c r="I39" s="3">
+        <v>0</v>
+      </c>
+      <c r="J39" s="14">
+        <v>0</v>
+      </c>
+      <c r="K39" s="14">
+        <v>0</v>
+      </c>
+      <c r="L39" s="14">
+        <v>0</v>
+      </c>
+      <c r="M39" s="14">
+        <v>0</v>
+      </c>
+      <c r="N39" s="3">
+        <v>1</v>
+      </c>
+      <c r="O39" s="3">
+        <v>0</v>
+      </c>
+      <c r="P39" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q39" s="3">
+        <v>1</v>
+      </c>
+      <c r="R39" s="8">
+        <v>1</v>
+      </c>
+      <c r="S39" s="8">
+        <v>0</v>
+      </c>
+      <c r="T39" s="7">
+        <v>0</v>
+      </c>
+      <c r="U39" s="7">
+        <v>0</v>
+      </c>
+      <c r="V39" s="7">
+        <v>0</v>
+      </c>
+      <c r="W39" s="7">
+        <v>0</v>
+      </c>
+      <c r="X39" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y39" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z39" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA39" s="5">
+        <v>1</v>
+      </c>
+      <c r="AB39" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC39" s="6">
+        <v>1</v>
+      </c>
+      <c r="AD39" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE39" s="6">
+        <v>1</v>
+      </c>
+      <c r="AF39" s="6">
+        <v>0</v>
+      </c>
+      <c r="AG39" s="6">
+        <v>0</v>
+      </c>
+      <c r="AH39" s="6">
+        <v>0</v>
+      </c>
+      <c r="AI39" s="15">
+        <v>0</v>
+      </c>
+      <c r="AJ39" t="s">
+        <v>244</v>
+      </c>
+    </row>
     <row r="42" spans="1:37" x14ac:dyDescent="0.25">
       <c r="AB42" t="s">
         <v>204</v>
@@ -5560,10 +5677,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CV38"/>
+  <dimension ref="A1:CV39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K45" sqref="K45"/>
+      <selection activeCell="CV44" sqref="CV44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18050,6 +18167,335 @@
         <v>XCub</v>
       </c>
     </row>
+    <row r="39" spans="1:100" x14ac:dyDescent="0.25">
+      <c r="A39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="F39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="G39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="H39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="I39" s="12">
+        <f>Tabelle1!F39</f>
+        <v>0</v>
+      </c>
+      <c r="J39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="K39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="L39" s="12">
+        <f>Tabelle1!AA39</f>
+        <v>1</v>
+      </c>
+      <c r="M39" s="12">
+        <f>Tabelle1!Z39</f>
+        <v>0</v>
+      </c>
+      <c r="N39" s="12">
+        <f>Tabelle1!R39</f>
+        <v>1</v>
+      </c>
+      <c r="O39" s="12">
+        <f>Tabelle1!S39</f>
+        <v>0</v>
+      </c>
+      <c r="P39" s="12">
+        <f>Tabelle1!AC39</f>
+        <v>1</v>
+      </c>
+      <c r="Q39" s="12">
+        <f>Tabelle1!AE39</f>
+        <v>1</v>
+      </c>
+      <c r="R39" s="12">
+        <f>Tabelle1!T39</f>
+        <v>0</v>
+      </c>
+      <c r="S39" s="12">
+        <f>Tabelle1!P39</f>
+        <v>1</v>
+      </c>
+      <c r="T39" s="12">
+        <f>Tabelle1!L39</f>
+        <v>0</v>
+      </c>
+      <c r="U39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="V39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="W39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="X39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="Z39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AB39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AC39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AE39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AF39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AH39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AI39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AJ39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AK39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AL39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AM39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AN39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AO39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AP39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AQ39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AR39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AS39" s="12">
+        <f>Tabelle1!X39</f>
+        <v>0</v>
+      </c>
+      <c r="AT39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AU39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AV39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AW39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AX39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AY39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AZ39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="BA39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="BB39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="BC39" s="12">
+        <f>Tabelle1!J39</f>
+        <v>0</v>
+      </c>
+      <c r="BD39" s="12">
+        <f>Tabelle1!M39</f>
+        <v>0</v>
+      </c>
+      <c r="BE39" s="12">
+        <f>Tabelle1!AF39</f>
+        <v>0</v>
+      </c>
+      <c r="BF39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="BG39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="BH39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="BI39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="BJ39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="BK39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="BL39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="BM39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="BN39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="BO39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="BP39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="BQ39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="BR39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="BS39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="BT39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="BU39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="BV39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="BW39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="BX39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="BY39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="BZ39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="CA39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="CB39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="CC39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="CD39" s="12">
+        <f>Tabelle1!U39</f>
+        <v>0</v>
+      </c>
+      <c r="CE39" s="12">
+        <f>Tabelle1!V39</f>
+        <v>0</v>
+      </c>
+      <c r="CF39" s="12">
+        <f>Tabelle1!W39</f>
+        <v>0</v>
+      </c>
+      <c r="CG39" s="12">
+        <f>Tabelle1!Y39</f>
+        <v>0</v>
+      </c>
+      <c r="CH39" s="12">
+        <f>Tabelle1!AD39</f>
+        <v>0</v>
+      </c>
+      <c r="CI39" s="12">
+        <f>Tabelle1!N39</f>
+        <v>1</v>
+      </c>
+      <c r="CJ39" s="12">
+        <f>Tabelle1!Q39</f>
+        <v>1</v>
+      </c>
+      <c r="CK39" s="12">
+        <f>Tabelle1!K39</f>
+        <v>0</v>
+      </c>
+      <c r="CL39" s="12">
+        <f>Tabelle1!O39</f>
+        <v>0</v>
+      </c>
+      <c r="CM39" s="12">
+        <f>Tabelle1!AG39</f>
+        <v>0</v>
+      </c>
+      <c r="CN39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="CO39" s="12">
+        <f>Tabelle1!AH39</f>
+        <v>0</v>
+      </c>
+      <c r="CP39" s="12">
+        <f>Tabelle1!AI39</f>
+        <v>0</v>
+      </c>
+      <c r="CQ39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="CR39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="CS39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="CT39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="CU39" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="CV39" t="str">
+        <f>Tabelle1!AJ39</f>
+        <v>SWS Kodiak 100 II</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
- Update FP Capture and Save disabled when on ground - Update QuickGuide Update version tag on build
</commit_message>
<xml_diff>
--- a/Config/EngineMerge.xlsx
+++ b/Config/EngineMerge.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3063" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3102" uniqueCount="247">
   <si>
     <t>ACFT</t>
   </si>
@@ -756,6 +756,9 @@
   </si>
   <si>
     <t>Kodiak 100 II Wheel</t>
+  </si>
+  <si>
+    <t>LOG</t>
   </si>
 </sst>
 </file>
@@ -5677,10 +5680,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CV39"/>
+  <dimension ref="A1:CW39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="CV44" sqref="CV44"/>
+      <selection activeCell="CS41" sqref="CS41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5688,11 +5691,11 @@
     <col min="1" max="75" width="3.7109375" bestFit="1" customWidth="1"/>
     <col min="76" max="77" width="3.7109375" customWidth="1"/>
     <col min="78" max="86" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="87" max="99" width="3.7109375" customWidth="1"/>
-    <col min="100" max="100" width="36.28515625" customWidth="1"/>
+    <col min="87" max="100" width="3.7109375" customWidth="1"/>
+    <col min="101" max="101" width="36.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:100" s="11" customFormat="1" ht="72" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:101" s="11" customFormat="1" ht="72" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>95</v>
       </c>
@@ -5988,13 +5991,16 @@
         <v>243</v>
       </c>
       <c r="CU1" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="CV1" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="CV1" t="s">
+      <c r="CW1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>88</v>
       </c>
@@ -6316,14 +6322,17 @@
         <v>88</v>
       </c>
       <c r="CU2" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="CV2" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="CV2" t="str">
+      <c r="CW2" t="str">
         <f>Tabelle1!AJ2</f>
         <v>Airbus A320 Neo</v>
       </c>
     </row>
-    <row r="3" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>88</v>
       </c>
@@ -6645,14 +6654,17 @@
         <v>88</v>
       </c>
       <c r="CU3" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="CV3" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="CV3" t="str">
+      <c r="CW3" t="str">
         <f>Tabelle1!AJ3</f>
         <v>Boeing 747-8i</v>
       </c>
     </row>
-    <row r="4" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>88</v>
       </c>
@@ -6974,14 +6986,17 @@
         <v>88</v>
       </c>
       <c r="CU4" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="CV4" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="CV4" t="str">
+      <c r="CW4" t="str">
         <f>Tabelle1!AJ4</f>
         <v>Boeing 787-10</v>
       </c>
     </row>
-    <row r="5" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>88</v>
       </c>
@@ -7303,14 +7318,17 @@
         <v>88</v>
       </c>
       <c r="CU5" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="CV5" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="CV5" t="str">
+      <c r="CW5" t="str">
         <f>Tabelle1!AJ5</f>
         <v>Boeing F/A 18E Super Hornet</v>
       </c>
     </row>
-    <row r="6" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>88</v>
       </c>
@@ -7632,14 +7650,17 @@
         <v>88</v>
       </c>
       <c r="CU6" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="CV6" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="CV6" t="str">
+      <c r="CW6" t="str">
         <f>Tabelle1!AJ6</f>
         <v>Baron G58</v>
       </c>
     </row>
-    <row r="7" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>88</v>
       </c>
@@ -7961,14 +7982,17 @@
         <v>88</v>
       </c>
       <c r="CU7" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="CV7" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="CV7" t="str">
+      <c r="CW7" t="str">
         <f>Tabelle1!AJ7</f>
         <v>Bonanza G36</v>
       </c>
     </row>
-    <row r="8" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>88</v>
       </c>
@@ -8290,14 +8314,17 @@
         <v>88</v>
       </c>
       <c r="CU8" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="CV8" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="CV8" t="str">
+      <c r="CW8" t="str">
         <f>Tabelle1!AJ8</f>
         <v>Beechcraft King Air 350i</v>
       </c>
     </row>
-    <row r="9" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>88</v>
       </c>
@@ -8619,14 +8646,17 @@
         <v>88</v>
       </c>
       <c r="CU9" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="CV9" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="CV9" t="str">
+      <c r="CW9" t="str">
         <f>Tabelle1!AJ9</f>
         <v>Cessna 152</v>
       </c>
     </row>
-    <row r="10" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>88</v>
       </c>
@@ -8948,14 +8978,17 @@
         <v>88</v>
       </c>
       <c r="CU10" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="CV10" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="CV10" t="str">
+      <c r="CW10" t="str">
         <f>Tabelle1!AJ10</f>
         <v>Cessna 152 Aero</v>
       </c>
     </row>
-    <row r="11" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>88</v>
       </c>
@@ -9277,14 +9310,17 @@
         <v>88</v>
       </c>
       <c r="CU11" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="CV11" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="CV11" t="str">
+      <c r="CW11" t="str">
         <f>Tabelle1!AJ11</f>
         <v>Cessna 172sp Skyhawk G1000</v>
       </c>
     </row>
-    <row r="12" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>88</v>
       </c>
@@ -9606,14 +9642,17 @@
         <v>88</v>
       </c>
       <c r="CU12" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="CV12" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="CV12" t="str">
+      <c r="CW12" t="str">
         <f>Tabelle1!AJ12</f>
         <v>Cessna 172sp Skyhawk</v>
       </c>
     </row>
-    <row r="13" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>88</v>
       </c>
@@ -9935,14 +9974,17 @@
         <v>88</v>
       </c>
       <c r="CU13" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="CV13" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="CV13" t="str">
+      <c r="CW13" t="str">
         <f>Tabelle1!AJ13</f>
         <v>Cessna 208B Grand Caravan EX</v>
       </c>
     </row>
-    <row r="14" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>88</v>
       </c>
@@ -10264,14 +10306,17 @@
         <v>88</v>
       </c>
       <c r="CU14" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="CV14" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="CV14" t="str">
+      <c r="CW14" t="str">
         <f>Tabelle1!AJ14</f>
         <v>Cessna CJ4 Citation</v>
       </c>
     </row>
-    <row r="15" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>88</v>
       </c>
@@ -10593,14 +10638,17 @@
         <v>88</v>
       </c>
       <c r="CU15" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="CV15" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="CV15" t="str">
+      <c r="CW15" t="str">
         <f>Tabelle1!AJ15</f>
         <v>Cessna Longitude</v>
       </c>
     </row>
-    <row r="16" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>88</v>
       </c>
@@ -10922,14 +10970,17 @@
         <v>88</v>
       </c>
       <c r="CU16" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="CV16" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="CV16" t="str">
+      <c r="CW16" t="str">
         <f>Tabelle1!AJ16</f>
         <v>DA40-NG</v>
       </c>
     </row>
-    <row r="17" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>88</v>
       </c>
@@ -11251,14 +11302,17 @@
         <v>88</v>
       </c>
       <c r="CU17" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="CV17" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="CV17" t="str">
+      <c r="CW17" t="str">
         <f>Tabelle1!AJ17</f>
         <v>DA40 TDI</v>
       </c>
     </row>
-    <row r="18" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>88</v>
       </c>
@@ -11580,14 +11634,17 @@
         <v>88</v>
       </c>
       <c r="CU18" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="CV18" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="CV18" t="str">
+      <c r="CW18" t="str">
         <f>Tabelle1!AJ18</f>
         <v>DA62</v>
       </c>
     </row>
-    <row r="19" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>88</v>
       </c>
@@ -11909,14 +11966,17 @@
         <v>88</v>
       </c>
       <c r="CU19" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="CV19" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="CV19" t="str">
+      <c r="CW19" t="str">
         <f>Tabelle1!AJ19</f>
         <v>DR400</v>
       </c>
     </row>
-    <row r="20" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>88</v>
       </c>
@@ -12238,14 +12298,17 @@
         <v>88</v>
       </c>
       <c r="CU20" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="CV20" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="CV20" t="str">
+      <c r="CW20" t="str">
         <f>Tabelle1!AJ20</f>
         <v>DV20</v>
       </c>
     </row>
-    <row r="21" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>88</v>
       </c>
@@ -12567,14 +12630,17 @@
         <v>88</v>
       </c>
       <c r="CU21" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="CV21" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="CV21" t="str">
+      <c r="CW21" t="str">
         <f>Tabelle1!AJ21</f>
         <v>Extra 330</v>
       </c>
     </row>
-    <row r="22" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>88</v>
       </c>
@@ -12896,14 +12962,17 @@
         <v>88</v>
       </c>
       <c r="CU22" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="CV22" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="CV22" t="str">
+      <c r="CW22" t="str">
         <f>Tabelle1!AJ22</f>
         <v>FlightDesignCT</v>
       </c>
     </row>
-    <row r="23" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>88</v>
       </c>
@@ -13225,14 +13294,17 @@
         <v>88</v>
       </c>
       <c r="CU23" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="CV23" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="CV23" t="str">
+      <c r="CW23" t="str">
         <f>Tabelle1!AJ23</f>
         <v>Icon A5</v>
       </c>
     </row>
-    <row r="24" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>88</v>
       </c>
@@ -13554,14 +13626,17 @@
         <v>88</v>
       </c>
       <c r="CU24" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="CV24" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="CV24" t="str">
+      <c r="CW24" t="str">
         <f>Tabelle1!AJ24</f>
         <v>Mudry Cap 10 C</v>
       </c>
     </row>
-    <row r="25" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>88</v>
       </c>
@@ -13883,14 +13958,17 @@
         <v>88</v>
       </c>
       <c r="CU25" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="CV25" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="CV25" t="str">
+      <c r="CW25" t="str">
         <f>Tabelle1!AJ25</f>
         <v>Pilatus PC-6 Gauge</v>
       </c>
     </row>
-    <row r="26" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>88</v>
       </c>
@@ -14212,14 +14290,17 @@
         <v>88</v>
       </c>
       <c r="CU26" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="CV26" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="CV26" t="str">
+      <c r="CW26" t="str">
         <f>Tabelle1!AJ26</f>
         <v>Pilatus PC-6 G950</v>
       </c>
     </row>
-    <row r="27" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>88</v>
       </c>
@@ -14541,14 +14622,17 @@
         <v>88</v>
       </c>
       <c r="CU27" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="CV27" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="CV27" t="str">
+      <c r="CW27" t="str">
         <f>Tabelle1!AJ27</f>
         <v>Pipistrel Alpha Electro</v>
       </c>
     </row>
-    <row r="28" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>88</v>
       </c>
@@ -14870,14 +14954,17 @@
         <v>88</v>
       </c>
       <c r="CU28" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="CV28" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="CV28" t="str">
+      <c r="CW28" t="str">
         <f>Tabelle1!AJ28</f>
         <v>Pitts Special 1S</v>
       </c>
     </row>
-    <row r="29" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>88</v>
       </c>
@@ -15199,14 +15286,17 @@
         <v>88</v>
       </c>
       <c r="CU29" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="CV29" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="CV29" t="str">
+      <c r="CW29" t="str">
         <f>Tabelle1!AJ29</f>
         <v>Pitts Special S2S</v>
       </c>
     </row>
-    <row r="30" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>88</v>
       </c>
@@ -15528,14 +15618,17 @@
         <v>88</v>
       </c>
       <c r="CU30" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="CV30" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="CV30" t="str">
+      <c r="CW30" t="str">
         <f>Tabelle1!AJ30</f>
         <v>Savage Cub</v>
       </c>
     </row>
-    <row r="31" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>88</v>
       </c>
@@ -15857,14 +15950,17 @@
         <v>88</v>
       </c>
       <c r="CU31" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="CV31" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="CV31" t="str">
+      <c r="CW31" t="str">
         <f>Tabelle1!AJ31</f>
         <v>Savage Shock Ultra</v>
       </c>
     </row>
-    <row r="32" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>88</v>
       </c>
@@ -16186,14 +16282,17 @@
         <v>88</v>
       </c>
       <c r="CU32" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="CV32" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="CV32" t="str">
+      <c r="CW32" t="str">
         <f>Tabelle1!AJ32</f>
         <v>SR22</v>
       </c>
     </row>
-    <row r="33" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>88</v>
       </c>
@@ -16515,14 +16614,17 @@
         <v>88</v>
       </c>
       <c r="CU33" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="CV33" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="CV33" t="str">
+      <c r="CW33" t="str">
         <f>Tabelle1!AJ33</f>
         <v>TBM 930</v>
       </c>
     </row>
-    <row r="34" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>88</v>
       </c>
@@ -16844,14 +16946,17 @@
         <v>88</v>
       </c>
       <c r="CU34" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="CV34" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="CV34" t="str">
+      <c r="CW34" t="str">
         <f>Tabelle1!AJ34</f>
         <v>Vertigo</v>
       </c>
     </row>
-    <row r="35" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
         <v>88</v>
       </c>
@@ -17173,14 +17278,17 @@
         <v>88</v>
       </c>
       <c r="CU35" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="CV35" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="CV35" t="str">
+      <c r="CW35" t="str">
         <f>Tabelle1!AJ35</f>
         <v>VL3</v>
       </c>
     </row>
-    <row r="36" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>88</v>
       </c>
@@ -17502,14 +17610,17 @@
         <v>88</v>
       </c>
       <c r="CU36" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="CV36" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="CV36" t="str">
+      <c r="CW36" t="str">
         <f>Tabelle1!AJ36</f>
         <v>Volocity</v>
       </c>
     </row>
-    <row r="37" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
         <v>88</v>
       </c>
@@ -17831,14 +17942,17 @@
         <v>88</v>
       </c>
       <c r="CU37" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="CV37" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="CV37" t="str">
+      <c r="CW37" t="str">
         <f>Tabelle1!AJ37</f>
         <v>NXCub</v>
       </c>
     </row>
-    <row r="38" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>88</v>
       </c>
@@ -18160,14 +18274,17 @@
         <v>88</v>
       </c>
       <c r="CU38" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="CV38" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="CV38" t="str">
+      <c r="CW38" t="str">
         <f>Tabelle1!AJ38</f>
         <v>XCub</v>
       </c>
     </row>
-    <row r="39" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>88</v>
       </c>
@@ -18489,9 +18606,12 @@
         <v>88</v>
       </c>
       <c r="CU39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="CV39" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="CV39" t="str">
+      <c r="CW39" t="str">
         <f>Tabelle1!AJ39</f>
         <v>SWS Kodiak 100 II</v>
       </c>

</xml_diff>

<commit_message>
V 0.45-B42 Release and SU8 Compatibility Check - Add Graph items for many of % items and others where ranges are known - Add 'ESI' graphical item (Attitude/FPA) - Add Wind arrow for the Wind Dir@Speed item (Wind direction the Acft will see) - Add Cowl Flaps as % Graph - Update Set HudBar visible in Windows Taskbar - Update IAS text gets Orange (5kt before) and Red (Stall) when approaching Config Stall Speed - Fix Flight Path Angle calculation - Fix Layout issue with Trim items - Refacturing disposal of not shown items - SU8 Compatibility Check - Update QuickGuide
</commit_message>
<xml_diff>
--- a/Config/EngineMerge.xlsx
+++ b/Config/EngineMerge.xlsx
@@ -11,14 +11,14 @@
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$AN$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$AO$1</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3348" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3790" uniqueCount="276">
   <si>
     <t>ACFT</t>
   </si>
@@ -794,9 +794,6 @@
     <t>VARIO_MPS</t>
   </si>
   <si>
-    <t>VARIO_TE</t>
-  </si>
-  <si>
     <t>Glider</t>
   </si>
   <si>
@@ -807,6 +804,48 @@
   </si>
   <si>
     <t>Any</t>
+  </si>
+  <si>
+    <t>FUEL_ANI</t>
+  </si>
+  <si>
+    <t>VARIO_KTS</t>
+  </si>
+  <si>
+    <t>VARIO_ANI</t>
+  </si>
+  <si>
+    <t>N1_ANI</t>
+  </si>
+  <si>
+    <t>N2_ANI</t>
+  </si>
+  <si>
+    <t>ERPM_ANI</t>
+  </si>
+  <si>
+    <t>PRPM_ANI</t>
+  </si>
+  <si>
+    <t>COWL_ANI</t>
+  </si>
+  <si>
+    <t>TORQP_ANI</t>
+  </si>
+  <si>
+    <t>AFTB_ANI</t>
+  </si>
+  <si>
+    <t>FLAPS_ANI</t>
+  </si>
+  <si>
+    <t>SPOILER_ANI</t>
+  </si>
+  <si>
+    <t>ESI_ANI</t>
+  </si>
+  <si>
+    <t>VARIO MPS</t>
   </si>
 </sst>
 </file>
@@ -833,7 +872,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -906,6 +945,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -935,7 +980,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -959,6 +1004,46 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Komma" xfId="1" builtinId="3"/>
@@ -1264,149 +1349,155 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO42"/>
+  <dimension ref="A1:AP42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+      <selection activeCell="AN39" sqref="AN39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.28515625" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" customWidth="1"/>
-    <col min="5" max="5" width="10" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10" style="17" customWidth="1"/>
-    <col min="12" max="12" width="10.85546875" customWidth="1"/>
-    <col min="28" max="28" width="11.42578125" customWidth="1"/>
-    <col min="40" max="41" width="36.28515625" customWidth="1"/>
+    <col min="2" max="3" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.7109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="31" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="3.28515625" customWidth="1"/>
+    <col min="33" max="39" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="3.7109375" customWidth="1"/>
+    <col min="41" max="42" width="36.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:42" s="11" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="23" t="s">
         <v>225</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="K1" s="23" t="s">
         <v>233</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="L1" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="M1" s="23" t="s">
         <v>223</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="22" t="s">
         <v>226</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="22" t="s">
         <v>234</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="22" t="s">
         <v>222</v>
       </c>
-      <c r="R1" s="18" t="s">
+      <c r="R1" s="24" t="s">
         <v>253</v>
       </c>
-      <c r="S1" s="18" t="s">
+      <c r="S1" s="24" t="s">
         <v>254</v>
       </c>
-      <c r="T1" s="18" t="s">
+      <c r="T1" s="24" t="s">
         <v>255</v>
       </c>
-      <c r="U1" s="18" t="s">
+      <c r="U1" s="24" t="s">
         <v>256</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="V1" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="W1" s="8" t="s">
+      <c r="W1" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="X1" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="Y1" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="Z1" s="7" t="s">
+      <c r="Z1" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="AA1" s="7" t="s">
+      <c r="AA1" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AB1" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AC1" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="AD1" s="5" t="s">
+      <c r="AD1" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="AE1" s="5" t="s">
+      <c r="AE1" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="AF1" s="5" t="s">
+      <c r="AF1" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="AG1" s="6" t="s">
+      <c r="AG1" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="AH1" s="6" t="s">
+      <c r="AH1" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="AI1" s="6" t="s">
+      <c r="AI1" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="AJ1" s="6" t="s">
+      <c r="AJ1" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="AK1" s="6" t="s">
+      <c r="AK1" s="29" t="s">
         <v>229</v>
       </c>
-      <c r="AL1" s="6" t="s">
+      <c r="AL1" s="29" t="s">
         <v>230</v>
       </c>
-      <c r="AM1" s="15" t="s">
+      <c r="AM1" s="30" t="s">
         <v>232</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AN1" s="31" t="s">
+        <v>275</v>
+      </c>
+      <c r="AO1" s="11" t="s">
         <v>220</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" s="11" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>20</v>
       </c>
@@ -1525,14 +1616,17 @@
       <c r="AM2" s="15">
         <v>1</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AN2" s="32">
+        <v>0</v>
+      </c>
+      <c r="AO2" t="s">
         <v>196</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="AP2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>22</v>
       </c>
@@ -1651,14 +1745,17 @@
       <c r="AM3" s="15">
         <v>1</v>
       </c>
-      <c r="AN3" t="s">
+      <c r="AN3" s="32">
+        <v>0</v>
+      </c>
+      <c r="AO3" t="s">
         <v>198</v>
       </c>
-      <c r="AO3" t="s">
+      <c r="AP3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>21</v>
       </c>
@@ -1777,14 +1874,17 @@
       <c r="AM4" s="15">
         <v>1</v>
       </c>
-      <c r="AN4" t="s">
+      <c r="AN4" s="32">
+        <v>0</v>
+      </c>
+      <c r="AO4" t="s">
         <v>197</v>
       </c>
-      <c r="AO4" t="s">
+      <c r="AP4" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>211</v>
       </c>
@@ -1903,14 +2003,17 @@
       <c r="AM5" s="15">
         <v>1</v>
       </c>
-      <c r="AN5" t="s">
+      <c r="AN5" s="32">
+        <v>0</v>
+      </c>
+      <c r="AO5" t="s">
         <v>217</v>
       </c>
-      <c r="AO5" t="s">
+      <c r="AP5" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
@@ -2029,14 +2132,17 @@
       <c r="AM6" s="15">
         <v>0</v>
       </c>
-      <c r="AN6" t="s">
+      <c r="AN6" s="32">
+        <v>0</v>
+      </c>
+      <c r="AO6" t="s">
         <v>187</v>
       </c>
-      <c r="AO6" t="s">
+      <c r="AP6" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
@@ -2155,14 +2261,17 @@
       <c r="AM7" s="15">
         <v>0</v>
       </c>
-      <c r="AN7" t="s">
+      <c r="AN7" s="32">
+        <v>0</v>
+      </c>
+      <c r="AO7" t="s">
         <v>188</v>
       </c>
-      <c r="AO7" t="s">
+      <c r="AP7" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>39</v>
       </c>
@@ -2281,14 +2390,17 @@
       <c r="AM8" s="15">
         <v>0</v>
       </c>
-      <c r="AN8" t="s">
+      <c r="AN8" s="32">
+        <v>0</v>
+      </c>
+      <c r="AO8" t="s">
         <v>194</v>
       </c>
-      <c r="AO8" t="s">
+      <c r="AP8" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>27</v>
       </c>
@@ -2407,14 +2519,17 @@
       <c r="AM9" s="15">
         <v>0</v>
       </c>
-      <c r="AN9" t="s">
+      <c r="AN9" s="32">
+        <v>0</v>
+      </c>
+      <c r="AO9" t="s">
         <v>176</v>
       </c>
-      <c r="AO9" t="s">
+      <c r="AP9" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
@@ -2533,14 +2648,17 @@
       <c r="AM10" s="15">
         <v>0</v>
       </c>
-      <c r="AN10" t="s">
+      <c r="AN10" s="32">
+        <v>0</v>
+      </c>
+      <c r="AO10" t="s">
         <v>177</v>
       </c>
-      <c r="AO10" t="s">
+      <c r="AP10" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -2659,14 +2777,17 @@
       <c r="AM11" s="15">
         <v>0</v>
       </c>
-      <c r="AN11" t="s">
+      <c r="AN11" s="32">
+        <v>0</v>
+      </c>
+      <c r="AO11" t="s">
         <v>201</v>
       </c>
-      <c r="AO11" t="s">
+      <c r="AP11" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>29</v>
       </c>
@@ -2785,14 +2906,17 @@
       <c r="AM12" s="15">
         <v>0</v>
       </c>
-      <c r="AN12" t="s">
+      <c r="AN12" s="32">
+        <v>0</v>
+      </c>
+      <c r="AO12" t="s">
         <v>202</v>
       </c>
-      <c r="AO12" t="s">
+      <c r="AP12" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>18</v>
       </c>
@@ -2911,14 +3035,17 @@
       <c r="AM13" s="15">
         <v>0</v>
       </c>
-      <c r="AN13" t="s">
-        <v>52</v>
+      <c r="AN13" s="32">
+        <v>0</v>
       </c>
       <c r="AO13" t="s">
         <v>52</v>
       </c>
+      <c r="AP13" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>31</v>
       </c>
@@ -3037,14 +3164,17 @@
       <c r="AM14" s="15">
         <v>1</v>
       </c>
-      <c r="AN14" t="s">
+      <c r="AN14" s="32">
+        <v>0</v>
+      </c>
+      <c r="AO14" t="s">
         <v>199</v>
       </c>
-      <c r="AO14" t="s">
+      <c r="AP14" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>40</v>
       </c>
@@ -3163,14 +3293,17 @@
       <c r="AM15" s="15">
         <v>1</v>
       </c>
-      <c r="AN15" t="s">
+      <c r="AN15" s="32">
+        <v>0</v>
+      </c>
+      <c r="AO15" t="s">
         <v>200</v>
       </c>
-      <c r="AO15" t="s">
+      <c r="AP15" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>32</v>
       </c>
@@ -3289,14 +3422,17 @@
       <c r="AM16" s="15">
         <v>0</v>
       </c>
-      <c r="AN16" t="s">
+      <c r="AN16" s="32">
+        <v>0</v>
+      </c>
+      <c r="AO16" t="s">
         <v>191</v>
       </c>
-      <c r="AO16" t="s">
+      <c r="AP16" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>33</v>
       </c>
@@ -3415,14 +3551,17 @@
       <c r="AM17" s="15">
         <v>0</v>
       </c>
-      <c r="AN17" t="s">
+      <c r="AN17" s="32">
+        <v>0</v>
+      </c>
+      <c r="AO17" t="s">
         <v>192</v>
       </c>
-      <c r="AO17" t="s">
+      <c r="AP17" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>13</v>
       </c>
@@ -3541,14 +3680,17 @@
       <c r="AM18" s="15">
         <v>1</v>
       </c>
-      <c r="AN18" t="s">
+      <c r="AN18" s="32">
+        <v>0</v>
+      </c>
+      <c r="AO18" t="s">
         <v>193</v>
       </c>
-      <c r="AO18" t="s">
+      <c r="AP18" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>34</v>
       </c>
@@ -3667,14 +3809,17 @@
       <c r="AM19" s="15">
         <v>0</v>
       </c>
-      <c r="AN19" t="s">
+      <c r="AN19" s="32">
+        <v>0</v>
+      </c>
+      <c r="AO19" t="s">
         <v>184</v>
       </c>
-      <c r="AO19" t="s">
+      <c r="AP19" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>35</v>
       </c>
@@ -3793,14 +3938,17 @@
       <c r="AM20" s="15">
         <v>0</v>
       </c>
-      <c r="AN20" t="s">
+      <c r="AN20" s="32">
+        <v>0</v>
+      </c>
+      <c r="AO20" t="s">
         <v>180</v>
       </c>
-      <c r="AO20" t="s">
+      <c r="AP20" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>36</v>
       </c>
@@ -3919,14 +4067,17 @@
       <c r="AM21" s="15">
         <v>0</v>
       </c>
-      <c r="AN21" t="s">
+      <c r="AN21" s="32">
+        <v>0</v>
+      </c>
+      <c r="AO21" t="s">
         <v>189</v>
       </c>
-      <c r="AO21" t="s">
+      <c r="AP21" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>37</v>
       </c>
@@ -4045,14 +4196,17 @@
       <c r="AM22" s="15">
         <v>0</v>
       </c>
-      <c r="AN22" t="s">
+      <c r="AN22" s="32">
+        <v>0</v>
+      </c>
+      <c r="AO22" t="s">
         <v>185</v>
       </c>
-      <c r="AO22" t="s">
+      <c r="AP22" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>38</v>
       </c>
@@ -4171,14 +4325,17 @@
       <c r="AM23" s="15">
         <v>0</v>
       </c>
-      <c r="AN23" t="s">
+      <c r="AN23" s="32">
+        <v>0</v>
+      </c>
+      <c r="AO23" t="s">
         <v>178</v>
       </c>
-      <c r="AO23" t="s">
+      <c r="AP23" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
@@ -4297,14 +4454,17 @@
       <c r="AM24" s="15">
         <v>0</v>
       </c>
-      <c r="AN24" t="s">
-        <v>54</v>
+      <c r="AN24" s="32">
+        <v>0</v>
       </c>
       <c r="AO24" t="s">
         <v>54</v>
       </c>
+      <c r="AP24" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="25" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>207</v>
       </c>
@@ -4423,14 +4583,17 @@
       <c r="AM25" s="15">
         <v>0</v>
       </c>
-      <c r="AN25" t="s">
-        <v>207</v>
+      <c r="AN25" s="32">
+        <v>0</v>
       </c>
       <c r="AO25" t="s">
         <v>207</v>
       </c>
+      <c r="AP25" t="s">
+        <v>207</v>
+      </c>
     </row>
-    <row r="26" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>208</v>
       </c>
@@ -4549,14 +4712,17 @@
       <c r="AM26" s="15">
         <v>0</v>
       </c>
-      <c r="AN26" t="s">
-        <v>208</v>
+      <c r="AN26" s="32">
+        <v>0</v>
       </c>
       <c r="AO26" t="s">
         <v>208</v>
       </c>
+      <c r="AP26" t="s">
+        <v>208</v>
+      </c>
     </row>
-    <row r="27" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>41</v>
       </c>
@@ -4675,14 +4841,17 @@
       <c r="AM27" s="15">
         <v>0</v>
       </c>
-      <c r="AN27" t="s">
+      <c r="AN27" s="32">
+        <v>0</v>
+      </c>
+      <c r="AO27" t="s">
         <v>181</v>
       </c>
-      <c r="AO27" t="s">
+      <c r="AP27" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="28" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>214</v>
       </c>
@@ -4801,14 +4970,17 @@
       <c r="AM28" s="15">
         <v>0</v>
       </c>
-      <c r="AN28" t="s">
+      <c r="AN28" s="32">
+        <v>0</v>
+      </c>
+      <c r="AO28" t="s">
         <v>218</v>
       </c>
-      <c r="AO28" t="s">
+      <c r="AP28" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="29" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>42</v>
       </c>
@@ -4927,14 +5099,17 @@
       <c r="AM29" s="15">
         <v>0</v>
       </c>
-      <c r="AN29" t="s">
+      <c r="AN29" s="32">
+        <v>0</v>
+      </c>
+      <c r="AO29" t="s">
         <v>219</v>
       </c>
-      <c r="AO29" t="s">
+      <c r="AP29" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>43</v>
       </c>
@@ -5053,14 +5228,17 @@
       <c r="AM30" s="15">
         <v>0</v>
       </c>
-      <c r="AN30" t="s">
+      <c r="AN30" s="32">
+        <v>0</v>
+      </c>
+      <c r="AO30" t="s">
         <v>186</v>
       </c>
-      <c r="AO30" t="s">
+      <c r="AP30" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>44</v>
       </c>
@@ -5179,14 +5357,17 @@
       <c r="AM31" s="15">
         <v>0</v>
       </c>
-      <c r="AN31" t="s">
+      <c r="AN31" s="32">
+        <v>0</v>
+      </c>
+      <c r="AO31" t="s">
         <v>182</v>
       </c>
-      <c r="AO31" t="s">
+      <c r="AP31" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="32" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>45</v>
       </c>
@@ -5305,14 +5486,17 @@
       <c r="AM32" s="15">
         <v>0</v>
       </c>
-      <c r="AN32" t="s">
+      <c r="AN32" s="32">
+        <v>0</v>
+      </c>
+      <c r="AO32" t="s">
         <v>179</v>
       </c>
-      <c r="AO32" t="s">
+      <c r="AP32" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="33" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>15</v>
       </c>
@@ -5431,14 +5615,17 @@
       <c r="AM33" s="15">
         <v>1</v>
       </c>
-      <c r="AN33" t="s">
+      <c r="AN33" s="32">
+        <v>0</v>
+      </c>
+      <c r="AO33" t="s">
         <v>195</v>
       </c>
-      <c r="AO33" t="s">
+      <c r="AP33" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="34" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>93</v>
       </c>
@@ -5557,14 +5744,17 @@
       <c r="AM34" s="15">
         <v>0</v>
       </c>
-      <c r="AN34" t="s">
-        <v>92</v>
+      <c r="AN34" s="32">
+        <v>0</v>
       </c>
       <c r="AO34" t="s">
         <v>92</v>
       </c>
+      <c r="AP34" t="s">
+        <v>92</v>
+      </c>
     </row>
-    <row r="35" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>46</v>
       </c>
@@ -5683,14 +5873,17 @@
       <c r="AM35" s="15">
         <v>0</v>
       </c>
-      <c r="AN35" t="s">
+      <c r="AN35" s="32">
+        <v>0</v>
+      </c>
+      <c r="AO35" t="s">
         <v>183</v>
       </c>
-      <c r="AO35" t="s">
+      <c r="AP35" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="36" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>205</v>
       </c>
@@ -5809,14 +6002,17 @@
       <c r="AM36" s="15">
         <v>0</v>
       </c>
-      <c r="AN36" t="s">
-        <v>205</v>
+      <c r="AN36" s="32">
+        <v>0</v>
       </c>
       <c r="AO36" t="s">
         <v>205</v>
       </c>
+      <c r="AP36" t="s">
+        <v>205</v>
+      </c>
     </row>
-    <row r="37" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>209</v>
       </c>
@@ -5935,14 +6131,17 @@
       <c r="AM37" s="15">
         <v>0</v>
       </c>
-      <c r="AN37" t="s">
+      <c r="AN37" s="32">
+        <v>0</v>
+      </c>
+      <c r="AO37" t="s">
         <v>216</v>
       </c>
-      <c r="AO37" t="s">
+      <c r="AP37" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="38" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>47</v>
       </c>
@@ -6061,14 +6260,17 @@
       <c r="AM38" s="15">
         <v>0</v>
       </c>
-      <c r="AN38" t="s">
+      <c r="AN38" s="32">
+        <v>0</v>
+      </c>
+      <c r="AO38" t="s">
         <v>190</v>
       </c>
-      <c r="AO38" t="s">
+      <c r="AP38" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="39" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>245</v>
       </c>
@@ -6082,7 +6284,7 @@
         <v>750</v>
       </c>
       <c r="E39" s="9">
-        <f t="shared" ref="E39:E40" si="4">D39/C39</f>
+        <f t="shared" ref="E39" si="4">D39/C39</f>
         <v>750</v>
       </c>
       <c r="F39" s="16">
@@ -6187,136 +6389,142 @@
       <c r="AM39" s="15">
         <v>0</v>
       </c>
-      <c r="AN39" t="s">
+      <c r="AN39" s="32">
+        <v>0</v>
+      </c>
+      <c r="AO39" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="40" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="B40" s="13" t="s">
         <v>259</v>
       </c>
-      <c r="B40" s="13" t="s">
+      <c r="C40" s="13">
+        <v>0</v>
+      </c>
+      <c r="D40" s="13">
+        <v>0</v>
+      </c>
+      <c r="E40" s="9">
+        <v>0</v>
+      </c>
+      <c r="F40" s="16">
+        <v>1</v>
+      </c>
+      <c r="G40" s="3">
+        <v>0</v>
+      </c>
+      <c r="H40" s="3">
+        <v>0</v>
+      </c>
+      <c r="I40" s="3">
+        <v>0</v>
+      </c>
+      <c r="J40" s="14">
+        <v>0</v>
+      </c>
+      <c r="K40" s="14">
+        <v>0</v>
+      </c>
+      <c r="L40" s="14">
+        <v>0</v>
+      </c>
+      <c r="M40" s="14">
+        <v>0</v>
+      </c>
+      <c r="N40" s="3">
+        <v>0</v>
+      </c>
+      <c r="O40" s="3">
+        <v>0</v>
+      </c>
+      <c r="P40" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q40" s="3">
+        <v>0</v>
+      </c>
+      <c r="R40" s="18">
+        <v>0</v>
+      </c>
+      <c r="S40" s="18">
+        <v>0</v>
+      </c>
+      <c r="T40" s="18">
+        <v>0</v>
+      </c>
+      <c r="U40" s="18">
+        <v>0</v>
+      </c>
+      <c r="V40" s="8">
+        <v>0</v>
+      </c>
+      <c r="W40" s="8">
+        <v>0</v>
+      </c>
+      <c r="X40" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y40" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z40" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA40" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB40" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC40" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD40" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE40" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF40" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG40" s="6">
+        <v>0</v>
+      </c>
+      <c r="AH40" s="6">
+        <v>0</v>
+      </c>
+      <c r="AI40" s="6">
+        <v>0</v>
+      </c>
+      <c r="AJ40" s="6">
+        <v>0</v>
+      </c>
+      <c r="AK40" s="6">
+        <v>0</v>
+      </c>
+      <c r="AL40" s="6">
+        <v>0</v>
+      </c>
+      <c r="AM40" s="15">
+        <v>1</v>
+      </c>
+      <c r="AN40" s="32">
+        <v>1</v>
+      </c>
+      <c r="AO40" t="s">
         <v>260</v>
       </c>
-      <c r="C40" s="13">
-        <v>0</v>
-      </c>
-      <c r="D40" s="13">
-        <v>0</v>
-      </c>
-      <c r="E40" s="9">
-        <v>0</v>
-      </c>
-      <c r="F40" s="16">
-        <v>1</v>
-      </c>
-      <c r="G40" s="3">
-        <v>0</v>
-      </c>
-      <c r="H40" s="3">
-        <v>0</v>
-      </c>
-      <c r="I40" s="3">
-        <v>0</v>
-      </c>
-      <c r="J40" s="14">
-        <v>0</v>
-      </c>
-      <c r="K40" s="14">
-        <v>0</v>
-      </c>
-      <c r="L40" s="14">
-        <v>0</v>
-      </c>
-      <c r="M40" s="14">
-        <v>0</v>
-      </c>
-      <c r="N40" s="3">
-        <v>0</v>
-      </c>
-      <c r="O40" s="3">
-        <v>0</v>
-      </c>
-      <c r="P40" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q40" s="3">
-        <v>0</v>
-      </c>
-      <c r="R40" s="18">
-        <v>0</v>
-      </c>
-      <c r="S40" s="18">
-        <v>0</v>
-      </c>
-      <c r="T40" s="18">
-        <v>0</v>
-      </c>
-      <c r="U40" s="18">
-        <v>0</v>
-      </c>
-      <c r="V40" s="8">
-        <v>0</v>
-      </c>
-      <c r="W40" s="8">
-        <v>0</v>
-      </c>
-      <c r="X40" s="7">
-        <v>0</v>
-      </c>
-      <c r="Y40" s="7">
-        <v>0</v>
-      </c>
-      <c r="Z40" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA40" s="7">
-        <v>0</v>
-      </c>
-      <c r="AB40" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC40" s="2">
-        <v>0</v>
-      </c>
-      <c r="AD40" s="5">
-        <v>0</v>
-      </c>
-      <c r="AE40" s="5">
-        <v>0</v>
-      </c>
-      <c r="AF40" s="5">
-        <v>0</v>
-      </c>
-      <c r="AG40" s="6">
-        <v>0</v>
-      </c>
-      <c r="AH40" s="6">
-        <v>0</v>
-      </c>
-      <c r="AI40" s="6">
-        <v>0</v>
-      </c>
-      <c r="AJ40" s="6">
-        <v>0</v>
-      </c>
-      <c r="AK40" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL40" s="6">
-        <v>0</v>
-      </c>
-      <c r="AM40" s="15">
-        <v>1</v>
-      </c>
-      <c r="AN40" t="s">
+      <c r="AP40" t="s">
         <v>261</v>
       </c>
-      <c r="AO40" t="s">
-        <v>262</v>
-      </c>
     </row>
-    <row r="42" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:42" x14ac:dyDescent="0.25">
       <c r="AF42" t="s">
         <v>204</v>
       </c>
@@ -6328,10 +6536,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DE40"/>
+  <dimension ref="A1:DQ40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J46" sqref="J46"/>
+      <selection activeCell="CS47" sqref="CS47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6339,11 +6547,11 @@
     <col min="1" max="75" width="3.7109375" bestFit="1" customWidth="1"/>
     <col min="76" max="77" width="3.7109375" customWidth="1"/>
     <col min="78" max="86" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="87" max="108" width="3.7109375" customWidth="1"/>
-    <col min="109" max="109" width="36.28515625" customWidth="1"/>
+    <col min="87" max="120" width="3.7109375" customWidth="1"/>
+    <col min="121" max="121" width="36.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:109" s="11" customFormat="1" ht="72" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:121" s="11" customFormat="1" ht="72" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>95</v>
       </c>
@@ -6663,16 +6871,52 @@
         <v>257</v>
       </c>
       <c r="DC1" s="11" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="DD1" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="DE1" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="DF1" s="11" t="s">
+        <v>265</v>
+      </c>
+      <c r="DG1" s="11" t="s">
+        <v>266</v>
+      </c>
+      <c r="DH1" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="DI1" s="11" t="s">
+        <v>268</v>
+      </c>
+      <c r="DJ1" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="DK1" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="DL1" s="11" t="s">
+        <v>271</v>
+      </c>
+      <c r="DM1" s="11" t="s">
+        <v>272</v>
+      </c>
+      <c r="DN1" s="11" t="s">
+        <v>273</v>
+      </c>
+      <c r="DO1" s="11" t="s">
+        <v>274</v>
+      </c>
+      <c r="DP1" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="DE1" t="s">
+      <c r="DQ1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:121" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>88</v>
       </c>
@@ -7018,21 +7262,58 @@
         <f>Tabelle1!U2</f>
         <v>1</v>
       </c>
-      <c r="DB2" s="12" t="s">
-        <v>88</v>
+      <c r="DB2" s="12">
+        <f>Tabelle1!AN2</f>
+        <v>0</v>
       </c>
       <c r="DC2" s="12" t="s">
         <v>88</v>
       </c>
       <c r="DD2" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DE2" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DF2" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DG2" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DH2" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DI2" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DJ2" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DK2" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DL2" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DM2" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DN2" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DO2" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DP2" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DE2" t="str">
-        <f>Tabelle1!AN2</f>
+      <c r="DQ2" t="str">
+        <f>Tabelle1!AO2</f>
         <v>Airbus A320 Neo</v>
       </c>
     </row>
-    <row r="3" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:121" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>88</v>
       </c>
@@ -7378,21 +7659,58 @@
         <f>Tabelle1!U3</f>
         <v>0</v>
       </c>
-      <c r="DB3" s="12" t="s">
-        <v>88</v>
+      <c r="DB3" s="12">
+        <f>Tabelle1!AN3</f>
+        <v>0</v>
       </c>
       <c r="DC3" s="12" t="s">
         <v>88</v>
       </c>
       <c r="DD3" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DE3" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DF3" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DG3" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DH3" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DI3" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DJ3" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DK3" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DL3" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DM3" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DN3" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DO3" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DP3" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DE3" t="str">
-        <f>Tabelle1!AN3</f>
+      <c r="DQ3" t="str">
+        <f>Tabelle1!AO3</f>
         <v>Boeing 747-8i</v>
       </c>
     </row>
-    <row r="4" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:121" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>88</v>
       </c>
@@ -7738,21 +8056,58 @@
         <f>Tabelle1!U4</f>
         <v>0</v>
       </c>
-      <c r="DB4" s="12" t="s">
-        <v>88</v>
+      <c r="DB4" s="12">
+        <f>Tabelle1!AN4</f>
+        <v>0</v>
       </c>
       <c r="DC4" s="12" t="s">
         <v>88</v>
       </c>
       <c r="DD4" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DE4" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DF4" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DG4" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DH4" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DI4" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DJ4" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DK4" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DL4" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DM4" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DN4" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DO4" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DP4" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DE4" t="str">
-        <f>Tabelle1!AN4</f>
+      <c r="DQ4" t="str">
+        <f>Tabelle1!AO4</f>
         <v>Boeing 787-10</v>
       </c>
     </row>
-    <row r="5" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:121" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>88</v>
       </c>
@@ -8098,21 +8453,58 @@
         <f>Tabelle1!U5</f>
         <v>0</v>
       </c>
-      <c r="DB5" s="12" t="s">
-        <v>88</v>
+      <c r="DB5" s="12">
+        <f>Tabelle1!AN5</f>
+        <v>0</v>
       </c>
       <c r="DC5" s="12" t="s">
         <v>88</v>
       </c>
       <c r="DD5" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DE5" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DF5" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DG5" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DH5" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DI5" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DJ5" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DK5" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DL5" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DM5" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DN5" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DO5" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DP5" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DE5" t="str">
-        <f>Tabelle1!AN5</f>
+      <c r="DQ5" t="str">
+        <f>Tabelle1!AO5</f>
         <v>Boeing F/A 18E Super Hornet</v>
       </c>
     </row>
-    <row r="6" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:121" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>88</v>
       </c>
@@ -8458,21 +8850,58 @@
         <f>Tabelle1!U6</f>
         <v>0</v>
       </c>
-      <c r="DB6" s="12" t="s">
-        <v>88</v>
+      <c r="DB6" s="12">
+        <f>Tabelle1!AN6</f>
+        <v>0</v>
       </c>
       <c r="DC6" s="12" t="s">
         <v>88</v>
       </c>
       <c r="DD6" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DE6" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DF6" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DG6" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DH6" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DI6" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DJ6" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DK6" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DL6" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DM6" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DN6" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DO6" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DP6" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DE6" t="str">
-        <f>Tabelle1!AN6</f>
+      <c r="DQ6" t="str">
+        <f>Tabelle1!AO6</f>
         <v>Baron G58</v>
       </c>
     </row>
-    <row r="7" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:121" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>88</v>
       </c>
@@ -8818,21 +9247,58 @@
         <f>Tabelle1!U7</f>
         <v>0</v>
       </c>
-      <c r="DB7" s="12" t="s">
-        <v>88</v>
+      <c r="DB7" s="12">
+        <f>Tabelle1!AN7</f>
+        <v>0</v>
       </c>
       <c r="DC7" s="12" t="s">
         <v>88</v>
       </c>
       <c r="DD7" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DE7" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DF7" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DG7" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DH7" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DI7" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DJ7" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DK7" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DL7" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DM7" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DN7" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DO7" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DP7" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DE7" t="str">
-        <f>Tabelle1!AN7</f>
+      <c r="DQ7" t="str">
+        <f>Tabelle1!AO7</f>
         <v>Bonanza G36</v>
       </c>
     </row>
-    <row r="8" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:121" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>88</v>
       </c>
@@ -9178,21 +9644,58 @@
         <f>Tabelle1!U8</f>
         <v>0</v>
       </c>
-      <c r="DB8" s="12" t="s">
-        <v>88</v>
+      <c r="DB8" s="12">
+        <f>Tabelle1!AN8</f>
+        <v>0</v>
       </c>
       <c r="DC8" s="12" t="s">
         <v>88</v>
       </c>
       <c r="DD8" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DE8" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DF8" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DG8" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DH8" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DI8" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DJ8" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DK8" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DL8" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DM8" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DN8" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DO8" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DP8" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DE8" t="str">
-        <f>Tabelle1!AN8</f>
+      <c r="DQ8" t="str">
+        <f>Tabelle1!AO8</f>
         <v>Beechcraft King Air 350i</v>
       </c>
     </row>
-    <row r="9" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:121" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>88</v>
       </c>
@@ -9538,21 +10041,58 @@
         <f>Tabelle1!U9</f>
         <v>0</v>
       </c>
-      <c r="DB9" s="12" t="s">
-        <v>88</v>
+      <c r="DB9" s="12">
+        <f>Tabelle1!AN9</f>
+        <v>0</v>
       </c>
       <c r="DC9" s="12" t="s">
         <v>88</v>
       </c>
       <c r="DD9" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DE9" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DF9" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DG9" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DH9" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DI9" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DJ9" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DK9" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DL9" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DM9" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DN9" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DO9" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DP9" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DE9" t="str">
-        <f>Tabelle1!AN9</f>
+      <c r="DQ9" t="str">
+        <f>Tabelle1!AO9</f>
         <v>Cessna 152</v>
       </c>
     </row>
-    <row r="10" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:121" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>88</v>
       </c>
@@ -9898,21 +10438,58 @@
         <f>Tabelle1!U10</f>
         <v>0</v>
       </c>
-      <c r="DB10" s="12" t="s">
-        <v>88</v>
+      <c r="DB10" s="12">
+        <f>Tabelle1!AN10</f>
+        <v>0</v>
       </c>
       <c r="DC10" s="12" t="s">
         <v>88</v>
       </c>
       <c r="DD10" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DE10" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DF10" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DG10" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DH10" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DI10" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DJ10" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DK10" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DL10" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DM10" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DN10" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DO10" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DP10" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DE10" t="str">
-        <f>Tabelle1!AN10</f>
+      <c r="DQ10" t="str">
+        <f>Tabelle1!AO10</f>
         <v>Cessna 152 Aero</v>
       </c>
     </row>
-    <row r="11" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:121" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>88</v>
       </c>
@@ -10258,21 +10835,58 @@
         <f>Tabelle1!U11</f>
         <v>0</v>
       </c>
-      <c r="DB11" s="12" t="s">
-        <v>88</v>
+      <c r="DB11" s="12">
+        <f>Tabelle1!AN11</f>
+        <v>0</v>
       </c>
       <c r="DC11" s="12" t="s">
         <v>88</v>
       </c>
       <c r="DD11" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DE11" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DF11" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DG11" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DH11" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DI11" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DJ11" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DK11" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DL11" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DM11" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DN11" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DO11" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DP11" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DE11" t="str">
-        <f>Tabelle1!AN11</f>
+      <c r="DQ11" t="str">
+        <f>Tabelle1!AO11</f>
         <v>Cessna 172sp Skyhawk G1000</v>
       </c>
     </row>
-    <row r="12" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:121" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>88</v>
       </c>
@@ -10618,21 +11232,58 @@
         <f>Tabelle1!U12</f>
         <v>0</v>
       </c>
-      <c r="DB12" s="12" t="s">
-        <v>88</v>
+      <c r="DB12" s="12">
+        <f>Tabelle1!AN12</f>
+        <v>0</v>
       </c>
       <c r="DC12" s="12" t="s">
         <v>88</v>
       </c>
       <c r="DD12" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DE12" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DF12" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DG12" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DH12" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DI12" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DJ12" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DK12" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DL12" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DM12" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DN12" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DO12" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DP12" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DE12" t="str">
-        <f>Tabelle1!AN12</f>
+      <c r="DQ12" t="str">
+        <f>Tabelle1!AO12</f>
         <v>Cessna 172sp Skyhawk</v>
       </c>
     </row>
-    <row r="13" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:121" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>88</v>
       </c>
@@ -10978,21 +11629,58 @@
         <f>Tabelle1!U13</f>
         <v>0</v>
       </c>
-      <c r="DB13" s="12" t="s">
-        <v>88</v>
+      <c r="DB13" s="12">
+        <f>Tabelle1!AN13</f>
+        <v>0</v>
       </c>
       <c r="DC13" s="12" t="s">
         <v>88</v>
       </c>
       <c r="DD13" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DE13" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DF13" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DG13" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DH13" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DI13" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DJ13" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DK13" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DL13" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DM13" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DN13" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DO13" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DP13" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DE13" t="str">
-        <f>Tabelle1!AN13</f>
+      <c r="DQ13" t="str">
+        <f>Tabelle1!AO13</f>
         <v>Cessna 208B Grand Caravan EX</v>
       </c>
     </row>
-    <row r="14" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:121" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>88</v>
       </c>
@@ -11338,21 +12026,58 @@
         <f>Tabelle1!U14</f>
         <v>0</v>
       </c>
-      <c r="DB14" s="12" t="s">
-        <v>88</v>
+      <c r="DB14" s="12">
+        <f>Tabelle1!AN14</f>
+        <v>0</v>
       </c>
       <c r="DC14" s="12" t="s">
         <v>88</v>
       </c>
       <c r="DD14" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DE14" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DF14" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DG14" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DH14" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DI14" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DJ14" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DK14" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DL14" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DM14" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DN14" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DO14" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DP14" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DE14" t="str">
-        <f>Tabelle1!AN14</f>
+      <c r="DQ14" t="str">
+        <f>Tabelle1!AO14</f>
         <v>Cessna CJ4 Citation</v>
       </c>
     </row>
-    <row r="15" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:121" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>88</v>
       </c>
@@ -11698,21 +12423,58 @@
         <f>Tabelle1!U15</f>
         <v>0</v>
       </c>
-      <c r="DB15" s="12" t="s">
-        <v>88</v>
+      <c r="DB15" s="12">
+        <f>Tabelle1!AN15</f>
+        <v>0</v>
       </c>
       <c r="DC15" s="12" t="s">
         <v>88</v>
       </c>
       <c r="DD15" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DE15" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DF15" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DG15" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DH15" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DI15" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DJ15" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DK15" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DL15" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DM15" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DN15" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DO15" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DP15" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DE15" t="str">
-        <f>Tabelle1!AN15</f>
+      <c r="DQ15" t="str">
+        <f>Tabelle1!AO15</f>
         <v>Cessna Longitude</v>
       </c>
     </row>
-    <row r="16" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:121" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>88</v>
       </c>
@@ -12058,21 +12820,58 @@
         <f>Tabelle1!U16</f>
         <v>0</v>
       </c>
-      <c r="DB16" s="12" t="s">
-        <v>88</v>
+      <c r="DB16" s="12">
+        <f>Tabelle1!AN16</f>
+        <v>0</v>
       </c>
       <c r="DC16" s="12" t="s">
         <v>88</v>
       </c>
       <c r="DD16" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DE16" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DF16" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DG16" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DH16" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DI16" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DJ16" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DK16" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DL16" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DM16" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DN16" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DO16" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DP16" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DE16" t="str">
-        <f>Tabelle1!AN16</f>
+      <c r="DQ16" t="str">
+        <f>Tabelle1!AO16</f>
         <v>DA40-NG</v>
       </c>
     </row>
-    <row r="17" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:121" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>88</v>
       </c>
@@ -12418,21 +13217,58 @@
         <f>Tabelle1!U17</f>
         <v>0</v>
       </c>
-      <c r="DB17" s="12" t="s">
-        <v>88</v>
+      <c r="DB17" s="12">
+        <f>Tabelle1!AN17</f>
+        <v>0</v>
       </c>
       <c r="DC17" s="12" t="s">
         <v>88</v>
       </c>
       <c r="DD17" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DE17" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DF17" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DG17" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DH17" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DI17" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DJ17" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DK17" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DL17" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DM17" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DN17" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DO17" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DP17" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DE17" t="str">
-        <f>Tabelle1!AN17</f>
+      <c r="DQ17" t="str">
+        <f>Tabelle1!AO17</f>
         <v>DA40 TDI</v>
       </c>
     </row>
-    <row r="18" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:121" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>88</v>
       </c>
@@ -12778,21 +13614,58 @@
         <f>Tabelle1!U18</f>
         <v>0</v>
       </c>
-      <c r="DB18" s="12" t="s">
-        <v>88</v>
+      <c r="DB18" s="12">
+        <f>Tabelle1!AN18</f>
+        <v>0</v>
       </c>
       <c r="DC18" s="12" t="s">
         <v>88</v>
       </c>
       <c r="DD18" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DE18" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DF18" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DG18" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DH18" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DI18" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DJ18" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DK18" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DL18" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DM18" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DN18" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DO18" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DP18" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DE18" t="str">
-        <f>Tabelle1!AN18</f>
+      <c r="DQ18" t="str">
+        <f>Tabelle1!AO18</f>
         <v>DA62</v>
       </c>
     </row>
-    <row r="19" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:121" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>88</v>
       </c>
@@ -13138,21 +14011,58 @@
         <f>Tabelle1!U19</f>
         <v>0</v>
       </c>
-      <c r="DB19" s="12" t="s">
-        <v>88</v>
+      <c r="DB19" s="12">
+        <f>Tabelle1!AN19</f>
+        <v>0</v>
       </c>
       <c r="DC19" s="12" t="s">
         <v>88</v>
       </c>
       <c r="DD19" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DE19" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DF19" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DG19" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DH19" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DI19" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DJ19" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DK19" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DL19" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DM19" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DN19" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DO19" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DP19" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DE19" t="str">
-        <f>Tabelle1!AN19</f>
+      <c r="DQ19" t="str">
+        <f>Tabelle1!AO19</f>
         <v>DR400</v>
       </c>
     </row>
-    <row r="20" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:121" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>88</v>
       </c>
@@ -13498,21 +14408,58 @@
         <f>Tabelle1!U20</f>
         <v>0</v>
       </c>
-      <c r="DB20" s="12" t="s">
-        <v>88</v>
+      <c r="DB20" s="12">
+        <f>Tabelle1!AN20</f>
+        <v>0</v>
       </c>
       <c r="DC20" s="12" t="s">
         <v>88</v>
       </c>
       <c r="DD20" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DE20" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DF20" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DG20" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DH20" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DI20" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DJ20" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DK20" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DL20" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DM20" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DN20" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DO20" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DP20" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DE20" t="str">
-        <f>Tabelle1!AN20</f>
+      <c r="DQ20" t="str">
+        <f>Tabelle1!AO20</f>
         <v>DV20</v>
       </c>
     </row>
-    <row r="21" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:121" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>88</v>
       </c>
@@ -13858,21 +14805,58 @@
         <f>Tabelle1!U21</f>
         <v>0</v>
       </c>
-      <c r="DB21" s="12" t="s">
-        <v>88</v>
+      <c r="DB21" s="12">
+        <f>Tabelle1!AN21</f>
+        <v>0</v>
       </c>
       <c r="DC21" s="12" t="s">
         <v>88</v>
       </c>
       <c r="DD21" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DE21" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DF21" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DG21" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DH21" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DI21" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DJ21" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DK21" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DL21" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DM21" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DN21" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DO21" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DP21" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DE21" t="str">
-        <f>Tabelle1!AN21</f>
+      <c r="DQ21" t="str">
+        <f>Tabelle1!AO21</f>
         <v>Extra 330</v>
       </c>
     </row>
-    <row r="22" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:121" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>88</v>
       </c>
@@ -14218,21 +15202,58 @@
         <f>Tabelle1!U22</f>
         <v>0</v>
       </c>
-      <c r="DB22" s="12" t="s">
-        <v>88</v>
+      <c r="DB22" s="12">
+        <f>Tabelle1!AN22</f>
+        <v>0</v>
       </c>
       <c r="DC22" s="12" t="s">
         <v>88</v>
       </c>
       <c r="DD22" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DE22" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DF22" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DG22" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DH22" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DI22" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DJ22" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DK22" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DL22" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DM22" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DN22" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DO22" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DP22" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DE22" t="str">
-        <f>Tabelle1!AN22</f>
+      <c r="DQ22" t="str">
+        <f>Tabelle1!AO22</f>
         <v>FlightDesignCT</v>
       </c>
     </row>
-    <row r="23" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:121" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>88</v>
       </c>
@@ -14578,21 +15599,58 @@
         <f>Tabelle1!U23</f>
         <v>0</v>
       </c>
-      <c r="DB23" s="12" t="s">
-        <v>88</v>
+      <c r="DB23" s="12">
+        <f>Tabelle1!AN23</f>
+        <v>0</v>
       </c>
       <c r="DC23" s="12" t="s">
         <v>88</v>
       </c>
       <c r="DD23" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DE23" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DF23" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DG23" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DH23" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DI23" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DJ23" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DK23" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DL23" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DM23" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DN23" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DO23" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DP23" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DE23" t="str">
-        <f>Tabelle1!AN23</f>
+      <c r="DQ23" t="str">
+        <f>Tabelle1!AO23</f>
         <v>Icon A5</v>
       </c>
     </row>
-    <row r="24" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:121" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>88</v>
       </c>
@@ -14938,21 +15996,58 @@
         <f>Tabelle1!U24</f>
         <v>0</v>
       </c>
-      <c r="DB24" s="12" t="s">
-        <v>88</v>
+      <c r="DB24" s="12">
+        <f>Tabelle1!AN24</f>
+        <v>0</v>
       </c>
       <c r="DC24" s="12" t="s">
         <v>88</v>
       </c>
       <c r="DD24" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DE24" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DF24" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DG24" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DH24" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DI24" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DJ24" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DK24" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DL24" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DM24" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DN24" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DO24" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DP24" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DE24" t="str">
-        <f>Tabelle1!AN24</f>
+      <c r="DQ24" t="str">
+        <f>Tabelle1!AO24</f>
         <v>Mudry Cap 10 C</v>
       </c>
     </row>
-    <row r="25" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:121" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>88</v>
       </c>
@@ -15298,21 +16393,58 @@
         <f>Tabelle1!U25</f>
         <v>0</v>
       </c>
-      <c r="DB25" s="12" t="s">
-        <v>88</v>
+      <c r="DB25" s="12">
+        <f>Tabelle1!AN25</f>
+        <v>0</v>
       </c>
       <c r="DC25" s="12" t="s">
         <v>88</v>
       </c>
       <c r="DD25" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DE25" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DF25" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DG25" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DH25" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DI25" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DJ25" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DK25" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DL25" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DM25" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DN25" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DO25" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DP25" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DE25" t="str">
-        <f>Tabelle1!AN25</f>
+      <c r="DQ25" t="str">
+        <f>Tabelle1!AO25</f>
         <v>Pilatus PC-6 Gauge</v>
       </c>
     </row>
-    <row r="26" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:121" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>88</v>
       </c>
@@ -15658,21 +16790,58 @@
         <f>Tabelle1!U26</f>
         <v>0</v>
       </c>
-      <c r="DB26" s="12" t="s">
-        <v>88</v>
+      <c r="DB26" s="12">
+        <f>Tabelle1!AN26</f>
+        <v>0</v>
       </c>
       <c r="DC26" s="12" t="s">
         <v>88</v>
       </c>
       <c r="DD26" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DE26" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DF26" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DG26" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DH26" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DI26" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DJ26" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DK26" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DL26" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DM26" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DN26" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DO26" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DP26" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DE26" t="str">
-        <f>Tabelle1!AN26</f>
+      <c r="DQ26" t="str">
+        <f>Tabelle1!AO26</f>
         <v>Pilatus PC-6 G950</v>
       </c>
     </row>
-    <row r="27" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:121" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>88</v>
       </c>
@@ -16018,21 +17187,58 @@
         <f>Tabelle1!U27</f>
         <v>0</v>
       </c>
-      <c r="DB27" s="12" t="s">
-        <v>88</v>
+      <c r="DB27" s="12">
+        <f>Tabelle1!AN27</f>
+        <v>0</v>
       </c>
       <c r="DC27" s="12" t="s">
         <v>88</v>
       </c>
       <c r="DD27" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DE27" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DF27" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DG27" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DH27" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DI27" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DJ27" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DK27" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DL27" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DM27" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DN27" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DO27" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DP27" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DE27" t="str">
-        <f>Tabelle1!AN27</f>
+      <c r="DQ27" t="str">
+        <f>Tabelle1!AO27</f>
         <v>Pipistrel Alpha Electro</v>
       </c>
     </row>
-    <row r="28" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:121" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>88</v>
       </c>
@@ -16378,21 +17584,58 @@
         <f>Tabelle1!U28</f>
         <v>0</v>
       </c>
-      <c r="DB28" s="12" t="s">
-        <v>88</v>
+      <c r="DB28" s="12">
+        <f>Tabelle1!AN28</f>
+        <v>0</v>
       </c>
       <c r="DC28" s="12" t="s">
         <v>88</v>
       </c>
       <c r="DD28" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DE28" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DF28" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DG28" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DH28" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DI28" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DJ28" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DK28" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DL28" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DM28" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DN28" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DO28" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DP28" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DE28" t="str">
-        <f>Tabelle1!AN28</f>
+      <c r="DQ28" t="str">
+        <f>Tabelle1!AO28</f>
         <v>Pitts Special 1S</v>
       </c>
     </row>
-    <row r="29" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:121" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>88</v>
       </c>
@@ -16738,21 +17981,58 @@
         <f>Tabelle1!U29</f>
         <v>0</v>
       </c>
-      <c r="DB29" s="12" t="s">
-        <v>88</v>
+      <c r="DB29" s="12">
+        <f>Tabelle1!AN29</f>
+        <v>0</v>
       </c>
       <c r="DC29" s="12" t="s">
         <v>88</v>
       </c>
       <c r="DD29" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DE29" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DF29" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DG29" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DH29" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DI29" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DJ29" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DK29" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DL29" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DM29" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DN29" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DO29" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DP29" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DE29" t="str">
-        <f>Tabelle1!AN29</f>
+      <c r="DQ29" t="str">
+        <f>Tabelle1!AO29</f>
         <v>Pitts Special S2S</v>
       </c>
     </row>
-    <row r="30" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:121" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>88</v>
       </c>
@@ -17098,21 +18378,58 @@
         <f>Tabelle1!U30</f>
         <v>0</v>
       </c>
-      <c r="DB30" s="12" t="s">
-        <v>88</v>
+      <c r="DB30" s="12">
+        <f>Tabelle1!AN30</f>
+        <v>0</v>
       </c>
       <c r="DC30" s="12" t="s">
         <v>88</v>
       </c>
       <c r="DD30" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DE30" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DF30" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DG30" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DH30" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DI30" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DJ30" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DK30" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DL30" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DM30" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DN30" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DO30" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DP30" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DE30" t="str">
-        <f>Tabelle1!AN30</f>
+      <c r="DQ30" t="str">
+        <f>Tabelle1!AO30</f>
         <v>Savage Cub</v>
       </c>
     </row>
-    <row r="31" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:121" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>88</v>
       </c>
@@ -17458,21 +18775,58 @@
         <f>Tabelle1!U31</f>
         <v>0</v>
       </c>
-      <c r="DB31" s="12" t="s">
-        <v>88</v>
+      <c r="DB31" s="12">
+        <f>Tabelle1!AN31</f>
+        <v>0</v>
       </c>
       <c r="DC31" s="12" t="s">
         <v>88</v>
       </c>
       <c r="DD31" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DE31" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DF31" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DG31" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DH31" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DI31" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DJ31" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DK31" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DL31" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DM31" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DN31" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DO31" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DP31" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DE31" t="str">
-        <f>Tabelle1!AN31</f>
+      <c r="DQ31" t="str">
+        <f>Tabelle1!AO31</f>
         <v>Savage Shock Ultra</v>
       </c>
     </row>
-    <row r="32" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:121" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>88</v>
       </c>
@@ -17818,21 +19172,58 @@
         <f>Tabelle1!U32</f>
         <v>0</v>
       </c>
-      <c r="DB32" s="12" t="s">
-        <v>88</v>
+      <c r="DB32" s="12">
+        <f>Tabelle1!AN32</f>
+        <v>0</v>
       </c>
       <c r="DC32" s="12" t="s">
         <v>88</v>
       </c>
       <c r="DD32" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DE32" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DF32" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DG32" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DH32" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DI32" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DJ32" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DK32" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DL32" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DM32" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DN32" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DO32" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DP32" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DE32" t="str">
-        <f>Tabelle1!AN32</f>
+      <c r="DQ32" t="str">
+        <f>Tabelle1!AO32</f>
         <v>SR22</v>
       </c>
     </row>
-    <row r="33" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:121" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>88</v>
       </c>
@@ -18178,21 +19569,58 @@
         <f>Tabelle1!U33</f>
         <v>0</v>
       </c>
-      <c r="DB33" s="12" t="s">
-        <v>88</v>
+      <c r="DB33" s="12">
+        <f>Tabelle1!AN33</f>
+        <v>0</v>
       </c>
       <c r="DC33" s="12" t="s">
         <v>88</v>
       </c>
       <c r="DD33" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DE33" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DF33" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DG33" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DH33" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DI33" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DJ33" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DK33" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DL33" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DM33" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DN33" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DO33" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DP33" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DE33" t="str">
-        <f>Tabelle1!AN33</f>
+      <c r="DQ33" t="str">
+        <f>Tabelle1!AO33</f>
         <v>TBM 930</v>
       </c>
     </row>
-    <row r="34" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:121" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>88</v>
       </c>
@@ -18538,21 +19966,58 @@
         <f>Tabelle1!U34</f>
         <v>0</v>
       </c>
-      <c r="DB34" s="12" t="s">
-        <v>88</v>
+      <c r="DB34" s="12">
+        <f>Tabelle1!AN34</f>
+        <v>0</v>
       </c>
       <c r="DC34" s="12" t="s">
         <v>88</v>
       </c>
       <c r="DD34" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DE34" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DF34" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DG34" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DH34" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DI34" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DJ34" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DK34" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DL34" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DM34" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DN34" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DO34" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DP34" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DE34" t="str">
-        <f>Tabelle1!AN34</f>
+      <c r="DQ34" t="str">
+        <f>Tabelle1!AO34</f>
         <v>Vertigo</v>
       </c>
     </row>
-    <row r="35" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:121" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
         <v>88</v>
       </c>
@@ -18898,21 +20363,58 @@
         <f>Tabelle1!U35</f>
         <v>0</v>
       </c>
-      <c r="DB35" s="12" t="s">
-        <v>88</v>
+      <c r="DB35" s="12">
+        <f>Tabelle1!AN35</f>
+        <v>0</v>
       </c>
       <c r="DC35" s="12" t="s">
         <v>88</v>
       </c>
       <c r="DD35" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DE35" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DF35" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DG35" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DH35" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DI35" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DJ35" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DK35" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DL35" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DM35" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DN35" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DO35" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DP35" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DE35" t="str">
-        <f>Tabelle1!AN35</f>
+      <c r="DQ35" t="str">
+        <f>Tabelle1!AO35</f>
         <v>VL3</v>
       </c>
     </row>
-    <row r="36" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:121" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>88</v>
       </c>
@@ -19258,21 +20760,58 @@
         <f>Tabelle1!U36</f>
         <v>0</v>
       </c>
-      <c r="DB36" s="12" t="s">
-        <v>88</v>
+      <c r="DB36" s="12">
+        <f>Tabelle1!AN36</f>
+        <v>0</v>
       </c>
       <c r="DC36" s="12" t="s">
         <v>88</v>
       </c>
       <c r="DD36" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DE36" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DF36" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DG36" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DH36" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DI36" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DJ36" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DK36" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DL36" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DM36" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DN36" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DO36" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DP36" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DE36" t="str">
-        <f>Tabelle1!AN36</f>
+      <c r="DQ36" t="str">
+        <f>Tabelle1!AO36</f>
         <v>Volocity</v>
       </c>
     </row>
-    <row r="37" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:121" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
         <v>88</v>
       </c>
@@ -19618,21 +21157,58 @@
         <f>Tabelle1!U37</f>
         <v>0</v>
       </c>
-      <c r="DB37" s="12" t="s">
-        <v>88</v>
+      <c r="DB37" s="12">
+        <f>Tabelle1!AN37</f>
+        <v>0</v>
       </c>
       <c r="DC37" s="12" t="s">
         <v>88</v>
       </c>
       <c r="DD37" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DE37" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DF37" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DG37" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DH37" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DI37" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DJ37" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DK37" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DL37" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DM37" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DN37" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DO37" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DP37" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DE37" t="str">
-        <f>Tabelle1!AN37</f>
+      <c r="DQ37" t="str">
+        <f>Tabelle1!AO37</f>
         <v>NXCub</v>
       </c>
     </row>
-    <row r="38" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:121" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>88</v>
       </c>
@@ -19978,21 +21554,58 @@
         <f>Tabelle1!U38</f>
         <v>0</v>
       </c>
-      <c r="DB38" s="12" t="s">
-        <v>88</v>
+      <c r="DB38" s="12">
+        <f>Tabelle1!AN38</f>
+        <v>0</v>
       </c>
       <c r="DC38" s="12" t="s">
         <v>88</v>
       </c>
       <c r="DD38" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DE38" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DF38" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DG38" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DH38" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DI38" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DJ38" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DK38" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DL38" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DM38" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DN38" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DO38" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DP38" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DE38" t="str">
-        <f>Tabelle1!AN38</f>
+      <c r="DQ38" t="str">
+        <f>Tabelle1!AO38</f>
         <v>XCub</v>
       </c>
     </row>
-    <row r="39" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:121" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>88</v>
       </c>
@@ -20338,21 +21951,58 @@
         <f>Tabelle1!U39</f>
         <v>0</v>
       </c>
-      <c r="DB39" s="12" t="s">
-        <v>88</v>
+      <c r="DB39" s="12">
+        <f>Tabelle1!AN39</f>
+        <v>0</v>
       </c>
       <c r="DC39" s="12" t="s">
         <v>88</v>
       </c>
       <c r="DD39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DE39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DF39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DG39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DH39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DI39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DJ39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DK39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DL39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DM39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DN39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DO39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DP39" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DE39" t="str">
-        <f>Tabelle1!AN39</f>
+      <c r="DQ39" t="str">
+        <f>Tabelle1!AO39</f>
         <v>SWS Kodiak 100 II</v>
       </c>
     </row>
-    <row r="40" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:121" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
         <v>88</v>
       </c>
@@ -20698,17 +22348,54 @@
         <f>Tabelle1!U40</f>
         <v>0</v>
       </c>
-      <c r="DB40" s="12" t="s">
-        <v>88</v>
+      <c r="DB40" s="12">
+        <f>Tabelle1!AN40</f>
+        <v>1</v>
       </c>
       <c r="DC40" s="12" t="s">
         <v>88</v>
       </c>
       <c r="DD40" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DE40" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DF40" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DG40" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DH40" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DI40" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DJ40" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DK40" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DL40" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DM40" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DN40" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DO40" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DP40" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DE40" t="str">
-        <f>Tabelle1!AN40</f>
+      <c r="DQ40" t="str">
+        <f>Tabelle1!AO40</f>
         <v>Generic Glider</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V 0.46-B43 (PreRel) - Add Ability to set Fonts in Config - Add Free Text Field - Update VARIO sound (more like a real one - but still not pleasant..) - Updated Airport DB from SU8 - Fix issue with WPalt calculation - Fix Improve layout procedure for some items - Update QuickGuide
</commit_message>
<xml_diff>
--- a/Config/EngineMerge.xlsx
+++ b/Config/EngineMerge.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3790" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3830" uniqueCount="277">
   <si>
     <t>ACFT</t>
   </si>
@@ -846,6 +846,9 @@
   </si>
   <si>
     <t>VARIO MPS</t>
+  </si>
+  <si>
+    <t>TXT</t>
   </si>
 </sst>
 </file>
@@ -6536,10 +6539,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DQ40"/>
+  <dimension ref="A1:DR40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="CS47" sqref="CS47"/>
+      <selection activeCell="CR26" sqref="CR26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6547,11 +6550,11 @@
     <col min="1" max="75" width="3.7109375" bestFit="1" customWidth="1"/>
     <col min="76" max="77" width="3.7109375" customWidth="1"/>
     <col min="78" max="86" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="87" max="120" width="3.7109375" customWidth="1"/>
-    <col min="121" max="121" width="36.28515625" customWidth="1"/>
+    <col min="87" max="121" width="3.7109375" customWidth="1"/>
+    <col min="122" max="122" width="36.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:121" s="11" customFormat="1" ht="72" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:122" s="11" customFormat="1" ht="72" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>95</v>
       </c>
@@ -6910,13 +6913,16 @@
         <v>274</v>
       </c>
       <c r="DP1" s="11" t="s">
+        <v>276</v>
+      </c>
+      <c r="DQ1" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="DQ1" t="s">
+      <c r="DR1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:121" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:122" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>88</v>
       </c>
@@ -7306,14 +7312,17 @@
         <v>88</v>
       </c>
       <c r="DP2" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DQ2" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DQ2" t="str">
+      <c r="DR2" t="str">
         <f>Tabelle1!AO2</f>
         <v>Airbus A320 Neo</v>
       </c>
     </row>
-    <row r="3" spans="1:121" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:122" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>88</v>
       </c>
@@ -7703,14 +7712,17 @@
         <v>88</v>
       </c>
       <c r="DP3" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DQ3" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DQ3" t="str">
+      <c r="DR3" t="str">
         <f>Tabelle1!AO3</f>
         <v>Boeing 747-8i</v>
       </c>
     </row>
-    <row r="4" spans="1:121" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:122" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>88</v>
       </c>
@@ -8100,14 +8112,17 @@
         <v>88</v>
       </c>
       <c r="DP4" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DQ4" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DQ4" t="str">
+      <c r="DR4" t="str">
         <f>Tabelle1!AO4</f>
         <v>Boeing 787-10</v>
       </c>
     </row>
-    <row r="5" spans="1:121" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:122" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>88</v>
       </c>
@@ -8497,14 +8512,17 @@
         <v>88</v>
       </c>
       <c r="DP5" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DQ5" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DQ5" t="str">
+      <c r="DR5" t="str">
         <f>Tabelle1!AO5</f>
         <v>Boeing F/A 18E Super Hornet</v>
       </c>
     </row>
-    <row r="6" spans="1:121" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:122" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>88</v>
       </c>
@@ -8894,14 +8912,17 @@
         <v>88</v>
       </c>
       <c r="DP6" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DQ6" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DQ6" t="str">
+      <c r="DR6" t="str">
         <f>Tabelle1!AO6</f>
         <v>Baron G58</v>
       </c>
     </row>
-    <row r="7" spans="1:121" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:122" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>88</v>
       </c>
@@ -9291,14 +9312,17 @@
         <v>88</v>
       </c>
       <c r="DP7" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DQ7" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DQ7" t="str">
+      <c r="DR7" t="str">
         <f>Tabelle1!AO7</f>
         <v>Bonanza G36</v>
       </c>
     </row>
-    <row r="8" spans="1:121" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:122" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>88</v>
       </c>
@@ -9688,14 +9712,17 @@
         <v>88</v>
       </c>
       <c r="DP8" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DQ8" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DQ8" t="str">
+      <c r="DR8" t="str">
         <f>Tabelle1!AO8</f>
         <v>Beechcraft King Air 350i</v>
       </c>
     </row>
-    <row r="9" spans="1:121" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:122" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>88</v>
       </c>
@@ -10085,14 +10112,17 @@
         <v>88</v>
       </c>
       <c r="DP9" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DQ9" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DQ9" t="str">
+      <c r="DR9" t="str">
         <f>Tabelle1!AO9</f>
         <v>Cessna 152</v>
       </c>
     </row>
-    <row r="10" spans="1:121" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:122" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>88</v>
       </c>
@@ -10482,14 +10512,17 @@
         <v>88</v>
       </c>
       <c r="DP10" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DQ10" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DQ10" t="str">
+      <c r="DR10" t="str">
         <f>Tabelle1!AO10</f>
         <v>Cessna 152 Aero</v>
       </c>
     </row>
-    <row r="11" spans="1:121" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:122" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>88</v>
       </c>
@@ -10879,14 +10912,17 @@
         <v>88</v>
       </c>
       <c r="DP11" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DQ11" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DQ11" t="str">
+      <c r="DR11" t="str">
         <f>Tabelle1!AO11</f>
         <v>Cessna 172sp Skyhawk G1000</v>
       </c>
     </row>
-    <row r="12" spans="1:121" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:122" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>88</v>
       </c>
@@ -11276,14 +11312,17 @@
         <v>88</v>
       </c>
       <c r="DP12" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DQ12" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DQ12" t="str">
+      <c r="DR12" t="str">
         <f>Tabelle1!AO12</f>
         <v>Cessna 172sp Skyhawk</v>
       </c>
     </row>
-    <row r="13" spans="1:121" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:122" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>88</v>
       </c>
@@ -11673,14 +11712,17 @@
         <v>88</v>
       </c>
       <c r="DP13" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DQ13" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DQ13" t="str">
+      <c r="DR13" t="str">
         <f>Tabelle1!AO13</f>
         <v>Cessna 208B Grand Caravan EX</v>
       </c>
     </row>
-    <row r="14" spans="1:121" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:122" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>88</v>
       </c>
@@ -12070,14 +12112,17 @@
         <v>88</v>
       </c>
       <c r="DP14" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DQ14" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DQ14" t="str">
+      <c r="DR14" t="str">
         <f>Tabelle1!AO14</f>
         <v>Cessna CJ4 Citation</v>
       </c>
     </row>
-    <row r="15" spans="1:121" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:122" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>88</v>
       </c>
@@ -12467,14 +12512,17 @@
         <v>88</v>
       </c>
       <c r="DP15" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DQ15" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DQ15" t="str">
+      <c r="DR15" t="str">
         <f>Tabelle1!AO15</f>
         <v>Cessna Longitude</v>
       </c>
     </row>
-    <row r="16" spans="1:121" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:122" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>88</v>
       </c>
@@ -12864,14 +12912,17 @@
         <v>88</v>
       </c>
       <c r="DP16" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DQ16" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DQ16" t="str">
+      <c r="DR16" t="str">
         <f>Tabelle1!AO16</f>
         <v>DA40-NG</v>
       </c>
     </row>
-    <row r="17" spans="1:121" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:122" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>88</v>
       </c>
@@ -13261,14 +13312,17 @@
         <v>88</v>
       </c>
       <c r="DP17" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DQ17" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DQ17" t="str">
+      <c r="DR17" t="str">
         <f>Tabelle1!AO17</f>
         <v>DA40 TDI</v>
       </c>
     </row>
-    <row r="18" spans="1:121" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:122" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>88</v>
       </c>
@@ -13658,14 +13712,17 @@
         <v>88</v>
       </c>
       <c r="DP18" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DQ18" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DQ18" t="str">
+      <c r="DR18" t="str">
         <f>Tabelle1!AO18</f>
         <v>DA62</v>
       </c>
     </row>
-    <row r="19" spans="1:121" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:122" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>88</v>
       </c>
@@ -14055,14 +14112,17 @@
         <v>88</v>
       </c>
       <c r="DP19" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DQ19" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DQ19" t="str">
+      <c r="DR19" t="str">
         <f>Tabelle1!AO19</f>
         <v>DR400</v>
       </c>
     </row>
-    <row r="20" spans="1:121" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:122" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>88</v>
       </c>
@@ -14452,14 +14512,17 @@
         <v>88</v>
       </c>
       <c r="DP20" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DQ20" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DQ20" t="str">
+      <c r="DR20" t="str">
         <f>Tabelle1!AO20</f>
         <v>DV20</v>
       </c>
     </row>
-    <row r="21" spans="1:121" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:122" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>88</v>
       </c>
@@ -14849,14 +14912,17 @@
         <v>88</v>
       </c>
       <c r="DP21" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DQ21" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DQ21" t="str">
+      <c r="DR21" t="str">
         <f>Tabelle1!AO21</f>
         <v>Extra 330</v>
       </c>
     </row>
-    <row r="22" spans="1:121" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:122" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>88</v>
       </c>
@@ -15246,14 +15312,17 @@
         <v>88</v>
       </c>
       <c r="DP22" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DQ22" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DQ22" t="str">
+      <c r="DR22" t="str">
         <f>Tabelle1!AO22</f>
         <v>FlightDesignCT</v>
       </c>
     </row>
-    <row r="23" spans="1:121" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:122" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>88</v>
       </c>
@@ -15643,14 +15712,17 @@
         <v>88</v>
       </c>
       <c r="DP23" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DQ23" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DQ23" t="str">
+      <c r="DR23" t="str">
         <f>Tabelle1!AO23</f>
         <v>Icon A5</v>
       </c>
     </row>
-    <row r="24" spans="1:121" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:122" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>88</v>
       </c>
@@ -16040,14 +16112,17 @@
         <v>88</v>
       </c>
       <c r="DP24" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DQ24" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DQ24" t="str">
+      <c r="DR24" t="str">
         <f>Tabelle1!AO24</f>
         <v>Mudry Cap 10 C</v>
       </c>
     </row>
-    <row r="25" spans="1:121" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:122" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>88</v>
       </c>
@@ -16437,14 +16512,17 @@
         <v>88</v>
       </c>
       <c r="DP25" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DQ25" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DQ25" t="str">
+      <c r="DR25" t="str">
         <f>Tabelle1!AO25</f>
         <v>Pilatus PC-6 Gauge</v>
       </c>
     </row>
-    <row r="26" spans="1:121" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:122" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>88</v>
       </c>
@@ -16834,14 +16912,17 @@
         <v>88</v>
       </c>
       <c r="DP26" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DQ26" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DQ26" t="str">
+      <c r="DR26" t="str">
         <f>Tabelle1!AO26</f>
         <v>Pilatus PC-6 G950</v>
       </c>
     </row>
-    <row r="27" spans="1:121" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:122" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>88</v>
       </c>
@@ -17231,14 +17312,17 @@
         <v>88</v>
       </c>
       <c r="DP27" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DQ27" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DQ27" t="str">
+      <c r="DR27" t="str">
         <f>Tabelle1!AO27</f>
         <v>Pipistrel Alpha Electro</v>
       </c>
     </row>
-    <row r="28" spans="1:121" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:122" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>88</v>
       </c>
@@ -17628,14 +17712,17 @@
         <v>88</v>
       </c>
       <c r="DP28" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DQ28" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DQ28" t="str">
+      <c r="DR28" t="str">
         <f>Tabelle1!AO28</f>
         <v>Pitts Special 1S</v>
       </c>
     </row>
-    <row r="29" spans="1:121" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:122" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>88</v>
       </c>
@@ -18025,14 +18112,17 @@
         <v>88</v>
       </c>
       <c r="DP29" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DQ29" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DQ29" t="str">
+      <c r="DR29" t="str">
         <f>Tabelle1!AO29</f>
         <v>Pitts Special S2S</v>
       </c>
     </row>
-    <row r="30" spans="1:121" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:122" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>88</v>
       </c>
@@ -18422,14 +18512,17 @@
         <v>88</v>
       </c>
       <c r="DP30" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DQ30" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DQ30" t="str">
+      <c r="DR30" t="str">
         <f>Tabelle1!AO30</f>
         <v>Savage Cub</v>
       </c>
     </row>
-    <row r="31" spans="1:121" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:122" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>88</v>
       </c>
@@ -18819,14 +18912,17 @@
         <v>88</v>
       </c>
       <c r="DP31" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DQ31" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DQ31" t="str">
+      <c r="DR31" t="str">
         <f>Tabelle1!AO31</f>
         <v>Savage Shock Ultra</v>
       </c>
     </row>
-    <row r="32" spans="1:121" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:122" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>88</v>
       </c>
@@ -19216,14 +19312,17 @@
         <v>88</v>
       </c>
       <c r="DP32" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DQ32" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DQ32" t="str">
+      <c r="DR32" t="str">
         <f>Tabelle1!AO32</f>
         <v>SR22</v>
       </c>
     </row>
-    <row r="33" spans="1:121" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:122" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>88</v>
       </c>
@@ -19613,14 +19712,17 @@
         <v>88</v>
       </c>
       <c r="DP33" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DQ33" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DQ33" t="str">
+      <c r="DR33" t="str">
         <f>Tabelle1!AO33</f>
         <v>TBM 930</v>
       </c>
     </row>
-    <row r="34" spans="1:121" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:122" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>88</v>
       </c>
@@ -20010,14 +20112,17 @@
         <v>88</v>
       </c>
       <c r="DP34" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DQ34" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DQ34" t="str">
+      <c r="DR34" t="str">
         <f>Tabelle1!AO34</f>
         <v>Vertigo</v>
       </c>
     </row>
-    <row r="35" spans="1:121" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:122" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
         <v>88</v>
       </c>
@@ -20407,14 +20512,17 @@
         <v>88</v>
       </c>
       <c r="DP35" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DQ35" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DQ35" t="str">
+      <c r="DR35" t="str">
         <f>Tabelle1!AO35</f>
         <v>VL3</v>
       </c>
     </row>
-    <row r="36" spans="1:121" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:122" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>88</v>
       </c>
@@ -20804,14 +20912,17 @@
         <v>88</v>
       </c>
       <c r="DP36" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DQ36" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DQ36" t="str">
+      <c r="DR36" t="str">
         <f>Tabelle1!AO36</f>
         <v>Volocity</v>
       </c>
     </row>
-    <row r="37" spans="1:121" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:122" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
         <v>88</v>
       </c>
@@ -21201,14 +21312,17 @@
         <v>88</v>
       </c>
       <c r="DP37" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DQ37" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DQ37" t="str">
+      <c r="DR37" t="str">
         <f>Tabelle1!AO37</f>
         <v>NXCub</v>
       </c>
     </row>
-    <row r="38" spans="1:121" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:122" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>88</v>
       </c>
@@ -21598,14 +21712,17 @@
         <v>88</v>
       </c>
       <c r="DP38" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DQ38" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DQ38" t="str">
+      <c r="DR38" t="str">
         <f>Tabelle1!AO38</f>
         <v>XCub</v>
       </c>
     </row>
-    <row r="39" spans="1:121" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:122" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>88</v>
       </c>
@@ -21995,14 +22112,17 @@
         <v>88</v>
       </c>
       <c r="DP39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DQ39" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DQ39" t="str">
+      <c r="DR39" t="str">
         <f>Tabelle1!AO39</f>
         <v>SWS Kodiak 100 II</v>
       </c>
     </row>
-    <row r="40" spans="1:121" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:122" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
         <v>88</v>
       </c>
@@ -22392,9 +22512,12 @@
         <v>88</v>
       </c>
       <c r="DP40" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DQ40" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DQ40" t="str">
+      <c r="DR40" t="str">
         <f>Tabelle1!AO40</f>
         <v>Generic Glider</v>
       </c>

</xml_diff>

<commit_message>
V 0.48-B45 PreRel for Audio Init Tests - Add AP Attitude Hold Item - Update Setup for Audio Speech Render Device (VoiceOut) - Add Debug module
</commit_message>
<xml_diff>
--- a/Config/EngineMerge.xlsx
+++ b/Config/EngineMerge.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3830" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3870" uniqueCount="278">
   <si>
     <t>ACFT</t>
   </si>
@@ -849,6 +849,9 @@
   </si>
   <si>
     <t>TXT</t>
+  </si>
+  <si>
+    <t>ATT</t>
   </si>
 </sst>
 </file>
@@ -6539,10 +6542,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DR40"/>
+  <dimension ref="A1:DS40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="CR26" sqref="CR26"/>
+      <selection activeCell="DO42" sqref="DO42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6550,11 +6553,11 @@
     <col min="1" max="75" width="3.7109375" bestFit="1" customWidth="1"/>
     <col min="76" max="77" width="3.7109375" customWidth="1"/>
     <col min="78" max="86" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="87" max="121" width="3.7109375" customWidth="1"/>
-    <col min="122" max="122" width="36.28515625" customWidth="1"/>
+    <col min="87" max="122" width="3.7109375" customWidth="1"/>
+    <col min="123" max="123" width="36.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:122" s="11" customFormat="1" ht="72" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:123" s="11" customFormat="1" ht="72" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>95</v>
       </c>
@@ -6916,13 +6919,16 @@
         <v>276</v>
       </c>
       <c r="DQ1" s="11" t="s">
+        <v>277</v>
+      </c>
+      <c r="DR1" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="DR1" t="s">
+      <c r="DS1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:122" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:123" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>88</v>
       </c>
@@ -7315,14 +7321,17 @@
         <v>88</v>
       </c>
       <c r="DQ2" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DR2" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DR2" t="str">
+      <c r="DS2" t="str">
         <f>Tabelle1!AO2</f>
         <v>Airbus A320 Neo</v>
       </c>
     </row>
-    <row r="3" spans="1:122" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:123" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>88</v>
       </c>
@@ -7715,14 +7724,17 @@
         <v>88</v>
       </c>
       <c r="DQ3" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DR3" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DR3" t="str">
+      <c r="DS3" t="str">
         <f>Tabelle1!AO3</f>
         <v>Boeing 747-8i</v>
       </c>
     </row>
-    <row r="4" spans="1:122" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:123" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>88</v>
       </c>
@@ -8115,14 +8127,17 @@
         <v>88</v>
       </c>
       <c r="DQ4" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DR4" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DR4" t="str">
+      <c r="DS4" t="str">
         <f>Tabelle1!AO4</f>
         <v>Boeing 787-10</v>
       </c>
     </row>
-    <row r="5" spans="1:122" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:123" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>88</v>
       </c>
@@ -8515,14 +8530,17 @@
         <v>88</v>
       </c>
       <c r="DQ5" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DR5" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DR5" t="str">
+      <c r="DS5" t="str">
         <f>Tabelle1!AO5</f>
         <v>Boeing F/A 18E Super Hornet</v>
       </c>
     </row>
-    <row r="6" spans="1:122" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:123" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>88</v>
       </c>
@@ -8915,14 +8933,17 @@
         <v>88</v>
       </c>
       <c r="DQ6" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DR6" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DR6" t="str">
+      <c r="DS6" t="str">
         <f>Tabelle1!AO6</f>
         <v>Baron G58</v>
       </c>
     </row>
-    <row r="7" spans="1:122" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:123" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>88</v>
       </c>
@@ -9315,14 +9336,17 @@
         <v>88</v>
       </c>
       <c r="DQ7" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DR7" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DR7" t="str">
+      <c r="DS7" t="str">
         <f>Tabelle1!AO7</f>
         <v>Bonanza G36</v>
       </c>
     </row>
-    <row r="8" spans="1:122" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:123" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>88</v>
       </c>
@@ -9715,14 +9739,17 @@
         <v>88</v>
       </c>
       <c r="DQ8" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DR8" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DR8" t="str">
+      <c r="DS8" t="str">
         <f>Tabelle1!AO8</f>
         <v>Beechcraft King Air 350i</v>
       </c>
     </row>
-    <row r="9" spans="1:122" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:123" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>88</v>
       </c>
@@ -10115,14 +10142,17 @@
         <v>88</v>
       </c>
       <c r="DQ9" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DR9" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DR9" t="str">
+      <c r="DS9" t="str">
         <f>Tabelle1!AO9</f>
         <v>Cessna 152</v>
       </c>
     </row>
-    <row r="10" spans="1:122" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:123" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>88</v>
       </c>
@@ -10515,14 +10545,17 @@
         <v>88</v>
       </c>
       <c r="DQ10" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DR10" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DR10" t="str">
+      <c r="DS10" t="str">
         <f>Tabelle1!AO10</f>
         <v>Cessna 152 Aero</v>
       </c>
     </row>
-    <row r="11" spans="1:122" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:123" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>88</v>
       </c>
@@ -10915,14 +10948,17 @@
         <v>88</v>
       </c>
       <c r="DQ11" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DR11" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DR11" t="str">
+      <c r="DS11" t="str">
         <f>Tabelle1!AO11</f>
         <v>Cessna 172sp Skyhawk G1000</v>
       </c>
     </row>
-    <row r="12" spans="1:122" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:123" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>88</v>
       </c>
@@ -11315,14 +11351,17 @@
         <v>88</v>
       </c>
       <c r="DQ12" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DR12" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DR12" t="str">
+      <c r="DS12" t="str">
         <f>Tabelle1!AO12</f>
         <v>Cessna 172sp Skyhawk</v>
       </c>
     </row>
-    <row r="13" spans="1:122" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:123" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>88</v>
       </c>
@@ -11715,14 +11754,17 @@
         <v>88</v>
       </c>
       <c r="DQ13" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DR13" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DR13" t="str">
+      <c r="DS13" t="str">
         <f>Tabelle1!AO13</f>
         <v>Cessna 208B Grand Caravan EX</v>
       </c>
     </row>
-    <row r="14" spans="1:122" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:123" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>88</v>
       </c>
@@ -12115,14 +12157,17 @@
         <v>88</v>
       </c>
       <c r="DQ14" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DR14" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DR14" t="str">
+      <c r="DS14" t="str">
         <f>Tabelle1!AO14</f>
         <v>Cessna CJ4 Citation</v>
       </c>
     </row>
-    <row r="15" spans="1:122" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:123" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>88</v>
       </c>
@@ -12515,14 +12560,17 @@
         <v>88</v>
       </c>
       <c r="DQ15" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DR15" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DR15" t="str">
+      <c r="DS15" t="str">
         <f>Tabelle1!AO15</f>
         <v>Cessna Longitude</v>
       </c>
     </row>
-    <row r="16" spans="1:122" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:123" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>88</v>
       </c>
@@ -12915,14 +12963,17 @@
         <v>88</v>
       </c>
       <c r="DQ16" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DR16" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DR16" t="str">
+      <c r="DS16" t="str">
         <f>Tabelle1!AO16</f>
         <v>DA40-NG</v>
       </c>
     </row>
-    <row r="17" spans="1:122" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:123" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>88</v>
       </c>
@@ -13315,14 +13366,17 @@
         <v>88</v>
       </c>
       <c r="DQ17" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DR17" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DR17" t="str">
+      <c r="DS17" t="str">
         <f>Tabelle1!AO17</f>
         <v>DA40 TDI</v>
       </c>
     </row>
-    <row r="18" spans="1:122" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:123" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>88</v>
       </c>
@@ -13715,14 +13769,17 @@
         <v>88</v>
       </c>
       <c r="DQ18" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DR18" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DR18" t="str">
+      <c r="DS18" t="str">
         <f>Tabelle1!AO18</f>
         <v>DA62</v>
       </c>
     </row>
-    <row r="19" spans="1:122" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:123" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>88</v>
       </c>
@@ -14115,14 +14172,17 @@
         <v>88</v>
       </c>
       <c r="DQ19" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DR19" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DR19" t="str">
+      <c r="DS19" t="str">
         <f>Tabelle1!AO19</f>
         <v>DR400</v>
       </c>
     </row>
-    <row r="20" spans="1:122" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:123" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>88</v>
       </c>
@@ -14515,14 +14575,17 @@
         <v>88</v>
       </c>
       <c r="DQ20" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DR20" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DR20" t="str">
+      <c r="DS20" t="str">
         <f>Tabelle1!AO20</f>
         <v>DV20</v>
       </c>
     </row>
-    <row r="21" spans="1:122" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:123" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>88</v>
       </c>
@@ -14915,14 +14978,17 @@
         <v>88</v>
       </c>
       <c r="DQ21" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DR21" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DR21" t="str">
+      <c r="DS21" t="str">
         <f>Tabelle1!AO21</f>
         <v>Extra 330</v>
       </c>
     </row>
-    <row r="22" spans="1:122" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:123" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>88</v>
       </c>
@@ -15315,14 +15381,17 @@
         <v>88</v>
       </c>
       <c r="DQ22" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DR22" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DR22" t="str">
+      <c r="DS22" t="str">
         <f>Tabelle1!AO22</f>
         <v>FlightDesignCT</v>
       </c>
     </row>
-    <row r="23" spans="1:122" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:123" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>88</v>
       </c>
@@ -15715,14 +15784,17 @@
         <v>88</v>
       </c>
       <c r="DQ23" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DR23" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DR23" t="str">
+      <c r="DS23" t="str">
         <f>Tabelle1!AO23</f>
         <v>Icon A5</v>
       </c>
     </row>
-    <row r="24" spans="1:122" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:123" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>88</v>
       </c>
@@ -16115,14 +16187,17 @@
         <v>88</v>
       </c>
       <c r="DQ24" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DR24" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DR24" t="str">
+      <c r="DS24" t="str">
         <f>Tabelle1!AO24</f>
         <v>Mudry Cap 10 C</v>
       </c>
     </row>
-    <row r="25" spans="1:122" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:123" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>88</v>
       </c>
@@ -16515,14 +16590,17 @@
         <v>88</v>
       </c>
       <c r="DQ25" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DR25" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DR25" t="str">
+      <c r="DS25" t="str">
         <f>Tabelle1!AO25</f>
         <v>Pilatus PC-6 Gauge</v>
       </c>
     </row>
-    <row r="26" spans="1:122" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:123" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>88</v>
       </c>
@@ -16915,14 +16993,17 @@
         <v>88</v>
       </c>
       <c r="DQ26" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DR26" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DR26" t="str">
+      <c r="DS26" t="str">
         <f>Tabelle1!AO26</f>
         <v>Pilatus PC-6 G950</v>
       </c>
     </row>
-    <row r="27" spans="1:122" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:123" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>88</v>
       </c>
@@ -17315,14 +17396,17 @@
         <v>88</v>
       </c>
       <c r="DQ27" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DR27" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DR27" t="str">
+      <c r="DS27" t="str">
         <f>Tabelle1!AO27</f>
         <v>Pipistrel Alpha Electro</v>
       </c>
     </row>
-    <row r="28" spans="1:122" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:123" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>88</v>
       </c>
@@ -17715,14 +17799,17 @@
         <v>88</v>
       </c>
       <c r="DQ28" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DR28" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DR28" t="str">
+      <c r="DS28" t="str">
         <f>Tabelle1!AO28</f>
         <v>Pitts Special 1S</v>
       </c>
     </row>
-    <row r="29" spans="1:122" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:123" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>88</v>
       </c>
@@ -18115,14 +18202,17 @@
         <v>88</v>
       </c>
       <c r="DQ29" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DR29" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DR29" t="str">
+      <c r="DS29" t="str">
         <f>Tabelle1!AO29</f>
         <v>Pitts Special S2S</v>
       </c>
     </row>
-    <row r="30" spans="1:122" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:123" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>88</v>
       </c>
@@ -18515,14 +18605,17 @@
         <v>88</v>
       </c>
       <c r="DQ30" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DR30" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DR30" t="str">
+      <c r="DS30" t="str">
         <f>Tabelle1!AO30</f>
         <v>Savage Cub</v>
       </c>
     </row>
-    <row r="31" spans="1:122" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:123" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>88</v>
       </c>
@@ -18915,14 +19008,17 @@
         <v>88</v>
       </c>
       <c r="DQ31" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DR31" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DR31" t="str">
+      <c r="DS31" t="str">
         <f>Tabelle1!AO31</f>
         <v>Savage Shock Ultra</v>
       </c>
     </row>
-    <row r="32" spans="1:122" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:123" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>88</v>
       </c>
@@ -19315,14 +19411,17 @@
         <v>88</v>
       </c>
       <c r="DQ32" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DR32" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DR32" t="str">
+      <c r="DS32" t="str">
         <f>Tabelle1!AO32</f>
         <v>SR22</v>
       </c>
     </row>
-    <row r="33" spans="1:122" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:123" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>88</v>
       </c>
@@ -19715,14 +19814,17 @@
         <v>88</v>
       </c>
       <c r="DQ33" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DR33" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DR33" t="str">
+      <c r="DS33" t="str">
         <f>Tabelle1!AO33</f>
         <v>TBM 930</v>
       </c>
     </row>
-    <row r="34" spans="1:122" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:123" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>88</v>
       </c>
@@ -20115,14 +20217,17 @@
         <v>88</v>
       </c>
       <c r="DQ34" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DR34" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DR34" t="str">
+      <c r="DS34" t="str">
         <f>Tabelle1!AO34</f>
         <v>Vertigo</v>
       </c>
     </row>
-    <row r="35" spans="1:122" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:123" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
         <v>88</v>
       </c>
@@ -20515,14 +20620,17 @@
         <v>88</v>
       </c>
       <c r="DQ35" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DR35" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DR35" t="str">
+      <c r="DS35" t="str">
         <f>Tabelle1!AO35</f>
         <v>VL3</v>
       </c>
     </row>
-    <row r="36" spans="1:122" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:123" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>88</v>
       </c>
@@ -20915,14 +21023,17 @@
         <v>88</v>
       </c>
       <c r="DQ36" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DR36" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DR36" t="str">
+      <c r="DS36" t="str">
         <f>Tabelle1!AO36</f>
         <v>Volocity</v>
       </c>
     </row>
-    <row r="37" spans="1:122" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:123" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
         <v>88</v>
       </c>
@@ -21315,14 +21426,17 @@
         <v>88</v>
       </c>
       <c r="DQ37" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DR37" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DR37" t="str">
+      <c r="DS37" t="str">
         <f>Tabelle1!AO37</f>
         <v>NXCub</v>
       </c>
     </row>
-    <row r="38" spans="1:122" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:123" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>88</v>
       </c>
@@ -21715,14 +21829,17 @@
         <v>88</v>
       </c>
       <c r="DQ38" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DR38" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DR38" t="str">
+      <c r="DS38" t="str">
         <f>Tabelle1!AO38</f>
         <v>XCub</v>
       </c>
     </row>
-    <row r="39" spans="1:122" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:123" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>88</v>
       </c>
@@ -22115,14 +22232,17 @@
         <v>88</v>
       </c>
       <c r="DQ39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DR39" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DR39" t="str">
+      <c r="DS39" t="str">
         <f>Tabelle1!AO39</f>
         <v>SWS Kodiak 100 II</v>
       </c>
     </row>
-    <row r="40" spans="1:122" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:123" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
         <v>88</v>
       </c>
@@ -22515,9 +22635,12 @@
         <v>88</v>
       </c>
       <c r="DQ40" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DR40" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DR40" t="str">
+      <c r="DS40" t="str">
         <f>Tabelle1!AO40</f>
         <v>Generic Glider</v>
       </c>

</xml_diff>

<commit_message>
V 0.48-B45 Intermediate consolidation - Add Engine 3 and 4 support - Add AP Attitude Hold Item - Add AP AutoThrottle item (ATHR, TOGA) - Add AP IAS Speed Hold item - Add COM Activ, Standby Frequ. (with mouse dial and swap) - Add NAV Activ, Standby Frequ. (with mouse dial and swap) - Update Setup for Audio Speech Render Device (VoiceOut) - Add Debug module - Refactoring of the Layout procedure - Fix some issues found throughout
</commit_message>
<xml_diff>
--- a/Config/EngineMerge.xlsx
+++ b/Config/EngineMerge.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3870" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4110" uniqueCount="284">
   <si>
     <t>ACFT</t>
   </si>
@@ -851,7 +851,25 @@
     <t>TXT</t>
   </si>
   <si>
-    <t>ATT</t>
+    <t>AP_ATT</t>
+  </si>
+  <si>
+    <t>COM1</t>
+  </si>
+  <si>
+    <t>COM1_NAME</t>
+  </si>
+  <si>
+    <t>COM2</t>
+  </si>
+  <si>
+    <t>COM2_NAME</t>
+  </si>
+  <si>
+    <t>NAV1_F</t>
+  </si>
+  <si>
+    <t>NAV2_F</t>
   </si>
 </sst>
 </file>
@@ -6542,10 +6560,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DS40"/>
+  <dimension ref="A1:DY40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="DO42" sqref="DO42"/>
+      <selection activeCell="BN42" sqref="BN42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6553,11 +6571,11 @@
     <col min="1" max="75" width="3.7109375" bestFit="1" customWidth="1"/>
     <col min="76" max="77" width="3.7109375" customWidth="1"/>
     <col min="78" max="86" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="87" max="122" width="3.7109375" customWidth="1"/>
-    <col min="123" max="123" width="36.28515625" customWidth="1"/>
+    <col min="87" max="128" width="3.7109375" customWidth="1"/>
+    <col min="129" max="129" width="36.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:123" s="11" customFormat="1" ht="72" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:129" s="11" customFormat="1" ht="72" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>95</v>
       </c>
@@ -6922,13 +6940,31 @@
         <v>277</v>
       </c>
       <c r="DR1" s="11" t="s">
+        <v>278</v>
+      </c>
+      <c r="DS1" s="11" t="s">
+        <v>279</v>
+      </c>
+      <c r="DT1" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="DU1" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="DV1" s="11" t="s">
+        <v>282</v>
+      </c>
+      <c r="DW1" s="11" t="s">
+        <v>283</v>
+      </c>
+      <c r="DX1" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="DS1" t="s">
+      <c r="DY1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>88</v>
       </c>
@@ -7324,14 +7360,32 @@
         <v>88</v>
       </c>
       <c r="DR2" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DS2" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DT2" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DU2" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DV2" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DW2" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DX2" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DS2" t="str">
+      <c r="DY2" t="str">
         <f>Tabelle1!AO2</f>
         <v>Airbus A320 Neo</v>
       </c>
     </row>
-    <row r="3" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>88</v>
       </c>
@@ -7727,14 +7781,32 @@
         <v>88</v>
       </c>
       <c r="DR3" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DS3" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DT3" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DU3" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DV3" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DW3" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DX3" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DS3" t="str">
+      <c r="DY3" t="str">
         <f>Tabelle1!AO3</f>
         <v>Boeing 747-8i</v>
       </c>
     </row>
-    <row r="4" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>88</v>
       </c>
@@ -8130,14 +8202,32 @@
         <v>88</v>
       </c>
       <c r="DR4" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DS4" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DT4" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DU4" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DV4" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DW4" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DX4" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DS4" t="str">
+      <c r="DY4" t="str">
         <f>Tabelle1!AO4</f>
         <v>Boeing 787-10</v>
       </c>
     </row>
-    <row r="5" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>88</v>
       </c>
@@ -8533,14 +8623,32 @@
         <v>88</v>
       </c>
       <c r="DR5" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DS5" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DT5" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DU5" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DV5" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DW5" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DX5" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DS5" t="str">
+      <c r="DY5" t="str">
         <f>Tabelle1!AO5</f>
         <v>Boeing F/A 18E Super Hornet</v>
       </c>
     </row>
-    <row r="6" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>88</v>
       </c>
@@ -8936,14 +9044,32 @@
         <v>88</v>
       </c>
       <c r="DR6" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DS6" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DT6" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DU6" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DV6" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DW6" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DX6" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DS6" t="str">
+      <c r="DY6" t="str">
         <f>Tabelle1!AO6</f>
         <v>Baron G58</v>
       </c>
     </row>
-    <row r="7" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>88</v>
       </c>
@@ -9339,14 +9465,32 @@
         <v>88</v>
       </c>
       <c r="DR7" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DS7" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DT7" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DU7" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DV7" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DW7" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DX7" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DS7" t="str">
+      <c r="DY7" t="str">
         <f>Tabelle1!AO7</f>
         <v>Bonanza G36</v>
       </c>
     </row>
-    <row r="8" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>88</v>
       </c>
@@ -9742,14 +9886,32 @@
         <v>88</v>
       </c>
       <c r="DR8" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DS8" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DT8" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DU8" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DV8" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DW8" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DX8" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DS8" t="str">
+      <c r="DY8" t="str">
         <f>Tabelle1!AO8</f>
         <v>Beechcraft King Air 350i</v>
       </c>
     </row>
-    <row r="9" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>88</v>
       </c>
@@ -10145,14 +10307,32 @@
         <v>88</v>
       </c>
       <c r="DR9" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DS9" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DT9" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DU9" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DV9" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DW9" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DX9" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DS9" t="str">
+      <c r="DY9" t="str">
         <f>Tabelle1!AO9</f>
         <v>Cessna 152</v>
       </c>
     </row>
-    <row r="10" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>88</v>
       </c>
@@ -10548,14 +10728,32 @@
         <v>88</v>
       </c>
       <c r="DR10" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DS10" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DT10" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DU10" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DV10" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DW10" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DX10" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DS10" t="str">
+      <c r="DY10" t="str">
         <f>Tabelle1!AO10</f>
         <v>Cessna 152 Aero</v>
       </c>
     </row>
-    <row r="11" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>88</v>
       </c>
@@ -10951,14 +11149,32 @@
         <v>88</v>
       </c>
       <c r="DR11" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DS11" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DT11" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DU11" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DV11" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DW11" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DX11" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DS11" t="str">
+      <c r="DY11" t="str">
         <f>Tabelle1!AO11</f>
         <v>Cessna 172sp Skyhawk G1000</v>
       </c>
     </row>
-    <row r="12" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>88</v>
       </c>
@@ -11354,14 +11570,32 @@
         <v>88</v>
       </c>
       <c r="DR12" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DS12" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DT12" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DU12" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DV12" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DW12" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DX12" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DS12" t="str">
+      <c r="DY12" t="str">
         <f>Tabelle1!AO12</f>
         <v>Cessna 172sp Skyhawk</v>
       </c>
     </row>
-    <row r="13" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>88</v>
       </c>
@@ -11757,14 +11991,32 @@
         <v>88</v>
       </c>
       <c r="DR13" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DS13" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DT13" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DU13" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DV13" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DW13" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DX13" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DS13" t="str">
+      <c r="DY13" t="str">
         <f>Tabelle1!AO13</f>
         <v>Cessna 208B Grand Caravan EX</v>
       </c>
     </row>
-    <row r="14" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>88</v>
       </c>
@@ -12160,14 +12412,32 @@
         <v>88</v>
       </c>
       <c r="DR14" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DS14" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DT14" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DU14" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DV14" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DW14" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DX14" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DS14" t="str">
+      <c r="DY14" t="str">
         <f>Tabelle1!AO14</f>
         <v>Cessna CJ4 Citation</v>
       </c>
     </row>
-    <row r="15" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>88</v>
       </c>
@@ -12563,14 +12833,32 @@
         <v>88</v>
       </c>
       <c r="DR15" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DS15" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DT15" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DU15" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DV15" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DW15" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DX15" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DS15" t="str">
+      <c r="DY15" t="str">
         <f>Tabelle1!AO15</f>
         <v>Cessna Longitude</v>
       </c>
     </row>
-    <row r="16" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>88</v>
       </c>
@@ -12966,14 +13254,32 @@
         <v>88</v>
       </c>
       <c r="DR16" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DS16" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DT16" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DU16" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DV16" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DW16" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DX16" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DS16" t="str">
+      <c r="DY16" t="str">
         <f>Tabelle1!AO16</f>
         <v>DA40-NG</v>
       </c>
     </row>
-    <row r="17" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>88</v>
       </c>
@@ -13369,14 +13675,32 @@
         <v>88</v>
       </c>
       <c r="DR17" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DS17" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DT17" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DU17" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DV17" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DW17" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DX17" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DS17" t="str">
+      <c r="DY17" t="str">
         <f>Tabelle1!AO17</f>
         <v>DA40 TDI</v>
       </c>
     </row>
-    <row r="18" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>88</v>
       </c>
@@ -13772,14 +14096,32 @@
         <v>88</v>
       </c>
       <c r="DR18" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DS18" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DT18" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DU18" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DV18" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DW18" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DX18" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DS18" t="str">
+      <c r="DY18" t="str">
         <f>Tabelle1!AO18</f>
         <v>DA62</v>
       </c>
     </row>
-    <row r="19" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>88</v>
       </c>
@@ -14175,14 +14517,32 @@
         <v>88</v>
       </c>
       <c r="DR19" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DS19" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DT19" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DU19" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DV19" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DW19" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DX19" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DS19" t="str">
+      <c r="DY19" t="str">
         <f>Tabelle1!AO19</f>
         <v>DR400</v>
       </c>
     </row>
-    <row r="20" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>88</v>
       </c>
@@ -14578,14 +14938,32 @@
         <v>88</v>
       </c>
       <c r="DR20" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DS20" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DT20" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DU20" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DV20" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DW20" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DX20" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DS20" t="str">
+      <c r="DY20" t="str">
         <f>Tabelle1!AO20</f>
         <v>DV20</v>
       </c>
     </row>
-    <row r="21" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>88</v>
       </c>
@@ -14981,14 +15359,32 @@
         <v>88</v>
       </c>
       <c r="DR21" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DS21" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DT21" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DU21" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DV21" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DW21" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DX21" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DS21" t="str">
+      <c r="DY21" t="str">
         <f>Tabelle1!AO21</f>
         <v>Extra 330</v>
       </c>
     </row>
-    <row r="22" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>88</v>
       </c>
@@ -15384,14 +15780,32 @@
         <v>88</v>
       </c>
       <c r="DR22" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DS22" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DT22" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DU22" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DV22" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DW22" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DX22" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DS22" t="str">
+      <c r="DY22" t="str">
         <f>Tabelle1!AO22</f>
         <v>FlightDesignCT</v>
       </c>
     </row>
-    <row r="23" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>88</v>
       </c>
@@ -15787,14 +16201,32 @@
         <v>88</v>
       </c>
       <c r="DR23" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DS23" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DT23" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DU23" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DV23" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DW23" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DX23" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DS23" t="str">
+      <c r="DY23" t="str">
         <f>Tabelle1!AO23</f>
         <v>Icon A5</v>
       </c>
     </row>
-    <row r="24" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>88</v>
       </c>
@@ -16190,14 +16622,32 @@
         <v>88</v>
       </c>
       <c r="DR24" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DS24" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DT24" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DU24" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DV24" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DW24" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DX24" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DS24" t="str">
+      <c r="DY24" t="str">
         <f>Tabelle1!AO24</f>
         <v>Mudry Cap 10 C</v>
       </c>
     </row>
-    <row r="25" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>88</v>
       </c>
@@ -16593,14 +17043,32 @@
         <v>88</v>
       </c>
       <c r="DR25" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DS25" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DT25" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DU25" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DV25" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DW25" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DX25" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DS25" t="str">
+      <c r="DY25" t="str">
         <f>Tabelle1!AO25</f>
         <v>Pilatus PC-6 Gauge</v>
       </c>
     </row>
-    <row r="26" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>88</v>
       </c>
@@ -16996,14 +17464,32 @@
         <v>88</v>
       </c>
       <c r="DR26" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DS26" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DT26" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DU26" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DV26" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DW26" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DX26" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DS26" t="str">
+      <c r="DY26" t="str">
         <f>Tabelle1!AO26</f>
         <v>Pilatus PC-6 G950</v>
       </c>
     </row>
-    <row r="27" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>88</v>
       </c>
@@ -17399,14 +17885,32 @@
         <v>88</v>
       </c>
       <c r="DR27" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DS27" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DT27" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DU27" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DV27" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DW27" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DX27" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DS27" t="str">
+      <c r="DY27" t="str">
         <f>Tabelle1!AO27</f>
         <v>Pipistrel Alpha Electro</v>
       </c>
     </row>
-    <row r="28" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>88</v>
       </c>
@@ -17802,14 +18306,32 @@
         <v>88</v>
       </c>
       <c r="DR28" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DS28" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DT28" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DU28" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DV28" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DW28" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DX28" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DS28" t="str">
+      <c r="DY28" t="str">
         <f>Tabelle1!AO28</f>
         <v>Pitts Special 1S</v>
       </c>
     </row>
-    <row r="29" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>88</v>
       </c>
@@ -18205,14 +18727,32 @@
         <v>88</v>
       </c>
       <c r="DR29" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DS29" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DT29" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DU29" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DV29" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DW29" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DX29" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DS29" t="str">
+      <c r="DY29" t="str">
         <f>Tabelle1!AO29</f>
         <v>Pitts Special S2S</v>
       </c>
     </row>
-    <row r="30" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>88</v>
       </c>
@@ -18608,14 +19148,32 @@
         <v>88</v>
       </c>
       <c r="DR30" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DS30" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DT30" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DU30" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DV30" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DW30" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DX30" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DS30" t="str">
+      <c r="DY30" t="str">
         <f>Tabelle1!AO30</f>
         <v>Savage Cub</v>
       </c>
     </row>
-    <row r="31" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>88</v>
       </c>
@@ -19011,14 +19569,32 @@
         <v>88</v>
       </c>
       <c r="DR31" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DS31" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DT31" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DU31" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DV31" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DW31" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DX31" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DS31" t="str">
+      <c r="DY31" t="str">
         <f>Tabelle1!AO31</f>
         <v>Savage Shock Ultra</v>
       </c>
     </row>
-    <row r="32" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>88</v>
       </c>
@@ -19414,14 +19990,32 @@
         <v>88</v>
       </c>
       <c r="DR32" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DS32" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DT32" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DU32" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DV32" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DW32" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DX32" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DS32" t="str">
+      <c r="DY32" t="str">
         <f>Tabelle1!AO32</f>
         <v>SR22</v>
       </c>
     </row>
-    <row r="33" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>88</v>
       </c>
@@ -19817,14 +20411,32 @@
         <v>88</v>
       </c>
       <c r="DR33" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DS33" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DT33" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DU33" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DV33" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DW33" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DX33" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DS33" t="str">
+      <c r="DY33" t="str">
         <f>Tabelle1!AO33</f>
         <v>TBM 930</v>
       </c>
     </row>
-    <row r="34" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>88</v>
       </c>
@@ -20220,14 +20832,32 @@
         <v>88</v>
       </c>
       <c r="DR34" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DS34" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DT34" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DU34" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DV34" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DW34" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DX34" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DS34" t="str">
+      <c r="DY34" t="str">
         <f>Tabelle1!AO34</f>
         <v>Vertigo</v>
       </c>
     </row>
-    <row r="35" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
         <v>88</v>
       </c>
@@ -20623,14 +21253,32 @@
         <v>88</v>
       </c>
       <c r="DR35" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DS35" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DT35" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DU35" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DV35" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DW35" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DX35" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DS35" t="str">
+      <c r="DY35" t="str">
         <f>Tabelle1!AO35</f>
         <v>VL3</v>
       </c>
     </row>
-    <row r="36" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>88</v>
       </c>
@@ -21026,14 +21674,32 @@
         <v>88</v>
       </c>
       <c r="DR36" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DS36" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DT36" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DU36" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DV36" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DW36" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DX36" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DS36" t="str">
+      <c r="DY36" t="str">
         <f>Tabelle1!AO36</f>
         <v>Volocity</v>
       </c>
     </row>
-    <row r="37" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
         <v>88</v>
       </c>
@@ -21429,14 +22095,32 @@
         <v>88</v>
       </c>
       <c r="DR37" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DS37" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DT37" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DU37" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DV37" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DW37" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DX37" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DS37" t="str">
+      <c r="DY37" t="str">
         <f>Tabelle1!AO37</f>
         <v>NXCub</v>
       </c>
     </row>
-    <row r="38" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>88</v>
       </c>
@@ -21832,14 +22516,32 @@
         <v>88</v>
       </c>
       <c r="DR38" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DS38" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DT38" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DU38" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DV38" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DW38" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DX38" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DS38" t="str">
+      <c r="DY38" t="str">
         <f>Tabelle1!AO38</f>
         <v>XCub</v>
       </c>
     </row>
-    <row r="39" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>88</v>
       </c>
@@ -22235,14 +22937,32 @@
         <v>88</v>
       </c>
       <c r="DR39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DS39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DT39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DU39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DV39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DW39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DX39" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DS39" t="str">
+      <c r="DY39" t="str">
         <f>Tabelle1!AO39</f>
         <v>SWS Kodiak 100 II</v>
       </c>
     </row>
-    <row r="40" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
         <v>88</v>
       </c>
@@ -22638,9 +23358,27 @@
         <v>88</v>
       </c>
       <c r="DR40" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DS40" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DT40" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DU40" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DV40" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DW40" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="DX40" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="DS40" t="str">
+      <c r="DY40" t="str">
         <f>Tabelle1!AO40</f>
         <v>Generic Glider</v>
       </c>

</xml_diff>

<commit_message>
V 0.48-B45 - bug fixes and final release - Add Engine 3 and 4 support - Add AP AutoThrottle item (ATHR, TOGA) - experimental, scroll to change, TOGA click to toggle - Add AP AutoBrake item (ABRK) - experimental, scroll to change - Add AP IAS/MACH Speed Hold item - Add AP Attitude Hold Item - Update AP Setting handling (mouse scroll over the setting number - not the Label anymore) - Update AP HDG setting number, click to set to current heading - Update AP ALT mode handling (as the Sim does not provide correct states) - Update AP settings, visual background changed to indicate active settings - Add COM Activ, Standby Frequ. (with mouse dial and swap) - Add NAV Activ, Standby Frequ. (with mouse dial and swap) - Add A320 Throttle Position Indicator - Update Setup for Audio Speech Render Device (VoiceOut) - Add Debug module - Refactoring of the Layout procedure - Fix some issues found throughout - Update QuickGuide
</commit_message>
<xml_diff>
--- a/Config/EngineMerge.xlsx
+++ b/Config/EngineMerge.xlsx
@@ -11,14 +11,14 @@
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$AR$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$AS$1</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4116" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4118" uniqueCount="288">
   <si>
     <t>ACFT</t>
   </si>
@@ -879,6 +879,9 @@
   </si>
   <si>
     <t>AP_SPDs</t>
+  </si>
+  <si>
+    <t>A320THR</t>
   </si>
 </sst>
 </file>
@@ -1405,10 +1408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AS42"/>
+  <dimension ref="A1:AT42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AO15" sqref="AO15"/>
+      <selection activeCell="AQ3" sqref="AQ3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1421,11 +1424,11 @@
     <col min="7" max="31" width="3.7109375" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="3.28515625" customWidth="1"/>
     <col min="33" max="39" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="40" max="43" width="3.7109375" customWidth="1"/>
-    <col min="44" max="45" width="36.28515625" customWidth="1"/>
+    <col min="40" max="44" width="3.7109375" customWidth="1"/>
+    <col min="45" max="46" width="36.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" s="11" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:46" s="11" customFormat="1" ht="57" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -1552,17 +1555,20 @@
       <c r="AP1" s="33" t="s">
         <v>286</v>
       </c>
-      <c r="AQ1" s="31" t="s">
+      <c r="AQ1" s="33" t="s">
+        <v>287</v>
+      </c>
+      <c r="AR1" s="31" t="s">
         <v>275</v>
       </c>
-      <c r="AR1" s="11" t="s">
+      <c r="AS1" s="11" t="s">
         <v>220</v>
       </c>
-      <c r="AS1" s="11" t="s">
+      <c r="AT1" s="11" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>20</v>
       </c>
@@ -1690,17 +1696,20 @@
       <c r="AP2" s="34">
         <v>1</v>
       </c>
-      <c r="AQ2" s="32">
-        <v>0</v>
-      </c>
-      <c r="AR2" t="s">
+      <c r="AQ2" s="34">
+        <v>1</v>
+      </c>
+      <c r="AR2" s="32">
+        <v>0</v>
+      </c>
+      <c r="AS2" t="s">
         <v>196</v>
       </c>
-      <c r="AS2" t="s">
+      <c r="AT2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>22</v>
       </c>
@@ -1828,17 +1837,20 @@
       <c r="AP3" s="34">
         <v>1</v>
       </c>
-      <c r="AQ3" s="32">
-        <v>0</v>
-      </c>
-      <c r="AR3" t="s">
+      <c r="AQ3" s="34">
+        <v>0</v>
+      </c>
+      <c r="AR3" s="32">
+        <v>0</v>
+      </c>
+      <c r="AS3" t="s">
         <v>198</v>
       </c>
-      <c r="AS3" t="s">
+      <c r="AT3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>21</v>
       </c>
@@ -1966,17 +1978,20 @@
       <c r="AP4" s="34">
         <v>1</v>
       </c>
-      <c r="AQ4" s="32">
-        <v>0</v>
-      </c>
-      <c r="AR4" t="s">
+      <c r="AQ4" s="34">
+        <v>0</v>
+      </c>
+      <c r="AR4" s="32">
+        <v>0</v>
+      </c>
+      <c r="AS4" t="s">
         <v>197</v>
       </c>
-      <c r="AS4" t="s">
+      <c r="AT4" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>211</v>
       </c>
@@ -2104,17 +2119,20 @@
       <c r="AP5" s="34">
         <v>0</v>
       </c>
-      <c r="AQ5" s="32">
-        <v>0</v>
-      </c>
-      <c r="AR5" t="s">
+      <c r="AQ5" s="34">
+        <v>0</v>
+      </c>
+      <c r="AR5" s="32">
+        <v>0</v>
+      </c>
+      <c r="AS5" t="s">
         <v>217</v>
       </c>
-      <c r="AS5" t="s">
+      <c r="AT5" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
@@ -2242,17 +2260,20 @@
       <c r="AP6" s="34">
         <v>0</v>
       </c>
-      <c r="AQ6" s="32">
-        <v>0</v>
-      </c>
-      <c r="AR6" t="s">
+      <c r="AQ6" s="34">
+        <v>0</v>
+      </c>
+      <c r="AR6" s="32">
+        <v>0</v>
+      </c>
+      <c r="AS6" t="s">
         <v>187</v>
       </c>
-      <c r="AS6" t="s">
+      <c r="AT6" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
@@ -2380,17 +2401,20 @@
       <c r="AP7" s="34">
         <v>0</v>
       </c>
-      <c r="AQ7" s="32">
-        <v>0</v>
-      </c>
-      <c r="AR7" t="s">
+      <c r="AQ7" s="34">
+        <v>0</v>
+      </c>
+      <c r="AR7" s="32">
+        <v>0</v>
+      </c>
+      <c r="AS7" t="s">
         <v>188</v>
       </c>
-      <c r="AS7" t="s">
+      <c r="AT7" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>39</v>
       </c>
@@ -2518,17 +2542,20 @@
       <c r="AP8" s="34">
         <v>0</v>
       </c>
-      <c r="AQ8" s="32">
-        <v>0</v>
-      </c>
-      <c r="AR8" t="s">
+      <c r="AQ8" s="34">
+        <v>0</v>
+      </c>
+      <c r="AR8" s="32">
+        <v>0</v>
+      </c>
+      <c r="AS8" t="s">
         <v>194</v>
       </c>
-      <c r="AS8" t="s">
+      <c r="AT8" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>27</v>
       </c>
@@ -2656,17 +2683,20 @@
       <c r="AP9" s="34">
         <v>0</v>
       </c>
-      <c r="AQ9" s="32">
-        <v>0</v>
-      </c>
-      <c r="AR9" t="s">
+      <c r="AQ9" s="34">
+        <v>0</v>
+      </c>
+      <c r="AR9" s="32">
+        <v>0</v>
+      </c>
+      <c r="AS9" t="s">
         <v>176</v>
       </c>
-      <c r="AS9" t="s">
+      <c r="AT9" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
@@ -2794,17 +2824,20 @@
       <c r="AP10" s="34">
         <v>0</v>
       </c>
-      <c r="AQ10" s="32">
-        <v>0</v>
-      </c>
-      <c r="AR10" t="s">
+      <c r="AQ10" s="34">
+        <v>0</v>
+      </c>
+      <c r="AR10" s="32">
+        <v>0</v>
+      </c>
+      <c r="AS10" t="s">
         <v>177</v>
       </c>
-      <c r="AS10" t="s">
+      <c r="AT10" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -2932,17 +2965,20 @@
       <c r="AP11" s="34">
         <v>0</v>
       </c>
-      <c r="AQ11" s="32">
-        <v>0</v>
-      </c>
-      <c r="AR11" t="s">
+      <c r="AQ11" s="34">
+        <v>0</v>
+      </c>
+      <c r="AR11" s="32">
+        <v>0</v>
+      </c>
+      <c r="AS11" t="s">
         <v>201</v>
       </c>
-      <c r="AS11" t="s">
+      <c r="AT11" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>29</v>
       </c>
@@ -3070,17 +3106,20 @@
       <c r="AP12" s="34">
         <v>0</v>
       </c>
-      <c r="AQ12" s="32">
-        <v>0</v>
-      </c>
-      <c r="AR12" t="s">
+      <c r="AQ12" s="34">
+        <v>0</v>
+      </c>
+      <c r="AR12" s="32">
+        <v>0</v>
+      </c>
+      <c r="AS12" t="s">
         <v>202</v>
       </c>
-      <c r="AS12" t="s">
+      <c r="AT12" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>18</v>
       </c>
@@ -3208,17 +3247,20 @@
       <c r="AP13" s="34">
         <v>0</v>
       </c>
-      <c r="AQ13" s="32">
-        <v>0</v>
-      </c>
-      <c r="AR13" t="s">
-        <v>52</v>
+      <c r="AQ13" s="34">
+        <v>0</v>
+      </c>
+      <c r="AR13" s="32">
+        <v>0</v>
       </c>
       <c r="AS13" t="s">
         <v>52</v>
       </c>
+      <c r="AT13" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>31</v>
       </c>
@@ -3346,17 +3388,20 @@
       <c r="AP14" s="34">
         <v>1</v>
       </c>
-      <c r="AQ14" s="32">
-        <v>0</v>
-      </c>
-      <c r="AR14" t="s">
+      <c r="AQ14" s="34">
+        <v>0</v>
+      </c>
+      <c r="AR14" s="32">
+        <v>0</v>
+      </c>
+      <c r="AS14" t="s">
         <v>199</v>
       </c>
-      <c r="AS14" t="s">
+      <c r="AT14" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>40</v>
       </c>
@@ -3484,17 +3529,20 @@
       <c r="AP15" s="34">
         <v>1</v>
       </c>
-      <c r="AQ15" s="32">
-        <v>0</v>
-      </c>
-      <c r="AR15" t="s">
+      <c r="AQ15" s="34">
+        <v>0</v>
+      </c>
+      <c r="AR15" s="32">
+        <v>0</v>
+      </c>
+      <c r="AS15" t="s">
         <v>200</v>
       </c>
-      <c r="AS15" t="s">
+      <c r="AT15" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>32</v>
       </c>
@@ -3622,17 +3670,20 @@
       <c r="AP16" s="34">
         <v>0</v>
       </c>
-      <c r="AQ16" s="32">
-        <v>0</v>
-      </c>
-      <c r="AR16" t="s">
+      <c r="AQ16" s="34">
+        <v>0</v>
+      </c>
+      <c r="AR16" s="32">
+        <v>0</v>
+      </c>
+      <c r="AS16" t="s">
         <v>191</v>
       </c>
-      <c r="AS16" t="s">
+      <c r="AT16" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>33</v>
       </c>
@@ -3760,17 +3811,20 @@
       <c r="AP17" s="34">
         <v>0</v>
       </c>
-      <c r="AQ17" s="32">
-        <v>0</v>
-      </c>
-      <c r="AR17" t="s">
+      <c r="AQ17" s="34">
+        <v>0</v>
+      </c>
+      <c r="AR17" s="32">
+        <v>0</v>
+      </c>
+      <c r="AS17" t="s">
         <v>192</v>
       </c>
-      <c r="AS17" t="s">
+      <c r="AT17" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>13</v>
       </c>
@@ -3898,17 +3952,20 @@
       <c r="AP18" s="34">
         <v>0</v>
       </c>
-      <c r="AQ18" s="32">
-        <v>0</v>
-      </c>
-      <c r="AR18" t="s">
+      <c r="AQ18" s="34">
+        <v>0</v>
+      </c>
+      <c r="AR18" s="32">
+        <v>0</v>
+      </c>
+      <c r="AS18" t="s">
         <v>193</v>
       </c>
-      <c r="AS18" t="s">
+      <c r="AT18" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>34</v>
       </c>
@@ -4036,17 +4093,20 @@
       <c r="AP19" s="34">
         <v>0</v>
       </c>
-      <c r="AQ19" s="32">
-        <v>0</v>
-      </c>
-      <c r="AR19" t="s">
+      <c r="AQ19" s="34">
+        <v>0</v>
+      </c>
+      <c r="AR19" s="32">
+        <v>0</v>
+      </c>
+      <c r="AS19" t="s">
         <v>184</v>
       </c>
-      <c r="AS19" t="s">
+      <c r="AT19" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>35</v>
       </c>
@@ -4174,17 +4234,20 @@
       <c r="AP20" s="34">
         <v>0</v>
       </c>
-      <c r="AQ20" s="32">
-        <v>0</v>
-      </c>
-      <c r="AR20" t="s">
+      <c r="AQ20" s="34">
+        <v>0</v>
+      </c>
+      <c r="AR20" s="32">
+        <v>0</v>
+      </c>
+      <c r="AS20" t="s">
         <v>180</v>
       </c>
-      <c r="AS20" t="s">
+      <c r="AT20" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>36</v>
       </c>
@@ -4312,17 +4375,20 @@
       <c r="AP21" s="34">
         <v>0</v>
       </c>
-      <c r="AQ21" s="32">
-        <v>0</v>
-      </c>
-      <c r="AR21" t="s">
+      <c r="AQ21" s="34">
+        <v>0</v>
+      </c>
+      <c r="AR21" s="32">
+        <v>0</v>
+      </c>
+      <c r="AS21" t="s">
         <v>189</v>
       </c>
-      <c r="AS21" t="s">
+      <c r="AT21" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>37</v>
       </c>
@@ -4450,17 +4516,20 @@
       <c r="AP22" s="34">
         <v>0</v>
       </c>
-      <c r="AQ22" s="32">
-        <v>0</v>
-      </c>
-      <c r="AR22" t="s">
+      <c r="AQ22" s="34">
+        <v>0</v>
+      </c>
+      <c r="AR22" s="32">
+        <v>0</v>
+      </c>
+      <c r="AS22" t="s">
         <v>185</v>
       </c>
-      <c r="AS22" t="s">
+      <c r="AT22" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>38</v>
       </c>
@@ -4588,17 +4657,20 @@
       <c r="AP23" s="34">
         <v>0</v>
       </c>
-      <c r="AQ23" s="32">
-        <v>0</v>
-      </c>
-      <c r="AR23" t="s">
+      <c r="AQ23" s="34">
+        <v>0</v>
+      </c>
+      <c r="AR23" s="32">
+        <v>0</v>
+      </c>
+      <c r="AS23" t="s">
         <v>178</v>
       </c>
-      <c r="AS23" t="s">
+      <c r="AT23" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
@@ -4726,17 +4798,20 @@
       <c r="AP24" s="34">
         <v>0</v>
       </c>
-      <c r="AQ24" s="32">
-        <v>0</v>
-      </c>
-      <c r="AR24" t="s">
-        <v>54</v>
+      <c r="AQ24" s="34">
+        <v>0</v>
+      </c>
+      <c r="AR24" s="32">
+        <v>0</v>
       </c>
       <c r="AS24" t="s">
         <v>54</v>
       </c>
+      <c r="AT24" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="25" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>207</v>
       </c>
@@ -4864,17 +4939,20 @@
       <c r="AP25" s="34">
         <v>0</v>
       </c>
-      <c r="AQ25" s="32">
-        <v>0</v>
-      </c>
-      <c r="AR25" t="s">
-        <v>207</v>
+      <c r="AQ25" s="34">
+        <v>0</v>
+      </c>
+      <c r="AR25" s="32">
+        <v>0</v>
       </c>
       <c r="AS25" t="s">
         <v>207</v>
       </c>
+      <c r="AT25" t="s">
+        <v>207</v>
+      </c>
     </row>
-    <row r="26" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>208</v>
       </c>
@@ -5002,17 +5080,20 @@
       <c r="AP26" s="34">
         <v>0</v>
       </c>
-      <c r="AQ26" s="32">
-        <v>0</v>
-      </c>
-      <c r="AR26" t="s">
-        <v>208</v>
+      <c r="AQ26" s="34">
+        <v>0</v>
+      </c>
+      <c r="AR26" s="32">
+        <v>0</v>
       </c>
       <c r="AS26" t="s">
         <v>208</v>
       </c>
+      <c r="AT26" t="s">
+        <v>208</v>
+      </c>
     </row>
-    <row r="27" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>41</v>
       </c>
@@ -5140,17 +5221,20 @@
       <c r="AP27" s="34">
         <v>0</v>
       </c>
-      <c r="AQ27" s="32">
-        <v>0</v>
-      </c>
-      <c r="AR27" t="s">
+      <c r="AQ27" s="34">
+        <v>0</v>
+      </c>
+      <c r="AR27" s="32">
+        <v>0</v>
+      </c>
+      <c r="AS27" t="s">
         <v>181</v>
       </c>
-      <c r="AS27" t="s">
+      <c r="AT27" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="28" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>214</v>
       </c>
@@ -5278,17 +5362,20 @@
       <c r="AP28" s="34">
         <v>0</v>
       </c>
-      <c r="AQ28" s="32">
-        <v>0</v>
-      </c>
-      <c r="AR28" t="s">
+      <c r="AQ28" s="34">
+        <v>0</v>
+      </c>
+      <c r="AR28" s="32">
+        <v>0</v>
+      </c>
+      <c r="AS28" t="s">
         <v>218</v>
       </c>
-      <c r="AS28" t="s">
+      <c r="AT28" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="29" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>42</v>
       </c>
@@ -5416,17 +5503,20 @@
       <c r="AP29" s="34">
         <v>0</v>
       </c>
-      <c r="AQ29" s="32">
-        <v>0</v>
-      </c>
-      <c r="AR29" t="s">
+      <c r="AQ29" s="34">
+        <v>0</v>
+      </c>
+      <c r="AR29" s="32">
+        <v>0</v>
+      </c>
+      <c r="AS29" t="s">
         <v>219</v>
       </c>
-      <c r="AS29" t="s">
+      <c r="AT29" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>43</v>
       </c>
@@ -5554,17 +5644,20 @@
       <c r="AP30" s="34">
         <v>0</v>
       </c>
-      <c r="AQ30" s="32">
-        <v>0</v>
-      </c>
-      <c r="AR30" t="s">
+      <c r="AQ30" s="34">
+        <v>0</v>
+      </c>
+      <c r="AR30" s="32">
+        <v>0</v>
+      </c>
+      <c r="AS30" t="s">
         <v>186</v>
       </c>
-      <c r="AS30" t="s">
+      <c r="AT30" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>44</v>
       </c>
@@ -5692,17 +5785,20 @@
       <c r="AP31" s="34">
         <v>0</v>
       </c>
-      <c r="AQ31" s="32">
-        <v>0</v>
-      </c>
-      <c r="AR31" t="s">
+      <c r="AQ31" s="34">
+        <v>0</v>
+      </c>
+      <c r="AR31" s="32">
+        <v>0</v>
+      </c>
+      <c r="AS31" t="s">
         <v>182</v>
       </c>
-      <c r="AS31" t="s">
+      <c r="AT31" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="32" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>45</v>
       </c>
@@ -5830,17 +5926,20 @@
       <c r="AP32" s="34">
         <v>0</v>
       </c>
-      <c r="AQ32" s="32">
-        <v>0</v>
-      </c>
-      <c r="AR32" t="s">
+      <c r="AQ32" s="34">
+        <v>0</v>
+      </c>
+      <c r="AR32" s="32">
+        <v>0</v>
+      </c>
+      <c r="AS32" t="s">
         <v>179</v>
       </c>
-      <c r="AS32" t="s">
+      <c r="AT32" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="33" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>15</v>
       </c>
@@ -5968,17 +6067,20 @@
       <c r="AP33" s="34">
         <v>0</v>
       </c>
-      <c r="AQ33" s="32">
-        <v>0</v>
-      </c>
-      <c r="AR33" t="s">
+      <c r="AQ33" s="34">
+        <v>0</v>
+      </c>
+      <c r="AR33" s="32">
+        <v>0</v>
+      </c>
+      <c r="AS33" t="s">
         <v>195</v>
       </c>
-      <c r="AS33" t="s">
+      <c r="AT33" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="34" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>93</v>
       </c>
@@ -6106,17 +6208,20 @@
       <c r="AP34" s="34">
         <v>0</v>
       </c>
-      <c r="AQ34" s="32">
-        <v>0</v>
-      </c>
-      <c r="AR34" t="s">
-        <v>92</v>
+      <c r="AQ34" s="34">
+        <v>0</v>
+      </c>
+      <c r="AR34" s="32">
+        <v>0</v>
       </c>
       <c r="AS34" t="s">
         <v>92</v>
       </c>
+      <c r="AT34" t="s">
+        <v>92</v>
+      </c>
     </row>
-    <row r="35" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>46</v>
       </c>
@@ -6244,17 +6349,20 @@
       <c r="AP35" s="34">
         <v>0</v>
       </c>
-      <c r="AQ35" s="32">
-        <v>0</v>
-      </c>
-      <c r="AR35" t="s">
+      <c r="AQ35" s="34">
+        <v>0</v>
+      </c>
+      <c r="AR35" s="32">
+        <v>0</v>
+      </c>
+      <c r="AS35" t="s">
         <v>183</v>
       </c>
-      <c r="AS35" t="s">
+      <c r="AT35" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="36" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>205</v>
       </c>
@@ -6382,17 +6490,20 @@
       <c r="AP36" s="34">
         <v>0</v>
       </c>
-      <c r="AQ36" s="32">
-        <v>0</v>
-      </c>
-      <c r="AR36" t="s">
-        <v>205</v>
+      <c r="AQ36" s="34">
+        <v>0</v>
+      </c>
+      <c r="AR36" s="32">
+        <v>0</v>
       </c>
       <c r="AS36" t="s">
         <v>205</v>
       </c>
+      <c r="AT36" t="s">
+        <v>205</v>
+      </c>
     </row>
-    <row r="37" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>209</v>
       </c>
@@ -6520,17 +6631,20 @@
       <c r="AP37" s="34">
         <v>0</v>
       </c>
-      <c r="AQ37" s="32">
-        <v>0</v>
-      </c>
-      <c r="AR37" t="s">
+      <c r="AQ37" s="34">
+        <v>0</v>
+      </c>
+      <c r="AR37" s="32">
+        <v>0</v>
+      </c>
+      <c r="AS37" t="s">
         <v>216</v>
       </c>
-      <c r="AS37" t="s">
+      <c r="AT37" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="38" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>47</v>
       </c>
@@ -6658,17 +6772,20 @@
       <c r="AP38" s="34">
         <v>0</v>
       </c>
-      <c r="AQ38" s="32">
-        <v>0</v>
-      </c>
-      <c r="AR38" t="s">
+      <c r="AQ38" s="34">
+        <v>0</v>
+      </c>
+      <c r="AR38" s="32">
+        <v>0</v>
+      </c>
+      <c r="AS38" t="s">
         <v>190</v>
       </c>
-      <c r="AS38" t="s">
+      <c r="AT38" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="39" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>245</v>
       </c>
@@ -6796,14 +6913,17 @@
       <c r="AP39" s="34">
         <v>0</v>
       </c>
-      <c r="AQ39" s="32">
-        <v>0</v>
-      </c>
-      <c r="AR39" t="s">
+      <c r="AQ39" s="34">
+        <v>0</v>
+      </c>
+      <c r="AR39" s="32">
+        <v>0</v>
+      </c>
+      <c r="AS39" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="40" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
         <v>258</v>
       </c>
@@ -6930,17 +7050,20 @@
       <c r="AP40" s="34">
         <v>0</v>
       </c>
-      <c r="AQ40" s="32">
-        <v>1</v>
-      </c>
-      <c r="AR40" t="s">
+      <c r="AQ40" s="34">
+        <v>0</v>
+      </c>
+      <c r="AR40" s="32">
+        <v>1</v>
+      </c>
+      <c r="AS40" t="s">
         <v>260</v>
       </c>
-      <c r="AS40" t="s">
+      <c r="AT40" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="42" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:46" x14ac:dyDescent="0.25">
       <c r="AF42" t="s">
         <v>204</v>
       </c>
@@ -6952,10 +7075,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:EB40"/>
+  <dimension ref="A1:EC40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="CQ1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="ED13" sqref="ED13"/>
+      <selection activeCell="ED35" sqref="ED35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6963,11 +7086,11 @@
     <col min="1" max="75" width="3.7109375" bestFit="1" customWidth="1"/>
     <col min="76" max="77" width="3.7109375" customWidth="1"/>
     <col min="78" max="86" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="87" max="131" width="3.7109375" customWidth="1"/>
-    <col min="132" max="132" width="36.28515625" customWidth="1"/>
+    <col min="87" max="132" width="3.7109375" customWidth="1"/>
+    <col min="133" max="133" width="36.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:132" s="11" customFormat="1" ht="72" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:133" s="11" customFormat="1" ht="72" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>95</v>
       </c>
@@ -7359,13 +7482,16 @@
         <v>283</v>
       </c>
       <c r="EA1" s="11" t="s">
+        <v>287</v>
+      </c>
+      <c r="EB1" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="EB1" t="s">
+      <c r="EC1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:133" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>88</v>
       </c>
@@ -7712,7 +7838,7 @@
         <v>1</v>
       </c>
       <c r="DB2" s="12">
-        <f>Tabelle1!AQ2</f>
+        <f>Tabelle1!AR2</f>
         <v>0</v>
       </c>
       <c r="DC2" s="12" t="s">
@@ -7790,15 +7916,19 @@
       <c r="DZ2" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EA2" s="12" t="s">
+      <c r="EA2" s="12">
+        <f>Tabelle1!AQ2</f>
+        <v>1</v>
+      </c>
+      <c r="EB2" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EB2" t="str">
-        <f>Tabelle1!AR2</f>
+      <c r="EC2" t="str">
+        <f>Tabelle1!AS2</f>
         <v>Airbus A320 Neo</v>
       </c>
     </row>
-    <row r="3" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:133" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>88</v>
       </c>
@@ -8145,7 +8275,7 @@
         <v>0</v>
       </c>
       <c r="DB3" s="12">
-        <f>Tabelle1!AQ3</f>
+        <f>Tabelle1!AR3</f>
         <v>0</v>
       </c>
       <c r="DC3" s="12" t="s">
@@ -8223,15 +8353,19 @@
       <c r="DZ3" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EA3" s="12" t="s">
+      <c r="EA3" s="12">
+        <f>Tabelle1!AQ3</f>
+        <v>0</v>
+      </c>
+      <c r="EB3" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EB3" t="str">
-        <f>Tabelle1!AR3</f>
+      <c r="EC3" t="str">
+        <f>Tabelle1!AS3</f>
         <v>Boeing 747-8i</v>
       </c>
     </row>
-    <row r="4" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:133" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>88</v>
       </c>
@@ -8578,7 +8712,7 @@
         <v>0</v>
       </c>
       <c r="DB4" s="12">
-        <f>Tabelle1!AQ4</f>
+        <f>Tabelle1!AR4</f>
         <v>0</v>
       </c>
       <c r="DC4" s="12" t="s">
@@ -8656,15 +8790,19 @@
       <c r="DZ4" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EA4" s="12" t="s">
+      <c r="EA4" s="12">
+        <f>Tabelle1!AQ4</f>
+        <v>0</v>
+      </c>
+      <c r="EB4" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EB4" t="str">
-        <f>Tabelle1!AR4</f>
+      <c r="EC4" t="str">
+        <f>Tabelle1!AS4</f>
         <v>Boeing 787-10</v>
       </c>
     </row>
-    <row r="5" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:133" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>88</v>
       </c>
@@ -9011,7 +9149,7 @@
         <v>0</v>
       </c>
       <c r="DB5" s="12">
-        <f>Tabelle1!AQ5</f>
+        <f>Tabelle1!AR5</f>
         <v>0</v>
       </c>
       <c r="DC5" s="12" t="s">
@@ -9089,15 +9227,19 @@
       <c r="DZ5" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EA5" s="12" t="s">
+      <c r="EA5" s="12">
+        <f>Tabelle1!AQ5</f>
+        <v>0</v>
+      </c>
+      <c r="EB5" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EB5" t="str">
-        <f>Tabelle1!AR5</f>
+      <c r="EC5" t="str">
+        <f>Tabelle1!AS5</f>
         <v>Boeing F/A 18E Super Hornet</v>
       </c>
     </row>
-    <row r="6" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:133" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>88</v>
       </c>
@@ -9444,7 +9586,7 @@
         <v>0</v>
       </c>
       <c r="DB6" s="12">
-        <f>Tabelle1!AQ6</f>
+        <f>Tabelle1!AR6</f>
         <v>0</v>
       </c>
       <c r="DC6" s="12" t="s">
@@ -9522,15 +9664,19 @@
       <c r="DZ6" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EA6" s="12" t="s">
+      <c r="EA6" s="12">
+        <f>Tabelle1!AQ6</f>
+        <v>0</v>
+      </c>
+      <c r="EB6" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EB6" t="str">
-        <f>Tabelle1!AR6</f>
+      <c r="EC6" t="str">
+        <f>Tabelle1!AS6</f>
         <v>Baron G58</v>
       </c>
     </row>
-    <row r="7" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:133" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>88</v>
       </c>
@@ -9877,7 +10023,7 @@
         <v>0</v>
       </c>
       <c r="DB7" s="12">
-        <f>Tabelle1!AQ7</f>
+        <f>Tabelle1!AR7</f>
         <v>0</v>
       </c>
       <c r="DC7" s="12" t="s">
@@ -9955,15 +10101,19 @@
       <c r="DZ7" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EA7" s="12" t="s">
+      <c r="EA7" s="12">
+        <f>Tabelle1!AQ7</f>
+        <v>0</v>
+      </c>
+      <c r="EB7" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EB7" t="str">
-        <f>Tabelle1!AR7</f>
+      <c r="EC7" t="str">
+        <f>Tabelle1!AS7</f>
         <v>Bonanza G36</v>
       </c>
     </row>
-    <row r="8" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:133" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>88</v>
       </c>
@@ -10310,7 +10460,7 @@
         <v>0</v>
       </c>
       <c r="DB8" s="12">
-        <f>Tabelle1!AQ8</f>
+        <f>Tabelle1!AR8</f>
         <v>0</v>
       </c>
       <c r="DC8" s="12" t="s">
@@ -10388,15 +10538,19 @@
       <c r="DZ8" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EA8" s="12" t="s">
+      <c r="EA8" s="12">
+        <f>Tabelle1!AQ8</f>
+        <v>0</v>
+      </c>
+      <c r="EB8" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EB8" t="str">
-        <f>Tabelle1!AR8</f>
+      <c r="EC8" t="str">
+        <f>Tabelle1!AS8</f>
         <v>Beechcraft King Air 350i</v>
       </c>
     </row>
-    <row r="9" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:133" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>88</v>
       </c>
@@ -10743,7 +10897,7 @@
         <v>0</v>
       </c>
       <c r="DB9" s="12">
-        <f>Tabelle1!AQ9</f>
+        <f>Tabelle1!AR9</f>
         <v>0</v>
       </c>
       <c r="DC9" s="12" t="s">
@@ -10821,15 +10975,19 @@
       <c r="DZ9" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EA9" s="12" t="s">
+      <c r="EA9" s="12">
+        <f>Tabelle1!AQ9</f>
+        <v>0</v>
+      </c>
+      <c r="EB9" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EB9" t="str">
-        <f>Tabelle1!AR9</f>
+      <c r="EC9" t="str">
+        <f>Tabelle1!AS9</f>
         <v>Cessna 152</v>
       </c>
     </row>
-    <row r="10" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:133" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>88</v>
       </c>
@@ -11176,7 +11334,7 @@
         <v>0</v>
       </c>
       <c r="DB10" s="12">
-        <f>Tabelle1!AQ10</f>
+        <f>Tabelle1!AR10</f>
         <v>0</v>
       </c>
       <c r="DC10" s="12" t="s">
@@ -11254,15 +11412,19 @@
       <c r="DZ10" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EA10" s="12" t="s">
+      <c r="EA10" s="12">
+        <f>Tabelle1!AQ10</f>
+        <v>0</v>
+      </c>
+      <c r="EB10" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EB10" t="str">
-        <f>Tabelle1!AR10</f>
+      <c r="EC10" t="str">
+        <f>Tabelle1!AS10</f>
         <v>Cessna 152 Aero</v>
       </c>
     </row>
-    <row r="11" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:133" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>88</v>
       </c>
@@ -11609,7 +11771,7 @@
         <v>0</v>
       </c>
       <c r="DB11" s="12">
-        <f>Tabelle1!AQ11</f>
+        <f>Tabelle1!AR11</f>
         <v>0</v>
       </c>
       <c r="DC11" s="12" t="s">
@@ -11687,15 +11849,19 @@
       <c r="DZ11" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EA11" s="12" t="s">
+      <c r="EA11" s="12">
+        <f>Tabelle1!AQ11</f>
+        <v>0</v>
+      </c>
+      <c r="EB11" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EB11" t="str">
-        <f>Tabelle1!AR11</f>
+      <c r="EC11" t="str">
+        <f>Tabelle1!AS11</f>
         <v>Cessna 172sp Skyhawk G1000</v>
       </c>
     </row>
-    <row r="12" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:133" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>88</v>
       </c>
@@ -12042,7 +12208,7 @@
         <v>0</v>
       </c>
       <c r="DB12" s="12">
-        <f>Tabelle1!AQ12</f>
+        <f>Tabelle1!AR12</f>
         <v>0</v>
       </c>
       <c r="DC12" s="12" t="s">
@@ -12120,15 +12286,19 @@
       <c r="DZ12" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EA12" s="12" t="s">
+      <c r="EA12" s="12">
+        <f>Tabelle1!AQ12</f>
+        <v>0</v>
+      </c>
+      <c r="EB12" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EB12" t="str">
-        <f>Tabelle1!AR12</f>
+      <c r="EC12" t="str">
+        <f>Tabelle1!AS12</f>
         <v>Cessna 172sp Skyhawk</v>
       </c>
     </row>
-    <row r="13" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:133" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>88</v>
       </c>
@@ -12475,7 +12645,7 @@
         <v>0</v>
       </c>
       <c r="DB13" s="12">
-        <f>Tabelle1!AQ13</f>
+        <f>Tabelle1!AR13</f>
         <v>0</v>
       </c>
       <c r="DC13" s="12" t="s">
@@ -12553,15 +12723,19 @@
       <c r="DZ13" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EA13" s="12" t="s">
+      <c r="EA13" s="12">
+        <f>Tabelle1!AQ13</f>
+        <v>0</v>
+      </c>
+      <c r="EB13" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EB13" t="str">
-        <f>Tabelle1!AR13</f>
+      <c r="EC13" t="str">
+        <f>Tabelle1!AS13</f>
         <v>Cessna 208B Grand Caravan EX</v>
       </c>
     </row>
-    <row r="14" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:133" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>88</v>
       </c>
@@ -12908,7 +13082,7 @@
         <v>0</v>
       </c>
       <c r="DB14" s="12">
-        <f>Tabelle1!AQ14</f>
+        <f>Tabelle1!AR14</f>
         <v>0</v>
       </c>
       <c r="DC14" s="12" t="s">
@@ -12986,15 +13160,19 @@
       <c r="DZ14" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EA14" s="12" t="s">
+      <c r="EA14" s="12">
+        <f>Tabelle1!AQ14</f>
+        <v>0</v>
+      </c>
+      <c r="EB14" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EB14" t="str">
-        <f>Tabelle1!AR14</f>
+      <c r="EC14" t="str">
+        <f>Tabelle1!AS14</f>
         <v>Cessna CJ4 Citation</v>
       </c>
     </row>
-    <row r="15" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:133" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>88</v>
       </c>
@@ -13341,7 +13519,7 @@
         <v>0</v>
       </c>
       <c r="DB15" s="12">
-        <f>Tabelle1!AQ15</f>
+        <f>Tabelle1!AR15</f>
         <v>0</v>
       </c>
       <c r="DC15" s="12" t="s">
@@ -13419,15 +13597,19 @@
       <c r="DZ15" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EA15" s="12" t="s">
+      <c r="EA15" s="12">
+        <f>Tabelle1!AQ15</f>
+        <v>0</v>
+      </c>
+      <c r="EB15" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EB15" t="str">
-        <f>Tabelle1!AR15</f>
+      <c r="EC15" t="str">
+        <f>Tabelle1!AS15</f>
         <v>Cessna Longitude</v>
       </c>
     </row>
-    <row r="16" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:133" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>88</v>
       </c>
@@ -13774,7 +13956,7 @@
         <v>0</v>
       </c>
       <c r="DB16" s="12">
-        <f>Tabelle1!AQ16</f>
+        <f>Tabelle1!AR16</f>
         <v>0</v>
       </c>
       <c r="DC16" s="12" t="s">
@@ -13852,15 +14034,19 @@
       <c r="DZ16" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EA16" s="12" t="s">
+      <c r="EA16" s="12">
+        <f>Tabelle1!AQ16</f>
+        <v>0</v>
+      </c>
+      <c r="EB16" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EB16" t="str">
-        <f>Tabelle1!AR16</f>
+      <c r="EC16" t="str">
+        <f>Tabelle1!AS16</f>
         <v>DA40-NG</v>
       </c>
     </row>
-    <row r="17" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:133" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>88</v>
       </c>
@@ -14207,7 +14393,7 @@
         <v>0</v>
       </c>
       <c r="DB17" s="12">
-        <f>Tabelle1!AQ17</f>
+        <f>Tabelle1!AR17</f>
         <v>0</v>
       </c>
       <c r="DC17" s="12" t="s">
@@ -14285,15 +14471,19 @@
       <c r="DZ17" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EA17" s="12" t="s">
+      <c r="EA17" s="12">
+        <f>Tabelle1!AQ17</f>
+        <v>0</v>
+      </c>
+      <c r="EB17" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EB17" t="str">
-        <f>Tabelle1!AR17</f>
+      <c r="EC17" t="str">
+        <f>Tabelle1!AS17</f>
         <v>DA40 TDI</v>
       </c>
     </row>
-    <row r="18" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:133" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>88</v>
       </c>
@@ -14640,7 +14830,7 @@
         <v>0</v>
       </c>
       <c r="DB18" s="12">
-        <f>Tabelle1!AQ18</f>
+        <f>Tabelle1!AR18</f>
         <v>0</v>
       </c>
       <c r="DC18" s="12" t="s">
@@ -14718,15 +14908,19 @@
       <c r="DZ18" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EA18" s="12" t="s">
+      <c r="EA18" s="12">
+        <f>Tabelle1!AQ18</f>
+        <v>0</v>
+      </c>
+      <c r="EB18" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EB18" t="str">
-        <f>Tabelle1!AR18</f>
+      <c r="EC18" t="str">
+        <f>Tabelle1!AS18</f>
         <v>DA62</v>
       </c>
     </row>
-    <row r="19" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:133" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>88</v>
       </c>
@@ -15073,7 +15267,7 @@
         <v>0</v>
       </c>
       <c r="DB19" s="12">
-        <f>Tabelle1!AQ19</f>
+        <f>Tabelle1!AR19</f>
         <v>0</v>
       </c>
       <c r="DC19" s="12" t="s">
@@ -15151,15 +15345,19 @@
       <c r="DZ19" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EA19" s="12" t="s">
+      <c r="EA19" s="12">
+        <f>Tabelle1!AQ19</f>
+        <v>0</v>
+      </c>
+      <c r="EB19" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EB19" t="str">
-        <f>Tabelle1!AR19</f>
+      <c r="EC19" t="str">
+        <f>Tabelle1!AS19</f>
         <v>DR400</v>
       </c>
     </row>
-    <row r="20" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:133" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>88</v>
       </c>
@@ -15506,7 +15704,7 @@
         <v>0</v>
       </c>
       <c r="DB20" s="12">
-        <f>Tabelle1!AQ20</f>
+        <f>Tabelle1!AR20</f>
         <v>0</v>
       </c>
       <c r="DC20" s="12" t="s">
@@ -15584,15 +15782,19 @@
       <c r="DZ20" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EA20" s="12" t="s">
+      <c r="EA20" s="12">
+        <f>Tabelle1!AQ20</f>
+        <v>0</v>
+      </c>
+      <c r="EB20" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EB20" t="str">
-        <f>Tabelle1!AR20</f>
+      <c r="EC20" t="str">
+        <f>Tabelle1!AS20</f>
         <v>DV20</v>
       </c>
     </row>
-    <row r="21" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:133" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>88</v>
       </c>
@@ -15939,7 +16141,7 @@
         <v>0</v>
       </c>
       <c r="DB21" s="12">
-        <f>Tabelle1!AQ21</f>
+        <f>Tabelle1!AR21</f>
         <v>0</v>
       </c>
       <c r="DC21" s="12" t="s">
@@ -16017,15 +16219,19 @@
       <c r="DZ21" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EA21" s="12" t="s">
+      <c r="EA21" s="12">
+        <f>Tabelle1!AQ21</f>
+        <v>0</v>
+      </c>
+      <c r="EB21" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EB21" t="str">
-        <f>Tabelle1!AR21</f>
+      <c r="EC21" t="str">
+        <f>Tabelle1!AS21</f>
         <v>Extra 330</v>
       </c>
     </row>
-    <row r="22" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:133" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>88</v>
       </c>
@@ -16372,7 +16578,7 @@
         <v>0</v>
       </c>
       <c r="DB22" s="12">
-        <f>Tabelle1!AQ22</f>
+        <f>Tabelle1!AR22</f>
         <v>0</v>
       </c>
       <c r="DC22" s="12" t="s">
@@ -16450,15 +16656,19 @@
       <c r="DZ22" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EA22" s="12" t="s">
+      <c r="EA22" s="12">
+        <f>Tabelle1!AQ22</f>
+        <v>0</v>
+      </c>
+      <c r="EB22" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EB22" t="str">
-        <f>Tabelle1!AR22</f>
+      <c r="EC22" t="str">
+        <f>Tabelle1!AS22</f>
         <v>FlightDesignCT</v>
       </c>
     </row>
-    <row r="23" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:133" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>88</v>
       </c>
@@ -16805,7 +17015,7 @@
         <v>0</v>
       </c>
       <c r="DB23" s="12">
-        <f>Tabelle1!AQ23</f>
+        <f>Tabelle1!AR23</f>
         <v>0</v>
       </c>
       <c r="DC23" s="12" t="s">
@@ -16883,15 +17093,19 @@
       <c r="DZ23" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EA23" s="12" t="s">
+      <c r="EA23" s="12">
+        <f>Tabelle1!AQ23</f>
+        <v>0</v>
+      </c>
+      <c r="EB23" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EB23" t="str">
-        <f>Tabelle1!AR23</f>
+      <c r="EC23" t="str">
+        <f>Tabelle1!AS23</f>
         <v>Icon A5</v>
       </c>
     </row>
-    <row r="24" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:133" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>88</v>
       </c>
@@ -17238,7 +17452,7 @@
         <v>0</v>
       </c>
       <c r="DB24" s="12">
-        <f>Tabelle1!AQ24</f>
+        <f>Tabelle1!AR24</f>
         <v>0</v>
       </c>
       <c r="DC24" s="12" t="s">
@@ -17316,15 +17530,19 @@
       <c r="DZ24" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EA24" s="12" t="s">
+      <c r="EA24" s="12">
+        <f>Tabelle1!AQ24</f>
+        <v>0</v>
+      </c>
+      <c r="EB24" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EB24" t="str">
-        <f>Tabelle1!AR24</f>
+      <c r="EC24" t="str">
+        <f>Tabelle1!AS24</f>
         <v>Mudry Cap 10 C</v>
       </c>
     </row>
-    <row r="25" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:133" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>88</v>
       </c>
@@ -17671,7 +17889,7 @@
         <v>0</v>
       </c>
       <c r="DB25" s="12">
-        <f>Tabelle1!AQ25</f>
+        <f>Tabelle1!AR25</f>
         <v>0</v>
       </c>
       <c r="DC25" s="12" t="s">
@@ -17749,15 +17967,19 @@
       <c r="DZ25" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EA25" s="12" t="s">
+      <c r="EA25" s="12">
+        <f>Tabelle1!AQ25</f>
+        <v>0</v>
+      </c>
+      <c r="EB25" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EB25" t="str">
-        <f>Tabelle1!AR25</f>
+      <c r="EC25" t="str">
+        <f>Tabelle1!AS25</f>
         <v>Pilatus PC-6 Gauge</v>
       </c>
     </row>
-    <row r="26" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:133" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>88</v>
       </c>
@@ -18104,7 +18326,7 @@
         <v>0</v>
       </c>
       <c r="DB26" s="12">
-        <f>Tabelle1!AQ26</f>
+        <f>Tabelle1!AR26</f>
         <v>0</v>
       </c>
       <c r="DC26" s="12" t="s">
@@ -18182,15 +18404,19 @@
       <c r="DZ26" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EA26" s="12" t="s">
+      <c r="EA26" s="12">
+        <f>Tabelle1!AQ26</f>
+        <v>0</v>
+      </c>
+      <c r="EB26" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EB26" t="str">
-        <f>Tabelle1!AR26</f>
+      <c r="EC26" t="str">
+        <f>Tabelle1!AS26</f>
         <v>Pilatus PC-6 G950</v>
       </c>
     </row>
-    <row r="27" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:133" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>88</v>
       </c>
@@ -18537,7 +18763,7 @@
         <v>0</v>
       </c>
       <c r="DB27" s="12">
-        <f>Tabelle1!AQ27</f>
+        <f>Tabelle1!AR27</f>
         <v>0</v>
       </c>
       <c r="DC27" s="12" t="s">
@@ -18615,15 +18841,19 @@
       <c r="DZ27" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EA27" s="12" t="s">
+      <c r="EA27" s="12">
+        <f>Tabelle1!AQ27</f>
+        <v>0</v>
+      </c>
+      <c r="EB27" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EB27" t="str">
-        <f>Tabelle1!AR27</f>
+      <c r="EC27" t="str">
+        <f>Tabelle1!AS27</f>
         <v>Pipistrel Alpha Electro</v>
       </c>
     </row>
-    <row r="28" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:133" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>88</v>
       </c>
@@ -18970,7 +19200,7 @@
         <v>0</v>
       </c>
       <c r="DB28" s="12">
-        <f>Tabelle1!AQ28</f>
+        <f>Tabelle1!AR28</f>
         <v>0</v>
       </c>
       <c r="DC28" s="12" t="s">
@@ -19048,15 +19278,19 @@
       <c r="DZ28" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EA28" s="12" t="s">
+      <c r="EA28" s="12">
+        <f>Tabelle1!AQ28</f>
+        <v>0</v>
+      </c>
+      <c r="EB28" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EB28" t="str">
-        <f>Tabelle1!AR28</f>
+      <c r="EC28" t="str">
+        <f>Tabelle1!AS28</f>
         <v>Pitts Special 1S</v>
       </c>
     </row>
-    <row r="29" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:133" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>88</v>
       </c>
@@ -19403,7 +19637,7 @@
         <v>0</v>
       </c>
       <c r="DB29" s="12">
-        <f>Tabelle1!AQ29</f>
+        <f>Tabelle1!AR29</f>
         <v>0</v>
       </c>
       <c r="DC29" s="12" t="s">
@@ -19481,15 +19715,19 @@
       <c r="DZ29" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EA29" s="12" t="s">
+      <c r="EA29" s="12">
+        <f>Tabelle1!AQ29</f>
+        <v>0</v>
+      </c>
+      <c r="EB29" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EB29" t="str">
-        <f>Tabelle1!AR29</f>
+      <c r="EC29" t="str">
+        <f>Tabelle1!AS29</f>
         <v>Pitts Special S2S</v>
       </c>
     </row>
-    <row r="30" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:133" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>88</v>
       </c>
@@ -19836,7 +20074,7 @@
         <v>0</v>
       </c>
       <c r="DB30" s="12">
-        <f>Tabelle1!AQ30</f>
+        <f>Tabelle1!AR30</f>
         <v>0</v>
       </c>
       <c r="DC30" s="12" t="s">
@@ -19914,15 +20152,19 @@
       <c r="DZ30" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EA30" s="12" t="s">
+      <c r="EA30" s="12">
+        <f>Tabelle1!AQ30</f>
+        <v>0</v>
+      </c>
+      <c r="EB30" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EB30" t="str">
-        <f>Tabelle1!AR30</f>
+      <c r="EC30" t="str">
+        <f>Tabelle1!AS30</f>
         <v>Savage Cub</v>
       </c>
     </row>
-    <row r="31" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:133" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>88</v>
       </c>
@@ -20269,7 +20511,7 @@
         <v>0</v>
       </c>
       <c r="DB31" s="12">
-        <f>Tabelle1!AQ31</f>
+        <f>Tabelle1!AR31</f>
         <v>0</v>
       </c>
       <c r="DC31" s="12" t="s">
@@ -20347,15 +20589,19 @@
       <c r="DZ31" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EA31" s="12" t="s">
+      <c r="EA31" s="12">
+        <f>Tabelle1!AQ31</f>
+        <v>0</v>
+      </c>
+      <c r="EB31" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EB31" t="str">
-        <f>Tabelle1!AR31</f>
+      <c r="EC31" t="str">
+        <f>Tabelle1!AS31</f>
         <v>Savage Shock Ultra</v>
       </c>
     </row>
-    <row r="32" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:133" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>88</v>
       </c>
@@ -20702,7 +20948,7 @@
         <v>0</v>
       </c>
       <c r="DB32" s="12">
-        <f>Tabelle1!AQ32</f>
+        <f>Tabelle1!AR32</f>
         <v>0</v>
       </c>
       <c r="DC32" s="12" t="s">
@@ -20780,15 +21026,19 @@
       <c r="DZ32" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EA32" s="12" t="s">
+      <c r="EA32" s="12">
+        <f>Tabelle1!AQ32</f>
+        <v>0</v>
+      </c>
+      <c r="EB32" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EB32" t="str">
-        <f>Tabelle1!AR32</f>
+      <c r="EC32" t="str">
+        <f>Tabelle1!AS32</f>
         <v>SR22</v>
       </c>
     </row>
-    <row r="33" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:133" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>88</v>
       </c>
@@ -21135,7 +21385,7 @@
         <v>0</v>
       </c>
       <c r="DB33" s="12">
-        <f>Tabelle1!AQ33</f>
+        <f>Tabelle1!AR33</f>
         <v>0</v>
       </c>
       <c r="DC33" s="12" t="s">
@@ -21213,15 +21463,19 @@
       <c r="DZ33" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EA33" s="12" t="s">
+      <c r="EA33" s="12">
+        <f>Tabelle1!AQ33</f>
+        <v>0</v>
+      </c>
+      <c r="EB33" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EB33" t="str">
-        <f>Tabelle1!AR33</f>
+      <c r="EC33" t="str">
+        <f>Tabelle1!AS33</f>
         <v>TBM 930</v>
       </c>
     </row>
-    <row r="34" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:133" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>88</v>
       </c>
@@ -21568,7 +21822,7 @@
         <v>0</v>
       </c>
       <c r="DB34" s="12">
-        <f>Tabelle1!AQ34</f>
+        <f>Tabelle1!AR34</f>
         <v>0</v>
       </c>
       <c r="DC34" s="12" t="s">
@@ -21646,15 +21900,19 @@
       <c r="DZ34" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EA34" s="12" t="s">
+      <c r="EA34" s="12">
+        <f>Tabelle1!AQ34</f>
+        <v>0</v>
+      </c>
+      <c r="EB34" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EB34" t="str">
-        <f>Tabelle1!AR34</f>
+      <c r="EC34" t="str">
+        <f>Tabelle1!AS34</f>
         <v>Vertigo</v>
       </c>
     </row>
-    <row r="35" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:133" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
         <v>88</v>
       </c>
@@ -22001,7 +22259,7 @@
         <v>0</v>
       </c>
       <c r="DB35" s="12">
-        <f>Tabelle1!AQ35</f>
+        <f>Tabelle1!AR35</f>
         <v>0</v>
       </c>
       <c r="DC35" s="12" t="s">
@@ -22079,15 +22337,19 @@
       <c r="DZ35" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EA35" s="12" t="s">
+      <c r="EA35" s="12">
+        <f>Tabelle1!AQ35</f>
+        <v>0</v>
+      </c>
+      <c r="EB35" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EB35" t="str">
-        <f>Tabelle1!AR35</f>
+      <c r="EC35" t="str">
+        <f>Tabelle1!AS35</f>
         <v>VL3</v>
       </c>
     </row>
-    <row r="36" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:133" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>88</v>
       </c>
@@ -22434,7 +22696,7 @@
         <v>0</v>
       </c>
       <c r="DB36" s="12">
-        <f>Tabelle1!AQ36</f>
+        <f>Tabelle1!AR36</f>
         <v>0</v>
       </c>
       <c r="DC36" s="12" t="s">
@@ -22512,15 +22774,19 @@
       <c r="DZ36" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EA36" s="12" t="s">
+      <c r="EA36" s="12">
+        <f>Tabelle1!AQ36</f>
+        <v>0</v>
+      </c>
+      <c r="EB36" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EB36" t="str">
-        <f>Tabelle1!AR36</f>
+      <c r="EC36" t="str">
+        <f>Tabelle1!AS36</f>
         <v>Volocity</v>
       </c>
     </row>
-    <row r="37" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:133" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
         <v>88</v>
       </c>
@@ -22867,7 +23133,7 @@
         <v>0</v>
       </c>
       <c r="DB37" s="12">
-        <f>Tabelle1!AQ37</f>
+        <f>Tabelle1!AR37</f>
         <v>0</v>
       </c>
       <c r="DC37" s="12" t="s">
@@ -22945,15 +23211,19 @@
       <c r="DZ37" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EA37" s="12" t="s">
+      <c r="EA37" s="12">
+        <f>Tabelle1!AQ37</f>
+        <v>0</v>
+      </c>
+      <c r="EB37" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EB37" t="str">
-        <f>Tabelle1!AR37</f>
+      <c r="EC37" t="str">
+        <f>Tabelle1!AS37</f>
         <v>NXCub</v>
       </c>
     </row>
-    <row r="38" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:133" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>88</v>
       </c>
@@ -23300,7 +23570,7 @@
         <v>0</v>
       </c>
       <c r="DB38" s="12">
-        <f>Tabelle1!AQ38</f>
+        <f>Tabelle1!AR38</f>
         <v>0</v>
       </c>
       <c r="DC38" s="12" t="s">
@@ -23378,15 +23648,19 @@
       <c r="DZ38" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EA38" s="12" t="s">
+      <c r="EA38" s="12">
+        <f>Tabelle1!AQ38</f>
+        <v>0</v>
+      </c>
+      <c r="EB38" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EB38" t="str">
-        <f>Tabelle1!AR38</f>
+      <c r="EC38" t="str">
+        <f>Tabelle1!AS38</f>
         <v>XCub</v>
       </c>
     </row>
-    <row r="39" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:133" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>88</v>
       </c>
@@ -23733,7 +24007,7 @@
         <v>0</v>
       </c>
       <c r="DB39" s="12">
-        <f>Tabelle1!AQ39</f>
+        <f>Tabelle1!AR39</f>
         <v>0</v>
       </c>
       <c r="DC39" s="12" t="s">
@@ -23811,15 +24085,19 @@
       <c r="DZ39" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EA39" s="12" t="s">
+      <c r="EA39" s="12">
+        <f>Tabelle1!AQ39</f>
+        <v>0</v>
+      </c>
+      <c r="EB39" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EB39" t="str">
-        <f>Tabelle1!AR39</f>
+      <c r="EC39" t="str">
+        <f>Tabelle1!AS39</f>
         <v>SWS Kodiak 100 II</v>
       </c>
     </row>
-    <row r="40" spans="1:132" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:133" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
         <v>88</v>
       </c>
@@ -24166,7 +24444,7 @@
         <v>0</v>
       </c>
       <c r="DB40" s="12">
-        <f>Tabelle1!AQ40</f>
+        <f>Tabelle1!AR40</f>
         <v>1</v>
       </c>
       <c r="DC40" s="12" t="s">
@@ -24244,11 +24522,15 @@
       <c r="DZ40" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EA40" s="12" t="s">
+      <c r="EA40" s="12">
+        <f>Tabelle1!AQ40</f>
+        <v>0</v>
+      </c>
+      <c r="EB40" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EB40" t="str">
-        <f>Tabelle1!AR40</f>
+      <c r="EC40" t="str">
+        <f>Tabelle1!AS40</f>
         <v>Generic Glider</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V 0.50-B47 - SU9 checking - Add Control Surfaces Item as Graphics - SU9 Compatibility Check - Update QuickGuide
</commit_message>
<xml_diff>
--- a/Config/EngineMerge.xlsx
+++ b/Config/EngineMerge.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4118" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4158" uniqueCount="289">
   <si>
     <t>ACFT</t>
   </si>
@@ -882,6 +882,9 @@
   </si>
   <si>
     <t>A320THR</t>
+  </si>
+  <si>
+    <t>SURF_ANI</t>
   </si>
 </sst>
 </file>
@@ -7075,10 +7078,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:EC40"/>
+  <dimension ref="A1:ED40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CQ1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="ED35" sqref="ED35"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="EH6" sqref="EH6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7086,11 +7089,11 @@
     <col min="1" max="75" width="3.7109375" bestFit="1" customWidth="1"/>
     <col min="76" max="77" width="3.7109375" customWidth="1"/>
     <col min="78" max="86" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="87" max="132" width="3.7109375" customWidth="1"/>
-    <col min="133" max="133" width="36.28515625" customWidth="1"/>
+    <col min="87" max="133" width="3.7109375" customWidth="1"/>
+    <col min="134" max="134" width="36.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:133" s="11" customFormat="1" ht="72" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:134" s="11" customFormat="1" ht="72" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>95</v>
       </c>
@@ -7485,13 +7488,16 @@
         <v>287</v>
       </c>
       <c r="EB1" s="11" t="s">
+        <v>288</v>
+      </c>
+      <c r="EC1" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="EC1" t="s">
+      <c r="ED1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:133" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>88</v>
       </c>
@@ -7921,14 +7927,17 @@
         <v>1</v>
       </c>
       <c r="EB2" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EC2" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EC2" t="str">
+      <c r="ED2" t="str">
         <f>Tabelle1!AS2</f>
         <v>Airbus A320 Neo</v>
       </c>
     </row>
-    <row r="3" spans="1:133" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>88</v>
       </c>
@@ -8358,14 +8367,17 @@
         <v>0</v>
       </c>
       <c r="EB3" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EC3" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EC3" t="str">
+      <c r="ED3" t="str">
         <f>Tabelle1!AS3</f>
         <v>Boeing 747-8i</v>
       </c>
     </row>
-    <row r="4" spans="1:133" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>88</v>
       </c>
@@ -8795,14 +8807,17 @@
         <v>0</v>
       </c>
       <c r="EB4" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EC4" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EC4" t="str">
+      <c r="ED4" t="str">
         <f>Tabelle1!AS4</f>
         <v>Boeing 787-10</v>
       </c>
     </row>
-    <row r="5" spans="1:133" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>88</v>
       </c>
@@ -9232,14 +9247,17 @@
         <v>0</v>
       </c>
       <c r="EB5" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EC5" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EC5" t="str">
+      <c r="ED5" t="str">
         <f>Tabelle1!AS5</f>
         <v>Boeing F/A 18E Super Hornet</v>
       </c>
     </row>
-    <row r="6" spans="1:133" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>88</v>
       </c>
@@ -9669,14 +9687,17 @@
         <v>0</v>
       </c>
       <c r="EB6" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EC6" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EC6" t="str">
+      <c r="ED6" t="str">
         <f>Tabelle1!AS6</f>
         <v>Baron G58</v>
       </c>
     </row>
-    <row r="7" spans="1:133" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>88</v>
       </c>
@@ -10106,14 +10127,17 @@
         <v>0</v>
       </c>
       <c r="EB7" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EC7" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EC7" t="str">
+      <c r="ED7" t="str">
         <f>Tabelle1!AS7</f>
         <v>Bonanza G36</v>
       </c>
     </row>
-    <row r="8" spans="1:133" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>88</v>
       </c>
@@ -10543,14 +10567,17 @@
         <v>0</v>
       </c>
       <c r="EB8" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EC8" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EC8" t="str">
+      <c r="ED8" t="str">
         <f>Tabelle1!AS8</f>
         <v>Beechcraft King Air 350i</v>
       </c>
     </row>
-    <row r="9" spans="1:133" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>88</v>
       </c>
@@ -10980,14 +11007,17 @@
         <v>0</v>
       </c>
       <c r="EB9" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EC9" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EC9" t="str">
+      <c r="ED9" t="str">
         <f>Tabelle1!AS9</f>
         <v>Cessna 152</v>
       </c>
     </row>
-    <row r="10" spans="1:133" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>88</v>
       </c>
@@ -11417,14 +11447,17 @@
         <v>0</v>
       </c>
       <c r="EB10" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EC10" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EC10" t="str">
+      <c r="ED10" t="str">
         <f>Tabelle1!AS10</f>
         <v>Cessna 152 Aero</v>
       </c>
     </row>
-    <row r="11" spans="1:133" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>88</v>
       </c>
@@ -11854,14 +11887,17 @@
         <v>0</v>
       </c>
       <c r="EB11" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EC11" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EC11" t="str">
+      <c r="ED11" t="str">
         <f>Tabelle1!AS11</f>
         <v>Cessna 172sp Skyhawk G1000</v>
       </c>
     </row>
-    <row r="12" spans="1:133" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>88</v>
       </c>
@@ -12291,14 +12327,17 @@
         <v>0</v>
       </c>
       <c r="EB12" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EC12" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EC12" t="str">
+      <c r="ED12" t="str">
         <f>Tabelle1!AS12</f>
         <v>Cessna 172sp Skyhawk</v>
       </c>
     </row>
-    <row r="13" spans="1:133" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>88</v>
       </c>
@@ -12728,14 +12767,17 @@
         <v>0</v>
       </c>
       <c r="EB13" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EC13" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EC13" t="str">
+      <c r="ED13" t="str">
         <f>Tabelle1!AS13</f>
         <v>Cessna 208B Grand Caravan EX</v>
       </c>
     </row>
-    <row r="14" spans="1:133" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>88</v>
       </c>
@@ -13165,14 +13207,17 @@
         <v>0</v>
       </c>
       <c r="EB14" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EC14" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EC14" t="str">
+      <c r="ED14" t="str">
         <f>Tabelle1!AS14</f>
         <v>Cessna CJ4 Citation</v>
       </c>
     </row>
-    <row r="15" spans="1:133" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>88</v>
       </c>
@@ -13602,14 +13647,17 @@
         <v>0</v>
       </c>
       <c r="EB15" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EC15" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EC15" t="str">
+      <c r="ED15" t="str">
         <f>Tabelle1!AS15</f>
         <v>Cessna Longitude</v>
       </c>
     </row>
-    <row r="16" spans="1:133" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>88</v>
       </c>
@@ -14039,14 +14087,17 @@
         <v>0</v>
       </c>
       <c r="EB16" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EC16" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EC16" t="str">
+      <c r="ED16" t="str">
         <f>Tabelle1!AS16</f>
         <v>DA40-NG</v>
       </c>
     </row>
-    <row r="17" spans="1:133" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>88</v>
       </c>
@@ -14476,14 +14527,17 @@
         <v>0</v>
       </c>
       <c r="EB17" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EC17" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EC17" t="str">
+      <c r="ED17" t="str">
         <f>Tabelle1!AS17</f>
         <v>DA40 TDI</v>
       </c>
     </row>
-    <row r="18" spans="1:133" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>88</v>
       </c>
@@ -14913,14 +14967,17 @@
         <v>0</v>
       </c>
       <c r="EB18" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EC18" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EC18" t="str">
+      <c r="ED18" t="str">
         <f>Tabelle1!AS18</f>
         <v>DA62</v>
       </c>
     </row>
-    <row r="19" spans="1:133" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>88</v>
       </c>
@@ -15350,14 +15407,17 @@
         <v>0</v>
       </c>
       <c r="EB19" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EC19" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EC19" t="str">
+      <c r="ED19" t="str">
         <f>Tabelle1!AS19</f>
         <v>DR400</v>
       </c>
     </row>
-    <row r="20" spans="1:133" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>88</v>
       </c>
@@ -15787,14 +15847,17 @@
         <v>0</v>
       </c>
       <c r="EB20" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EC20" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EC20" t="str">
+      <c r="ED20" t="str">
         <f>Tabelle1!AS20</f>
         <v>DV20</v>
       </c>
     </row>
-    <row r="21" spans="1:133" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>88</v>
       </c>
@@ -16224,14 +16287,17 @@
         <v>0</v>
       </c>
       <c r="EB21" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EC21" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EC21" t="str">
+      <c r="ED21" t="str">
         <f>Tabelle1!AS21</f>
         <v>Extra 330</v>
       </c>
     </row>
-    <row r="22" spans="1:133" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>88</v>
       </c>
@@ -16661,14 +16727,17 @@
         <v>0</v>
       </c>
       <c r="EB22" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EC22" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EC22" t="str">
+      <c r="ED22" t="str">
         <f>Tabelle1!AS22</f>
         <v>FlightDesignCT</v>
       </c>
     </row>
-    <row r="23" spans="1:133" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>88</v>
       </c>
@@ -17098,14 +17167,17 @@
         <v>0</v>
       </c>
       <c r="EB23" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EC23" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EC23" t="str">
+      <c r="ED23" t="str">
         <f>Tabelle1!AS23</f>
         <v>Icon A5</v>
       </c>
     </row>
-    <row r="24" spans="1:133" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>88</v>
       </c>
@@ -17535,14 +17607,17 @@
         <v>0</v>
       </c>
       <c r="EB24" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EC24" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EC24" t="str">
+      <c r="ED24" t="str">
         <f>Tabelle1!AS24</f>
         <v>Mudry Cap 10 C</v>
       </c>
     </row>
-    <row r="25" spans="1:133" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>88</v>
       </c>
@@ -17972,14 +18047,17 @@
         <v>0</v>
       </c>
       <c r="EB25" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EC25" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EC25" t="str">
+      <c r="ED25" t="str">
         <f>Tabelle1!AS25</f>
         <v>Pilatus PC-6 Gauge</v>
       </c>
     </row>
-    <row r="26" spans="1:133" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>88</v>
       </c>
@@ -18409,14 +18487,17 @@
         <v>0</v>
       </c>
       <c r="EB26" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EC26" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EC26" t="str">
+      <c r="ED26" t="str">
         <f>Tabelle1!AS26</f>
         <v>Pilatus PC-6 G950</v>
       </c>
     </row>
-    <row r="27" spans="1:133" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>88</v>
       </c>
@@ -18846,14 +18927,17 @@
         <v>0</v>
       </c>
       <c r="EB27" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EC27" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EC27" t="str">
+      <c r="ED27" t="str">
         <f>Tabelle1!AS27</f>
         <v>Pipistrel Alpha Electro</v>
       </c>
     </row>
-    <row r="28" spans="1:133" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>88</v>
       </c>
@@ -19283,14 +19367,17 @@
         <v>0</v>
       </c>
       <c r="EB28" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EC28" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EC28" t="str">
+      <c r="ED28" t="str">
         <f>Tabelle1!AS28</f>
         <v>Pitts Special 1S</v>
       </c>
     </row>
-    <row r="29" spans="1:133" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>88</v>
       </c>
@@ -19720,14 +19807,17 @@
         <v>0</v>
       </c>
       <c r="EB29" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EC29" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EC29" t="str">
+      <c r="ED29" t="str">
         <f>Tabelle1!AS29</f>
         <v>Pitts Special S2S</v>
       </c>
     </row>
-    <row r="30" spans="1:133" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>88</v>
       </c>
@@ -20157,14 +20247,17 @@
         <v>0</v>
       </c>
       <c r="EB30" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EC30" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EC30" t="str">
+      <c r="ED30" t="str">
         <f>Tabelle1!AS30</f>
         <v>Savage Cub</v>
       </c>
     </row>
-    <row r="31" spans="1:133" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>88</v>
       </c>
@@ -20594,14 +20687,17 @@
         <v>0</v>
       </c>
       <c r="EB31" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EC31" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EC31" t="str">
+      <c r="ED31" t="str">
         <f>Tabelle1!AS31</f>
         <v>Savage Shock Ultra</v>
       </c>
     </row>
-    <row r="32" spans="1:133" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>88</v>
       </c>
@@ -21031,14 +21127,17 @@
         <v>0</v>
       </c>
       <c r="EB32" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EC32" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EC32" t="str">
+      <c r="ED32" t="str">
         <f>Tabelle1!AS32</f>
         <v>SR22</v>
       </c>
     </row>
-    <row r="33" spans="1:133" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>88</v>
       </c>
@@ -21468,14 +21567,17 @@
         <v>0</v>
       </c>
       <c r="EB33" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EC33" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EC33" t="str">
+      <c r="ED33" t="str">
         <f>Tabelle1!AS33</f>
         <v>TBM 930</v>
       </c>
     </row>
-    <row r="34" spans="1:133" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>88</v>
       </c>
@@ -21905,14 +22007,17 @@
         <v>0</v>
       </c>
       <c r="EB34" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EC34" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EC34" t="str">
+      <c r="ED34" t="str">
         <f>Tabelle1!AS34</f>
         <v>Vertigo</v>
       </c>
     </row>
-    <row r="35" spans="1:133" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
         <v>88</v>
       </c>
@@ -22342,14 +22447,17 @@
         <v>0</v>
       </c>
       <c r="EB35" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EC35" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EC35" t="str">
+      <c r="ED35" t="str">
         <f>Tabelle1!AS35</f>
         <v>VL3</v>
       </c>
     </row>
-    <row r="36" spans="1:133" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>88</v>
       </c>
@@ -22779,14 +22887,17 @@
         <v>0</v>
       </c>
       <c r="EB36" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EC36" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EC36" t="str">
+      <c r="ED36" t="str">
         <f>Tabelle1!AS36</f>
         <v>Volocity</v>
       </c>
     </row>
-    <row r="37" spans="1:133" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
         <v>88</v>
       </c>
@@ -23216,14 +23327,17 @@
         <v>0</v>
       </c>
       <c r="EB37" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EC37" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EC37" t="str">
+      <c r="ED37" t="str">
         <f>Tabelle1!AS37</f>
         <v>NXCub</v>
       </c>
     </row>
-    <row r="38" spans="1:133" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>88</v>
       </c>
@@ -23653,14 +23767,17 @@
         <v>0</v>
       </c>
       <c r="EB38" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EC38" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EC38" t="str">
+      <c r="ED38" t="str">
         <f>Tabelle1!AS38</f>
         <v>XCub</v>
       </c>
     </row>
-    <row r="39" spans="1:133" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>88</v>
       </c>
@@ -24090,14 +24207,17 @@
         <v>0</v>
       </c>
       <c r="EB39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EC39" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EC39" t="str">
+      <c r="ED39" t="str">
         <f>Tabelle1!AS39</f>
         <v>SWS Kodiak 100 II</v>
       </c>
     </row>
-    <row r="40" spans="1:133" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
         <v>88</v>
       </c>
@@ -24527,9 +24647,12 @@
         <v>0</v>
       </c>
       <c r="EB40" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EC40" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EC40" t="str">
+      <c r="ED40" t="str">
         <f>Tabelle1!AS40</f>
         <v>Generic Glider</v>
       </c>

</xml_diff>

<commit_message>
V 0.51-B48 Doc update
</commit_message>
<xml_diff>
--- a/Config/EngineMerge.xlsx
+++ b/Config/EngineMerge.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4158" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4198" uniqueCount="290">
   <si>
     <t>ACFT</t>
   </si>
@@ -885,6 +885,9 @@
   </si>
   <si>
     <t>SURF_ANI</t>
+  </si>
+  <si>
+    <t>DEPARR</t>
   </si>
 </sst>
 </file>
@@ -7078,10 +7081,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:ED40"/>
+  <dimension ref="A1:EE40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="EH6" sqref="EH6"/>
+      <selection activeCell="CZ14" sqref="CZ14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7089,11 +7092,11 @@
     <col min="1" max="75" width="3.7109375" bestFit="1" customWidth="1"/>
     <col min="76" max="77" width="3.7109375" customWidth="1"/>
     <col min="78" max="86" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="87" max="133" width="3.7109375" customWidth="1"/>
-    <col min="134" max="134" width="36.28515625" customWidth="1"/>
+    <col min="87" max="134" width="3.7109375" customWidth="1"/>
+    <col min="135" max="135" width="36.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:134" s="11" customFormat="1" ht="72" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:135" s="11" customFormat="1" ht="72" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>95</v>
       </c>
@@ -7491,13 +7494,16 @@
         <v>288</v>
       </c>
       <c r="EC1" s="11" t="s">
+        <v>289</v>
+      </c>
+      <c r="ED1" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="ED1" t="s">
+      <c r="EE1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:135" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>88</v>
       </c>
@@ -7930,14 +7936,17 @@
         <v>88</v>
       </c>
       <c r="EC2" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ED2" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ED2" t="str">
+      <c r="EE2" t="str">
         <f>Tabelle1!AS2</f>
         <v>Airbus A320 Neo</v>
       </c>
     </row>
-    <row r="3" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:135" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>88</v>
       </c>
@@ -8370,14 +8379,17 @@
         <v>88</v>
       </c>
       <c r="EC3" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ED3" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ED3" t="str">
+      <c r="EE3" t="str">
         <f>Tabelle1!AS3</f>
         <v>Boeing 747-8i</v>
       </c>
     </row>
-    <row r="4" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:135" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>88</v>
       </c>
@@ -8810,14 +8822,17 @@
         <v>88</v>
       </c>
       <c r="EC4" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ED4" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ED4" t="str">
+      <c r="EE4" t="str">
         <f>Tabelle1!AS4</f>
         <v>Boeing 787-10</v>
       </c>
     </row>
-    <row r="5" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:135" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>88</v>
       </c>
@@ -9250,14 +9265,17 @@
         <v>88</v>
       </c>
       <c r="EC5" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ED5" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ED5" t="str">
+      <c r="EE5" t="str">
         <f>Tabelle1!AS5</f>
         <v>Boeing F/A 18E Super Hornet</v>
       </c>
     </row>
-    <row r="6" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:135" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>88</v>
       </c>
@@ -9690,14 +9708,17 @@
         <v>88</v>
       </c>
       <c r="EC6" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ED6" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ED6" t="str">
+      <c r="EE6" t="str">
         <f>Tabelle1!AS6</f>
         <v>Baron G58</v>
       </c>
     </row>
-    <row r="7" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:135" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>88</v>
       </c>
@@ -10130,14 +10151,17 @@
         <v>88</v>
       </c>
       <c r="EC7" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ED7" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ED7" t="str">
+      <c r="EE7" t="str">
         <f>Tabelle1!AS7</f>
         <v>Bonanza G36</v>
       </c>
     </row>
-    <row r="8" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:135" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>88</v>
       </c>
@@ -10570,14 +10594,17 @@
         <v>88</v>
       </c>
       <c r="EC8" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ED8" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ED8" t="str">
+      <c r="EE8" t="str">
         <f>Tabelle1!AS8</f>
         <v>Beechcraft King Air 350i</v>
       </c>
     </row>
-    <row r="9" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:135" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>88</v>
       </c>
@@ -11010,14 +11037,17 @@
         <v>88</v>
       </c>
       <c r="EC9" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ED9" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ED9" t="str">
+      <c r="EE9" t="str">
         <f>Tabelle1!AS9</f>
         <v>Cessna 152</v>
       </c>
     </row>
-    <row r="10" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:135" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>88</v>
       </c>
@@ -11450,14 +11480,17 @@
         <v>88</v>
       </c>
       <c r="EC10" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ED10" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ED10" t="str">
+      <c r="EE10" t="str">
         <f>Tabelle1!AS10</f>
         <v>Cessna 152 Aero</v>
       </c>
     </row>
-    <row r="11" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:135" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>88</v>
       </c>
@@ -11890,14 +11923,17 @@
         <v>88</v>
       </c>
       <c r="EC11" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ED11" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ED11" t="str">
+      <c r="EE11" t="str">
         <f>Tabelle1!AS11</f>
         <v>Cessna 172sp Skyhawk G1000</v>
       </c>
     </row>
-    <row r="12" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:135" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>88</v>
       </c>
@@ -12330,14 +12366,17 @@
         <v>88</v>
       </c>
       <c r="EC12" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ED12" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ED12" t="str">
+      <c r="EE12" t="str">
         <f>Tabelle1!AS12</f>
         <v>Cessna 172sp Skyhawk</v>
       </c>
     </row>
-    <row r="13" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:135" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>88</v>
       </c>
@@ -12770,14 +12809,17 @@
         <v>88</v>
       </c>
       <c r="EC13" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ED13" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ED13" t="str">
+      <c r="EE13" t="str">
         <f>Tabelle1!AS13</f>
         <v>Cessna 208B Grand Caravan EX</v>
       </c>
     </row>
-    <row r="14" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:135" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>88</v>
       </c>
@@ -13210,14 +13252,17 @@
         <v>88</v>
       </c>
       <c r="EC14" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ED14" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ED14" t="str">
+      <c r="EE14" t="str">
         <f>Tabelle1!AS14</f>
         <v>Cessna CJ4 Citation</v>
       </c>
     </row>
-    <row r="15" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:135" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>88</v>
       </c>
@@ -13650,14 +13695,17 @@
         <v>88</v>
       </c>
       <c r="EC15" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ED15" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ED15" t="str">
+      <c r="EE15" t="str">
         <f>Tabelle1!AS15</f>
         <v>Cessna Longitude</v>
       </c>
     </row>
-    <row r="16" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:135" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>88</v>
       </c>
@@ -14090,14 +14138,17 @@
         <v>88</v>
       </c>
       <c r="EC16" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ED16" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ED16" t="str">
+      <c r="EE16" t="str">
         <f>Tabelle1!AS16</f>
         <v>DA40-NG</v>
       </c>
     </row>
-    <row r="17" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:135" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>88</v>
       </c>
@@ -14530,14 +14581,17 @@
         <v>88</v>
       </c>
       <c r="EC17" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ED17" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ED17" t="str">
+      <c r="EE17" t="str">
         <f>Tabelle1!AS17</f>
         <v>DA40 TDI</v>
       </c>
     </row>
-    <row r="18" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:135" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>88</v>
       </c>
@@ -14970,14 +15024,17 @@
         <v>88</v>
       </c>
       <c r="EC18" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ED18" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ED18" t="str">
+      <c r="EE18" t="str">
         <f>Tabelle1!AS18</f>
         <v>DA62</v>
       </c>
     </row>
-    <row r="19" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:135" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>88</v>
       </c>
@@ -15410,14 +15467,17 @@
         <v>88</v>
       </c>
       <c r="EC19" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ED19" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ED19" t="str">
+      <c r="EE19" t="str">
         <f>Tabelle1!AS19</f>
         <v>DR400</v>
       </c>
     </row>
-    <row r="20" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:135" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>88</v>
       </c>
@@ -15850,14 +15910,17 @@
         <v>88</v>
       </c>
       <c r="EC20" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ED20" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ED20" t="str">
+      <c r="EE20" t="str">
         <f>Tabelle1!AS20</f>
         <v>DV20</v>
       </c>
     </row>
-    <row r="21" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:135" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>88</v>
       </c>
@@ -16290,14 +16353,17 @@
         <v>88</v>
       </c>
       <c r="EC21" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ED21" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ED21" t="str">
+      <c r="EE21" t="str">
         <f>Tabelle1!AS21</f>
         <v>Extra 330</v>
       </c>
     </row>
-    <row r="22" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:135" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>88</v>
       </c>
@@ -16730,14 +16796,17 @@
         <v>88</v>
       </c>
       <c r="EC22" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ED22" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ED22" t="str">
+      <c r="EE22" t="str">
         <f>Tabelle1!AS22</f>
         <v>FlightDesignCT</v>
       </c>
     </row>
-    <row r="23" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:135" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>88</v>
       </c>
@@ -17170,14 +17239,17 @@
         <v>88</v>
       </c>
       <c r="EC23" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ED23" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ED23" t="str">
+      <c r="EE23" t="str">
         <f>Tabelle1!AS23</f>
         <v>Icon A5</v>
       </c>
     </row>
-    <row r="24" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:135" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>88</v>
       </c>
@@ -17610,14 +17682,17 @@
         <v>88</v>
       </c>
       <c r="EC24" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ED24" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ED24" t="str">
+      <c r="EE24" t="str">
         <f>Tabelle1!AS24</f>
         <v>Mudry Cap 10 C</v>
       </c>
     </row>
-    <row r="25" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:135" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>88</v>
       </c>
@@ -18050,14 +18125,17 @@
         <v>88</v>
       </c>
       <c r="EC25" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ED25" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ED25" t="str">
+      <c r="EE25" t="str">
         <f>Tabelle1!AS25</f>
         <v>Pilatus PC-6 Gauge</v>
       </c>
     </row>
-    <row r="26" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:135" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>88</v>
       </c>
@@ -18490,14 +18568,17 @@
         <v>88</v>
       </c>
       <c r="EC26" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ED26" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ED26" t="str">
+      <c r="EE26" t="str">
         <f>Tabelle1!AS26</f>
         <v>Pilatus PC-6 G950</v>
       </c>
     </row>
-    <row r="27" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:135" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>88</v>
       </c>
@@ -18930,14 +19011,17 @@
         <v>88</v>
       </c>
       <c r="EC27" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ED27" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ED27" t="str">
+      <c r="EE27" t="str">
         <f>Tabelle1!AS27</f>
         <v>Pipistrel Alpha Electro</v>
       </c>
     </row>
-    <row r="28" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:135" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>88</v>
       </c>
@@ -19370,14 +19454,17 @@
         <v>88</v>
       </c>
       <c r="EC28" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ED28" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ED28" t="str">
+      <c r="EE28" t="str">
         <f>Tabelle1!AS28</f>
         <v>Pitts Special 1S</v>
       </c>
     </row>
-    <row r="29" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:135" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>88</v>
       </c>
@@ -19810,14 +19897,17 @@
         <v>88</v>
       </c>
       <c r="EC29" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ED29" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ED29" t="str">
+      <c r="EE29" t="str">
         <f>Tabelle1!AS29</f>
         <v>Pitts Special S2S</v>
       </c>
     </row>
-    <row r="30" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:135" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>88</v>
       </c>
@@ -20250,14 +20340,17 @@
         <v>88</v>
       </c>
       <c r="EC30" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ED30" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ED30" t="str">
+      <c r="EE30" t="str">
         <f>Tabelle1!AS30</f>
         <v>Savage Cub</v>
       </c>
     </row>
-    <row r="31" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:135" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>88</v>
       </c>
@@ -20690,14 +20783,17 @@
         <v>88</v>
       </c>
       <c r="EC31" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ED31" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ED31" t="str">
+      <c r="EE31" t="str">
         <f>Tabelle1!AS31</f>
         <v>Savage Shock Ultra</v>
       </c>
     </row>
-    <row r="32" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:135" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>88</v>
       </c>
@@ -21130,14 +21226,17 @@
         <v>88</v>
       </c>
       <c r="EC32" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ED32" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ED32" t="str">
+      <c r="EE32" t="str">
         <f>Tabelle1!AS32</f>
         <v>SR22</v>
       </c>
     </row>
-    <row r="33" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:135" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>88</v>
       </c>
@@ -21570,14 +21669,17 @@
         <v>88</v>
       </c>
       <c r="EC33" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ED33" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ED33" t="str">
+      <c r="EE33" t="str">
         <f>Tabelle1!AS33</f>
         <v>TBM 930</v>
       </c>
     </row>
-    <row r="34" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:135" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>88</v>
       </c>
@@ -22010,14 +22112,17 @@
         <v>88</v>
       </c>
       <c r="EC34" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ED34" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ED34" t="str">
+      <c r="EE34" t="str">
         <f>Tabelle1!AS34</f>
         <v>Vertigo</v>
       </c>
     </row>
-    <row r="35" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:135" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
         <v>88</v>
       </c>
@@ -22450,14 +22555,17 @@
         <v>88</v>
       </c>
       <c r="EC35" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ED35" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ED35" t="str">
+      <c r="EE35" t="str">
         <f>Tabelle1!AS35</f>
         <v>VL3</v>
       </c>
     </row>
-    <row r="36" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:135" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>88</v>
       </c>
@@ -22890,14 +22998,17 @@
         <v>88</v>
       </c>
       <c r="EC36" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ED36" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ED36" t="str">
+      <c r="EE36" t="str">
         <f>Tabelle1!AS36</f>
         <v>Volocity</v>
       </c>
     </row>
-    <row r="37" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:135" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
         <v>88</v>
       </c>
@@ -23330,14 +23441,17 @@
         <v>88</v>
       </c>
       <c r="EC37" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ED37" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ED37" t="str">
+      <c r="EE37" t="str">
         <f>Tabelle1!AS37</f>
         <v>NXCub</v>
       </c>
     </row>
-    <row r="38" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:135" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>88</v>
       </c>
@@ -23770,14 +23884,17 @@
         <v>88</v>
       </c>
       <c r="EC38" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ED38" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ED38" t="str">
+      <c r="EE38" t="str">
         <f>Tabelle1!AS38</f>
         <v>XCub</v>
       </c>
     </row>
-    <row r="39" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:135" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>88</v>
       </c>
@@ -24210,14 +24327,17 @@
         <v>88</v>
       </c>
       <c r="EC39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ED39" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ED39" t="str">
+      <c r="EE39" t="str">
         <f>Tabelle1!AS39</f>
         <v>SWS Kodiak 100 II</v>
       </c>
     </row>
-    <row r="40" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:135" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
         <v>88</v>
       </c>
@@ -24650,9 +24770,12 @@
         <v>88</v>
       </c>
       <c r="EC40" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ED40" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ED40" t="str">
+      <c r="EE40" t="str">
         <f>Tabelle1!AS40</f>
         <v>Generic Glider</v>
       </c>

</xml_diff>

<commit_message>
V 0.52-B49 - intermediate push - Add Ambient Vertical Wind Item (LIFT) - Update Ability to enter the Route via Kbd (on RTE Item)
</commit_message>
<xml_diff>
--- a/Config/EngineMerge.xlsx
+++ b/Config/EngineMerge.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4198" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4238" uniqueCount="291">
   <si>
     <t>ACFT</t>
   </si>
@@ -888,6 +888,9 @@
   </si>
   <si>
     <t>DEPARR</t>
+  </si>
+  <si>
+    <t>VWIND</t>
   </si>
 </sst>
 </file>
@@ -7081,10 +7084,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:EE40"/>
+  <dimension ref="A1:EF40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="CZ14" sqref="CZ14"/>
+      <selection activeCell="EL3" sqref="EL3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7092,11 +7095,11 @@
     <col min="1" max="75" width="3.7109375" bestFit="1" customWidth="1"/>
     <col min="76" max="77" width="3.7109375" customWidth="1"/>
     <col min="78" max="86" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="87" max="134" width="3.7109375" customWidth="1"/>
-    <col min="135" max="135" width="36.28515625" customWidth="1"/>
+    <col min="87" max="135" width="3.7109375" customWidth="1"/>
+    <col min="136" max="136" width="36.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:135" s="11" customFormat="1" ht="72" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:136" s="11" customFormat="1" ht="72" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>95</v>
       </c>
@@ -7497,13 +7500,16 @@
         <v>289</v>
       </c>
       <c r="ED1" s="11" t="s">
+        <v>290</v>
+      </c>
+      <c r="EE1" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="EE1" t="s">
+      <c r="EF1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:135" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>88</v>
       </c>
@@ -7939,14 +7945,17 @@
         <v>88</v>
       </c>
       <c r="ED2" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EE2" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EE2" t="str">
+      <c r="EF2" t="str">
         <f>Tabelle1!AS2</f>
         <v>Airbus A320 Neo</v>
       </c>
     </row>
-    <row r="3" spans="1:135" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>88</v>
       </c>
@@ -8382,14 +8391,17 @@
         <v>88</v>
       </c>
       <c r="ED3" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EE3" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EE3" t="str">
+      <c r="EF3" t="str">
         <f>Tabelle1!AS3</f>
         <v>Boeing 747-8i</v>
       </c>
     </row>
-    <row r="4" spans="1:135" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>88</v>
       </c>
@@ -8825,14 +8837,17 @@
         <v>88</v>
       </c>
       <c r="ED4" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EE4" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EE4" t="str">
+      <c r="EF4" t="str">
         <f>Tabelle1!AS4</f>
         <v>Boeing 787-10</v>
       </c>
     </row>
-    <row r="5" spans="1:135" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>88</v>
       </c>
@@ -9268,14 +9283,17 @@
         <v>88</v>
       </c>
       <c r="ED5" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EE5" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EE5" t="str">
+      <c r="EF5" t="str">
         <f>Tabelle1!AS5</f>
         <v>Boeing F/A 18E Super Hornet</v>
       </c>
     </row>
-    <row r="6" spans="1:135" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>88</v>
       </c>
@@ -9711,14 +9729,17 @@
         <v>88</v>
       </c>
       <c r="ED6" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EE6" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EE6" t="str">
+      <c r="EF6" t="str">
         <f>Tabelle1!AS6</f>
         <v>Baron G58</v>
       </c>
     </row>
-    <row r="7" spans="1:135" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>88</v>
       </c>
@@ -10154,14 +10175,17 @@
         <v>88</v>
       </c>
       <c r="ED7" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EE7" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EE7" t="str">
+      <c r="EF7" t="str">
         <f>Tabelle1!AS7</f>
         <v>Bonanza G36</v>
       </c>
     </row>
-    <row r="8" spans="1:135" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>88</v>
       </c>
@@ -10597,14 +10621,17 @@
         <v>88</v>
       </c>
       <c r="ED8" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EE8" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EE8" t="str">
+      <c r="EF8" t="str">
         <f>Tabelle1!AS8</f>
         <v>Beechcraft King Air 350i</v>
       </c>
     </row>
-    <row r="9" spans="1:135" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>88</v>
       </c>
@@ -11040,14 +11067,17 @@
         <v>88</v>
       </c>
       <c r="ED9" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EE9" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EE9" t="str">
+      <c r="EF9" t="str">
         <f>Tabelle1!AS9</f>
         <v>Cessna 152</v>
       </c>
     </row>
-    <row r="10" spans="1:135" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>88</v>
       </c>
@@ -11483,14 +11513,17 @@
         <v>88</v>
       </c>
       <c r="ED10" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EE10" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EE10" t="str">
+      <c r="EF10" t="str">
         <f>Tabelle1!AS10</f>
         <v>Cessna 152 Aero</v>
       </c>
     </row>
-    <row r="11" spans="1:135" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>88</v>
       </c>
@@ -11926,14 +11959,17 @@
         <v>88</v>
       </c>
       <c r="ED11" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EE11" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EE11" t="str">
+      <c r="EF11" t="str">
         <f>Tabelle1!AS11</f>
         <v>Cessna 172sp Skyhawk G1000</v>
       </c>
     </row>
-    <row r="12" spans="1:135" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>88</v>
       </c>
@@ -12369,14 +12405,17 @@
         <v>88</v>
       </c>
       <c r="ED12" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EE12" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EE12" t="str">
+      <c r="EF12" t="str">
         <f>Tabelle1!AS12</f>
         <v>Cessna 172sp Skyhawk</v>
       </c>
     </row>
-    <row r="13" spans="1:135" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>88</v>
       </c>
@@ -12812,14 +12851,17 @@
         <v>88</v>
       </c>
       <c r="ED13" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EE13" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EE13" t="str">
+      <c r="EF13" t="str">
         <f>Tabelle1!AS13</f>
         <v>Cessna 208B Grand Caravan EX</v>
       </c>
     </row>
-    <row r="14" spans="1:135" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>88</v>
       </c>
@@ -13255,14 +13297,17 @@
         <v>88</v>
       </c>
       <c r="ED14" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EE14" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EE14" t="str">
+      <c r="EF14" t="str">
         <f>Tabelle1!AS14</f>
         <v>Cessna CJ4 Citation</v>
       </c>
     </row>
-    <row r="15" spans="1:135" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>88</v>
       </c>
@@ -13698,14 +13743,17 @@
         <v>88</v>
       </c>
       <c r="ED15" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EE15" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EE15" t="str">
+      <c r="EF15" t="str">
         <f>Tabelle1!AS15</f>
         <v>Cessna Longitude</v>
       </c>
     </row>
-    <row r="16" spans="1:135" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>88</v>
       </c>
@@ -14141,14 +14189,17 @@
         <v>88</v>
       </c>
       <c r="ED16" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EE16" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EE16" t="str">
+      <c r="EF16" t="str">
         <f>Tabelle1!AS16</f>
         <v>DA40-NG</v>
       </c>
     </row>
-    <row r="17" spans="1:135" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>88</v>
       </c>
@@ -14584,14 +14635,17 @@
         <v>88</v>
       </c>
       <c r="ED17" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EE17" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EE17" t="str">
+      <c r="EF17" t="str">
         <f>Tabelle1!AS17</f>
         <v>DA40 TDI</v>
       </c>
     </row>
-    <row r="18" spans="1:135" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>88</v>
       </c>
@@ -15027,14 +15081,17 @@
         <v>88</v>
       </c>
       <c r="ED18" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EE18" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EE18" t="str">
+      <c r="EF18" t="str">
         <f>Tabelle1!AS18</f>
         <v>DA62</v>
       </c>
     </row>
-    <row r="19" spans="1:135" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>88</v>
       </c>
@@ -15470,14 +15527,17 @@
         <v>88</v>
       </c>
       <c r="ED19" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EE19" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EE19" t="str">
+      <c r="EF19" t="str">
         <f>Tabelle1!AS19</f>
         <v>DR400</v>
       </c>
     </row>
-    <row r="20" spans="1:135" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>88</v>
       </c>
@@ -15913,14 +15973,17 @@
         <v>88</v>
       </c>
       <c r="ED20" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EE20" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EE20" t="str">
+      <c r="EF20" t="str">
         <f>Tabelle1!AS20</f>
         <v>DV20</v>
       </c>
     </row>
-    <row r="21" spans="1:135" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>88</v>
       </c>
@@ -16356,14 +16419,17 @@
         <v>88</v>
       </c>
       <c r="ED21" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EE21" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EE21" t="str">
+      <c r="EF21" t="str">
         <f>Tabelle1!AS21</f>
         <v>Extra 330</v>
       </c>
     </row>
-    <row r="22" spans="1:135" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>88</v>
       </c>
@@ -16799,14 +16865,17 @@
         <v>88</v>
       </c>
       <c r="ED22" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EE22" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EE22" t="str">
+      <c r="EF22" t="str">
         <f>Tabelle1!AS22</f>
         <v>FlightDesignCT</v>
       </c>
     </row>
-    <row r="23" spans="1:135" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>88</v>
       </c>
@@ -17242,14 +17311,17 @@
         <v>88</v>
       </c>
       <c r="ED23" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EE23" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EE23" t="str">
+      <c r="EF23" t="str">
         <f>Tabelle1!AS23</f>
         <v>Icon A5</v>
       </c>
     </row>
-    <row r="24" spans="1:135" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>88</v>
       </c>
@@ -17685,14 +17757,17 @@
         <v>88</v>
       </c>
       <c r="ED24" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EE24" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EE24" t="str">
+      <c r="EF24" t="str">
         <f>Tabelle1!AS24</f>
         <v>Mudry Cap 10 C</v>
       </c>
     </row>
-    <row r="25" spans="1:135" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>88</v>
       </c>
@@ -18128,14 +18203,17 @@
         <v>88</v>
       </c>
       <c r="ED25" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EE25" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EE25" t="str">
+      <c r="EF25" t="str">
         <f>Tabelle1!AS25</f>
         <v>Pilatus PC-6 Gauge</v>
       </c>
     </row>
-    <row r="26" spans="1:135" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>88</v>
       </c>
@@ -18571,14 +18649,17 @@
         <v>88</v>
       </c>
       <c r="ED26" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EE26" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EE26" t="str">
+      <c r="EF26" t="str">
         <f>Tabelle1!AS26</f>
         <v>Pilatus PC-6 G950</v>
       </c>
     </row>
-    <row r="27" spans="1:135" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>88</v>
       </c>
@@ -19014,14 +19095,17 @@
         <v>88</v>
       </c>
       <c r="ED27" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EE27" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EE27" t="str">
+      <c r="EF27" t="str">
         <f>Tabelle1!AS27</f>
         <v>Pipistrel Alpha Electro</v>
       </c>
     </row>
-    <row r="28" spans="1:135" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>88</v>
       </c>
@@ -19457,14 +19541,17 @@
         <v>88</v>
       </c>
       <c r="ED28" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EE28" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EE28" t="str">
+      <c r="EF28" t="str">
         <f>Tabelle1!AS28</f>
         <v>Pitts Special 1S</v>
       </c>
     </row>
-    <row r="29" spans="1:135" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>88</v>
       </c>
@@ -19900,14 +19987,17 @@
         <v>88</v>
       </c>
       <c r="ED29" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EE29" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EE29" t="str">
+      <c r="EF29" t="str">
         <f>Tabelle1!AS29</f>
         <v>Pitts Special S2S</v>
       </c>
     </row>
-    <row r="30" spans="1:135" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>88</v>
       </c>
@@ -20343,14 +20433,17 @@
         <v>88</v>
       </c>
       <c r="ED30" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EE30" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EE30" t="str">
+      <c r="EF30" t="str">
         <f>Tabelle1!AS30</f>
         <v>Savage Cub</v>
       </c>
     </row>
-    <row r="31" spans="1:135" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>88</v>
       </c>
@@ -20786,14 +20879,17 @@
         <v>88</v>
       </c>
       <c r="ED31" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EE31" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EE31" t="str">
+      <c r="EF31" t="str">
         <f>Tabelle1!AS31</f>
         <v>Savage Shock Ultra</v>
       </c>
     </row>
-    <row r="32" spans="1:135" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>88</v>
       </c>
@@ -21229,14 +21325,17 @@
         <v>88</v>
       </c>
       <c r="ED32" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EE32" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EE32" t="str">
+      <c r="EF32" t="str">
         <f>Tabelle1!AS32</f>
         <v>SR22</v>
       </c>
     </row>
-    <row r="33" spans="1:135" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>88</v>
       </c>
@@ -21672,14 +21771,17 @@
         <v>88</v>
       </c>
       <c r="ED33" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EE33" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EE33" t="str">
+      <c r="EF33" t="str">
         <f>Tabelle1!AS33</f>
         <v>TBM 930</v>
       </c>
     </row>
-    <row r="34" spans="1:135" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>88</v>
       </c>
@@ -22115,14 +22217,17 @@
         <v>88</v>
       </c>
       <c r="ED34" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EE34" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EE34" t="str">
+      <c r="EF34" t="str">
         <f>Tabelle1!AS34</f>
         <v>Vertigo</v>
       </c>
     </row>
-    <row r="35" spans="1:135" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
         <v>88</v>
       </c>
@@ -22558,14 +22663,17 @@
         <v>88</v>
       </c>
       <c r="ED35" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EE35" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EE35" t="str">
+      <c r="EF35" t="str">
         <f>Tabelle1!AS35</f>
         <v>VL3</v>
       </c>
     </row>
-    <row r="36" spans="1:135" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>88</v>
       </c>
@@ -23001,14 +23109,17 @@
         <v>88</v>
       </c>
       <c r="ED36" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EE36" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EE36" t="str">
+      <c r="EF36" t="str">
         <f>Tabelle1!AS36</f>
         <v>Volocity</v>
       </c>
     </row>
-    <row r="37" spans="1:135" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
         <v>88</v>
       </c>
@@ -23444,14 +23555,17 @@
         <v>88</v>
       </c>
       <c r="ED37" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EE37" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EE37" t="str">
+      <c r="EF37" t="str">
         <f>Tabelle1!AS37</f>
         <v>NXCub</v>
       </c>
     </row>
-    <row r="38" spans="1:135" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>88</v>
       </c>
@@ -23887,14 +24001,17 @@
         <v>88</v>
       </c>
       <c r="ED38" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EE38" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EE38" t="str">
+      <c r="EF38" t="str">
         <f>Tabelle1!AS38</f>
         <v>XCub</v>
       </c>
     </row>
-    <row r="39" spans="1:135" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>88</v>
       </c>
@@ -24330,14 +24447,17 @@
         <v>88</v>
       </c>
       <c r="ED39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EE39" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EE39" t="str">
+      <c r="EF39" t="str">
         <f>Tabelle1!AS39</f>
         <v>SWS Kodiak 100 II</v>
       </c>
     </row>
-    <row r="40" spans="1:135" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
         <v>88</v>
       </c>
@@ -24773,9 +24893,12 @@
         <v>88</v>
       </c>
       <c r="ED40" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EE40" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EE40" t="str">
+      <c r="EF40" t="str">
         <f>Tabelle1!AS40</f>
         <v>Generic Glider</v>
       </c>

</xml_diff>

<commit_message>
V 0.52-B49 (pre-Release for testing) - Add Ambient Vertical Wind Item (LIFT) - Add Compass degm and arrow (N-up) Item - Add Altitudes, Distances can be shown in Common (default) or Metric units - Update ShowUnits is now an interactive menu setting - Update Ability to enter the Route via Kbd when no ATC plan is available (on RTE Item) - Update Complete/improve actual weights data in IAS ToolTip (Design Speed and Weights) - Update Improve capturing of mouse wheel input focus (cannot prevent a single scroll event to the Sim though) - Update QuickGuide
</commit_message>
<xml_diff>
--- a/Config/EngineMerge.xlsx
+++ b/Config/EngineMerge.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4238" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4278" uniqueCount="292">
   <si>
     <t>ACFT</t>
   </si>
@@ -891,6 +891,9 @@
   </si>
   <si>
     <t>VWIND</t>
+  </si>
+  <si>
+    <t>COMPASS</t>
   </si>
 </sst>
 </file>
@@ -7084,10 +7087,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:EF40"/>
+  <dimension ref="A1:EG40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="EL3" sqref="EL3"/>
+      <selection activeCell="EJ12" sqref="EJ12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7095,11 +7098,11 @@
     <col min="1" max="75" width="3.7109375" bestFit="1" customWidth="1"/>
     <col min="76" max="77" width="3.7109375" customWidth="1"/>
     <col min="78" max="86" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="87" max="135" width="3.7109375" customWidth="1"/>
-    <col min="136" max="136" width="36.28515625" customWidth="1"/>
+    <col min="87" max="136" width="3.7109375" customWidth="1"/>
+    <col min="137" max="137" width="36.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:136" s="11" customFormat="1" ht="72" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:137" s="11" customFormat="1" ht="72" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>95</v>
       </c>
@@ -7503,13 +7506,16 @@
         <v>290</v>
       </c>
       <c r="EE1" s="11" t="s">
+        <v>291</v>
+      </c>
+      <c r="EF1" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="EF1" t="s">
+      <c r="EG1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:137" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>88</v>
       </c>
@@ -7948,14 +7954,17 @@
         <v>88</v>
       </c>
       <c r="EE2" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EF2" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EF2" t="str">
+      <c r="EG2" t="str">
         <f>Tabelle1!AS2</f>
         <v>Airbus A320 Neo</v>
       </c>
     </row>
-    <row r="3" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:137" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>88</v>
       </c>
@@ -8394,14 +8403,17 @@
         <v>88</v>
       </c>
       <c r="EE3" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EF3" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EF3" t="str">
+      <c r="EG3" t="str">
         <f>Tabelle1!AS3</f>
         <v>Boeing 747-8i</v>
       </c>
     </row>
-    <row r="4" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:137" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>88</v>
       </c>
@@ -8840,14 +8852,17 @@
         <v>88</v>
       </c>
       <c r="EE4" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EF4" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EF4" t="str">
+      <c r="EG4" t="str">
         <f>Tabelle1!AS4</f>
         <v>Boeing 787-10</v>
       </c>
     </row>
-    <row r="5" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:137" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>88</v>
       </c>
@@ -9286,14 +9301,17 @@
         <v>88</v>
       </c>
       <c r="EE5" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EF5" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EF5" t="str">
+      <c r="EG5" t="str">
         <f>Tabelle1!AS5</f>
         <v>Boeing F/A 18E Super Hornet</v>
       </c>
     </row>
-    <row r="6" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:137" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>88</v>
       </c>
@@ -9732,14 +9750,17 @@
         <v>88</v>
       </c>
       <c r="EE6" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EF6" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EF6" t="str">
+      <c r="EG6" t="str">
         <f>Tabelle1!AS6</f>
         <v>Baron G58</v>
       </c>
     </row>
-    <row r="7" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:137" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>88</v>
       </c>
@@ -10178,14 +10199,17 @@
         <v>88</v>
       </c>
       <c r="EE7" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EF7" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EF7" t="str">
+      <c r="EG7" t="str">
         <f>Tabelle1!AS7</f>
         <v>Bonanza G36</v>
       </c>
     </row>
-    <row r="8" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:137" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>88</v>
       </c>
@@ -10624,14 +10648,17 @@
         <v>88</v>
       </c>
       <c r="EE8" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EF8" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EF8" t="str">
+      <c r="EG8" t="str">
         <f>Tabelle1!AS8</f>
         <v>Beechcraft King Air 350i</v>
       </c>
     </row>
-    <row r="9" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:137" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>88</v>
       </c>
@@ -11070,14 +11097,17 @@
         <v>88</v>
       </c>
       <c r="EE9" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EF9" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EF9" t="str">
+      <c r="EG9" t="str">
         <f>Tabelle1!AS9</f>
         <v>Cessna 152</v>
       </c>
     </row>
-    <row r="10" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:137" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>88</v>
       </c>
@@ -11516,14 +11546,17 @@
         <v>88</v>
       </c>
       <c r="EE10" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EF10" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EF10" t="str">
+      <c r="EG10" t="str">
         <f>Tabelle1!AS10</f>
         <v>Cessna 152 Aero</v>
       </c>
     </row>
-    <row r="11" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:137" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>88</v>
       </c>
@@ -11962,14 +11995,17 @@
         <v>88</v>
       </c>
       <c r="EE11" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EF11" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EF11" t="str">
+      <c r="EG11" t="str">
         <f>Tabelle1!AS11</f>
         <v>Cessna 172sp Skyhawk G1000</v>
       </c>
     </row>
-    <row r="12" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:137" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>88</v>
       </c>
@@ -12408,14 +12444,17 @@
         <v>88</v>
       </c>
       <c r="EE12" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EF12" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EF12" t="str">
+      <c r="EG12" t="str">
         <f>Tabelle1!AS12</f>
         <v>Cessna 172sp Skyhawk</v>
       </c>
     </row>
-    <row r="13" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:137" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>88</v>
       </c>
@@ -12854,14 +12893,17 @@
         <v>88</v>
       </c>
       <c r="EE13" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EF13" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EF13" t="str">
+      <c r="EG13" t="str">
         <f>Tabelle1!AS13</f>
         <v>Cessna 208B Grand Caravan EX</v>
       </c>
     </row>
-    <row r="14" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:137" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>88</v>
       </c>
@@ -13300,14 +13342,17 @@
         <v>88</v>
       </c>
       <c r="EE14" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EF14" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EF14" t="str">
+      <c r="EG14" t="str">
         <f>Tabelle1!AS14</f>
         <v>Cessna CJ4 Citation</v>
       </c>
     </row>
-    <row r="15" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:137" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>88</v>
       </c>
@@ -13746,14 +13791,17 @@
         <v>88</v>
       </c>
       <c r="EE15" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EF15" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EF15" t="str">
+      <c r="EG15" t="str">
         <f>Tabelle1!AS15</f>
         <v>Cessna Longitude</v>
       </c>
     </row>
-    <row r="16" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:137" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>88</v>
       </c>
@@ -14192,14 +14240,17 @@
         <v>88</v>
       </c>
       <c r="EE16" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EF16" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EF16" t="str">
+      <c r="EG16" t="str">
         <f>Tabelle1!AS16</f>
         <v>DA40-NG</v>
       </c>
     </row>
-    <row r="17" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:137" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>88</v>
       </c>
@@ -14638,14 +14689,17 @@
         <v>88</v>
       </c>
       <c r="EE17" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EF17" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EF17" t="str">
+      <c r="EG17" t="str">
         <f>Tabelle1!AS17</f>
         <v>DA40 TDI</v>
       </c>
     </row>
-    <row r="18" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:137" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>88</v>
       </c>
@@ -15084,14 +15138,17 @@
         <v>88</v>
       </c>
       <c r="EE18" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EF18" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EF18" t="str">
+      <c r="EG18" t="str">
         <f>Tabelle1!AS18</f>
         <v>DA62</v>
       </c>
     </row>
-    <row r="19" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:137" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>88</v>
       </c>
@@ -15530,14 +15587,17 @@
         <v>88</v>
       </c>
       <c r="EE19" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EF19" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EF19" t="str">
+      <c r="EG19" t="str">
         <f>Tabelle1!AS19</f>
         <v>DR400</v>
       </c>
     </row>
-    <row r="20" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:137" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>88</v>
       </c>
@@ -15976,14 +16036,17 @@
         <v>88</v>
       </c>
       <c r="EE20" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EF20" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EF20" t="str">
+      <c r="EG20" t="str">
         <f>Tabelle1!AS20</f>
         <v>DV20</v>
       </c>
     </row>
-    <row r="21" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:137" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>88</v>
       </c>
@@ -16422,14 +16485,17 @@
         <v>88</v>
       </c>
       <c r="EE21" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EF21" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EF21" t="str">
+      <c r="EG21" t="str">
         <f>Tabelle1!AS21</f>
         <v>Extra 330</v>
       </c>
     </row>
-    <row r="22" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:137" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>88</v>
       </c>
@@ -16868,14 +16934,17 @@
         <v>88</v>
       </c>
       <c r="EE22" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EF22" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EF22" t="str">
+      <c r="EG22" t="str">
         <f>Tabelle1!AS22</f>
         <v>FlightDesignCT</v>
       </c>
     </row>
-    <row r="23" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:137" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>88</v>
       </c>
@@ -17314,14 +17383,17 @@
         <v>88</v>
       </c>
       <c r="EE23" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EF23" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EF23" t="str">
+      <c r="EG23" t="str">
         <f>Tabelle1!AS23</f>
         <v>Icon A5</v>
       </c>
     </row>
-    <row r="24" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:137" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>88</v>
       </c>
@@ -17760,14 +17832,17 @@
         <v>88</v>
       </c>
       <c r="EE24" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EF24" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EF24" t="str">
+      <c r="EG24" t="str">
         <f>Tabelle1!AS24</f>
         <v>Mudry Cap 10 C</v>
       </c>
     </row>
-    <row r="25" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:137" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>88</v>
       </c>
@@ -18206,14 +18281,17 @@
         <v>88</v>
       </c>
       <c r="EE25" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EF25" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EF25" t="str">
+      <c r="EG25" t="str">
         <f>Tabelle1!AS25</f>
         <v>Pilatus PC-6 Gauge</v>
       </c>
     </row>
-    <row r="26" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:137" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>88</v>
       </c>
@@ -18652,14 +18730,17 @@
         <v>88</v>
       </c>
       <c r="EE26" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EF26" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EF26" t="str">
+      <c r="EG26" t="str">
         <f>Tabelle1!AS26</f>
         <v>Pilatus PC-6 G950</v>
       </c>
     </row>
-    <row r="27" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:137" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>88</v>
       </c>
@@ -19098,14 +19179,17 @@
         <v>88</v>
       </c>
       <c r="EE27" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EF27" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EF27" t="str">
+      <c r="EG27" t="str">
         <f>Tabelle1!AS27</f>
         <v>Pipistrel Alpha Electro</v>
       </c>
     </row>
-    <row r="28" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:137" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>88</v>
       </c>
@@ -19544,14 +19628,17 @@
         <v>88</v>
       </c>
       <c r="EE28" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EF28" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EF28" t="str">
+      <c r="EG28" t="str">
         <f>Tabelle1!AS28</f>
         <v>Pitts Special 1S</v>
       </c>
     </row>
-    <row r="29" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:137" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>88</v>
       </c>
@@ -19990,14 +20077,17 @@
         <v>88</v>
       </c>
       <c r="EE29" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EF29" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EF29" t="str">
+      <c r="EG29" t="str">
         <f>Tabelle1!AS29</f>
         <v>Pitts Special S2S</v>
       </c>
     </row>
-    <row r="30" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:137" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>88</v>
       </c>
@@ -20436,14 +20526,17 @@
         <v>88</v>
       </c>
       <c r="EE30" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EF30" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EF30" t="str">
+      <c r="EG30" t="str">
         <f>Tabelle1!AS30</f>
         <v>Savage Cub</v>
       </c>
     </row>
-    <row r="31" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:137" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>88</v>
       </c>
@@ -20882,14 +20975,17 @@
         <v>88</v>
       </c>
       <c r="EE31" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EF31" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EF31" t="str">
+      <c r="EG31" t="str">
         <f>Tabelle1!AS31</f>
         <v>Savage Shock Ultra</v>
       </c>
     </row>
-    <row r="32" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:137" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>88</v>
       </c>
@@ -21328,14 +21424,17 @@
         <v>88</v>
       </c>
       <c r="EE32" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EF32" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EF32" t="str">
+      <c r="EG32" t="str">
         <f>Tabelle1!AS32</f>
         <v>SR22</v>
       </c>
     </row>
-    <row r="33" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:137" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>88</v>
       </c>
@@ -21774,14 +21873,17 @@
         <v>88</v>
       </c>
       <c r="EE33" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EF33" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EF33" t="str">
+      <c r="EG33" t="str">
         <f>Tabelle1!AS33</f>
         <v>TBM 930</v>
       </c>
     </row>
-    <row r="34" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:137" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>88</v>
       </c>
@@ -22220,14 +22322,17 @@
         <v>88</v>
       </c>
       <c r="EE34" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EF34" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EF34" t="str">
+      <c r="EG34" t="str">
         <f>Tabelle1!AS34</f>
         <v>Vertigo</v>
       </c>
     </row>
-    <row r="35" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:137" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
         <v>88</v>
       </c>
@@ -22666,14 +22771,17 @@
         <v>88</v>
       </c>
       <c r="EE35" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EF35" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EF35" t="str">
+      <c r="EG35" t="str">
         <f>Tabelle1!AS35</f>
         <v>VL3</v>
       </c>
     </row>
-    <row r="36" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:137" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>88</v>
       </c>
@@ -23112,14 +23220,17 @@
         <v>88</v>
       </c>
       <c r="EE36" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EF36" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EF36" t="str">
+      <c r="EG36" t="str">
         <f>Tabelle1!AS36</f>
         <v>Volocity</v>
       </c>
     </row>
-    <row r="37" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:137" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
         <v>88</v>
       </c>
@@ -23558,14 +23669,17 @@
         <v>88</v>
       </c>
       <c r="EE37" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EF37" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EF37" t="str">
+      <c r="EG37" t="str">
         <f>Tabelle1!AS37</f>
         <v>NXCub</v>
       </c>
     </row>
-    <row r="38" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:137" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>88</v>
       </c>
@@ -24004,14 +24118,17 @@
         <v>88</v>
       </c>
       <c r="EE38" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EF38" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EF38" t="str">
+      <c r="EG38" t="str">
         <f>Tabelle1!AS38</f>
         <v>XCub</v>
       </c>
     </row>
-    <row r="39" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:137" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>88</v>
       </c>
@@ -24450,14 +24567,17 @@
         <v>88</v>
       </c>
       <c r="EE39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EF39" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EF39" t="str">
+      <c r="EG39" t="str">
         <f>Tabelle1!AS39</f>
         <v>SWS Kodiak 100 II</v>
       </c>
     </row>
-    <row r="40" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:137" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
         <v>88</v>
       </c>
@@ -24896,9 +25016,12 @@
         <v>88</v>
       </c>
       <c r="EE40" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EF40" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EF40" t="str">
+      <c r="EG40" t="str">
         <f>Tabelle1!AS40</f>
         <v>Generic Glider</v>
       </c>

</xml_diff>

<commit_message>
V 0.53-B50 - final testing - Add Checklist Box as independent feature - Add ADF(1 only) Items Freq, Name, ID + Bearing + Needle - Add Distance to Destination item (calculated or from FPLan) - Add Scroll Wheel Inc/Dec for SimRate - Fix Some memory disposal of unused resources - Update QuickGuide
</commit_message>
<xml_diff>
--- a/Config/EngineMerge.xlsx
+++ b/Config/EngineMerge.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4278" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4438" uniqueCount="296">
   <si>
     <t>ACFT</t>
   </si>
@@ -894,6 +894,18 @@
   </si>
   <si>
     <t>COMPASS</t>
+  </si>
+  <si>
+    <t>GPS_DST</t>
+  </si>
+  <si>
+    <t>ADF1</t>
+  </si>
+  <si>
+    <t>ADF1_NAME</t>
+  </si>
+  <si>
+    <t>ADF1_F</t>
   </si>
 </sst>
 </file>
@@ -7087,10 +7099,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:EG40"/>
+  <dimension ref="A1:EK40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="EJ12" sqref="EJ12"/>
+      <selection activeCell="EL34" sqref="EL34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7098,11 +7110,11 @@
     <col min="1" max="75" width="3.7109375" bestFit="1" customWidth="1"/>
     <col min="76" max="77" width="3.7109375" customWidth="1"/>
     <col min="78" max="86" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="87" max="136" width="3.7109375" customWidth="1"/>
-    <col min="137" max="137" width="36.28515625" customWidth="1"/>
+    <col min="87" max="140" width="3.7109375" customWidth="1"/>
+    <col min="141" max="141" width="36.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:137" s="11" customFormat="1" ht="72" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:141" s="11" customFormat="1" ht="72" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>95</v>
       </c>
@@ -7509,13 +7521,25 @@
         <v>291</v>
       </c>
       <c r="EF1" s="11" t="s">
+        <v>292</v>
+      </c>
+      <c r="EG1" s="11" t="s">
+        <v>293</v>
+      </c>
+      <c r="EH1" s="11" t="s">
+        <v>294</v>
+      </c>
+      <c r="EI1" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="EJ1" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="EG1" t="s">
+      <c r="EK1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:137" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:141" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>88</v>
       </c>
@@ -7957,14 +7981,26 @@
         <v>88</v>
       </c>
       <c r="EF2" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EG2" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EH2" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EI2" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EJ2" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EG2" t="str">
+      <c r="EK2" t="str">
         <f>Tabelle1!AS2</f>
         <v>Airbus A320 Neo</v>
       </c>
     </row>
-    <row r="3" spans="1:137" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:141" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>88</v>
       </c>
@@ -8406,14 +8442,26 @@
         <v>88</v>
       </c>
       <c r="EF3" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EG3" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EH3" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EI3" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EJ3" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EG3" t="str">
+      <c r="EK3" t="str">
         <f>Tabelle1!AS3</f>
         <v>Boeing 747-8i</v>
       </c>
     </row>
-    <row r="4" spans="1:137" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:141" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>88</v>
       </c>
@@ -8855,14 +8903,26 @@
         <v>88</v>
       </c>
       <c r="EF4" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EG4" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EH4" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EI4" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EJ4" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EG4" t="str">
+      <c r="EK4" t="str">
         <f>Tabelle1!AS4</f>
         <v>Boeing 787-10</v>
       </c>
     </row>
-    <row r="5" spans="1:137" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:141" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>88</v>
       </c>
@@ -9304,14 +9364,26 @@
         <v>88</v>
       </c>
       <c r="EF5" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EG5" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EH5" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EI5" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EJ5" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EG5" t="str">
+      <c r="EK5" t="str">
         <f>Tabelle1!AS5</f>
         <v>Boeing F/A 18E Super Hornet</v>
       </c>
     </row>
-    <row r="6" spans="1:137" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:141" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>88</v>
       </c>
@@ -9753,14 +9825,26 @@
         <v>88</v>
       </c>
       <c r="EF6" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EG6" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EH6" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EI6" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EJ6" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EG6" t="str">
+      <c r="EK6" t="str">
         <f>Tabelle1!AS6</f>
         <v>Baron G58</v>
       </c>
     </row>
-    <row r="7" spans="1:137" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:141" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>88</v>
       </c>
@@ -10202,14 +10286,26 @@
         <v>88</v>
       </c>
       <c r="EF7" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EG7" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EH7" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EI7" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EJ7" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EG7" t="str">
+      <c r="EK7" t="str">
         <f>Tabelle1!AS7</f>
         <v>Bonanza G36</v>
       </c>
     </row>
-    <row r="8" spans="1:137" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:141" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>88</v>
       </c>
@@ -10651,14 +10747,26 @@
         <v>88</v>
       </c>
       <c r="EF8" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EG8" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EH8" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EI8" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EJ8" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EG8" t="str">
+      <c r="EK8" t="str">
         <f>Tabelle1!AS8</f>
         <v>Beechcraft King Air 350i</v>
       </c>
     </row>
-    <row r="9" spans="1:137" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:141" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>88</v>
       </c>
@@ -11100,14 +11208,26 @@
         <v>88</v>
       </c>
       <c r="EF9" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EG9" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EH9" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EI9" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EJ9" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EG9" t="str">
+      <c r="EK9" t="str">
         <f>Tabelle1!AS9</f>
         <v>Cessna 152</v>
       </c>
     </row>
-    <row r="10" spans="1:137" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:141" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>88</v>
       </c>
@@ -11549,14 +11669,26 @@
         <v>88</v>
       </c>
       <c r="EF10" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EG10" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EH10" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EI10" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EJ10" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EG10" t="str">
+      <c r="EK10" t="str">
         <f>Tabelle1!AS10</f>
         <v>Cessna 152 Aero</v>
       </c>
     </row>
-    <row r="11" spans="1:137" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:141" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>88</v>
       </c>
@@ -11998,14 +12130,26 @@
         <v>88</v>
       </c>
       <c r="EF11" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EG11" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EH11" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EI11" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EJ11" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EG11" t="str">
+      <c r="EK11" t="str">
         <f>Tabelle1!AS11</f>
         <v>Cessna 172sp Skyhawk G1000</v>
       </c>
     </row>
-    <row r="12" spans="1:137" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:141" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>88</v>
       </c>
@@ -12447,14 +12591,26 @@
         <v>88</v>
       </c>
       <c r="EF12" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EG12" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EH12" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EI12" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EJ12" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EG12" t="str">
+      <c r="EK12" t="str">
         <f>Tabelle1!AS12</f>
         <v>Cessna 172sp Skyhawk</v>
       </c>
     </row>
-    <row r="13" spans="1:137" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:141" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>88</v>
       </c>
@@ -12896,14 +13052,26 @@
         <v>88</v>
       </c>
       <c r="EF13" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EG13" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EH13" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EI13" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EJ13" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EG13" t="str">
+      <c r="EK13" t="str">
         <f>Tabelle1!AS13</f>
         <v>Cessna 208B Grand Caravan EX</v>
       </c>
     </row>
-    <row r="14" spans="1:137" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:141" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>88</v>
       </c>
@@ -13345,14 +13513,26 @@
         <v>88</v>
       </c>
       <c r="EF14" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EG14" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EH14" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EI14" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EJ14" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EG14" t="str">
+      <c r="EK14" t="str">
         <f>Tabelle1!AS14</f>
         <v>Cessna CJ4 Citation</v>
       </c>
     </row>
-    <row r="15" spans="1:137" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:141" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>88</v>
       </c>
@@ -13794,14 +13974,26 @@
         <v>88</v>
       </c>
       <c r="EF15" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EG15" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EH15" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EI15" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EJ15" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EG15" t="str">
+      <c r="EK15" t="str">
         <f>Tabelle1!AS15</f>
         <v>Cessna Longitude</v>
       </c>
     </row>
-    <row r="16" spans="1:137" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:141" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>88</v>
       </c>
@@ -14243,14 +14435,26 @@
         <v>88</v>
       </c>
       <c r="EF16" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EG16" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EH16" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EI16" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EJ16" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EG16" t="str">
+      <c r="EK16" t="str">
         <f>Tabelle1!AS16</f>
         <v>DA40-NG</v>
       </c>
     </row>
-    <row r="17" spans="1:137" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:141" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>88</v>
       </c>
@@ -14692,14 +14896,26 @@
         <v>88</v>
       </c>
       <c r="EF17" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EG17" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EH17" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EI17" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EJ17" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EG17" t="str">
+      <c r="EK17" t="str">
         <f>Tabelle1!AS17</f>
         <v>DA40 TDI</v>
       </c>
     </row>
-    <row r="18" spans="1:137" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:141" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>88</v>
       </c>
@@ -15141,14 +15357,26 @@
         <v>88</v>
       </c>
       <c r="EF18" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EG18" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EH18" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EI18" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EJ18" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EG18" t="str">
+      <c r="EK18" t="str">
         <f>Tabelle1!AS18</f>
         <v>DA62</v>
       </c>
     </row>
-    <row r="19" spans="1:137" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:141" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>88</v>
       </c>
@@ -15590,14 +15818,26 @@
         <v>88</v>
       </c>
       <c r="EF19" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EG19" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EH19" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EI19" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EJ19" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EG19" t="str">
+      <c r="EK19" t="str">
         <f>Tabelle1!AS19</f>
         <v>DR400</v>
       </c>
     </row>
-    <row r="20" spans="1:137" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:141" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>88</v>
       </c>
@@ -16039,14 +16279,26 @@
         <v>88</v>
       </c>
       <c r="EF20" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EG20" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EH20" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EI20" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EJ20" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EG20" t="str">
+      <c r="EK20" t="str">
         <f>Tabelle1!AS20</f>
         <v>DV20</v>
       </c>
     </row>
-    <row r="21" spans="1:137" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:141" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>88</v>
       </c>
@@ -16488,14 +16740,26 @@
         <v>88</v>
       </c>
       <c r="EF21" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EG21" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EH21" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EI21" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EJ21" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EG21" t="str">
+      <c r="EK21" t="str">
         <f>Tabelle1!AS21</f>
         <v>Extra 330</v>
       </c>
     </row>
-    <row r="22" spans="1:137" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:141" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>88</v>
       </c>
@@ -16937,14 +17201,26 @@
         <v>88</v>
       </c>
       <c r="EF22" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EG22" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EH22" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EI22" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EJ22" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EG22" t="str">
+      <c r="EK22" t="str">
         <f>Tabelle1!AS22</f>
         <v>FlightDesignCT</v>
       </c>
     </row>
-    <row r="23" spans="1:137" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:141" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>88</v>
       </c>
@@ -17386,14 +17662,26 @@
         <v>88</v>
       </c>
       <c r="EF23" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EG23" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EH23" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EI23" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EJ23" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EG23" t="str">
+      <c r="EK23" t="str">
         <f>Tabelle1!AS23</f>
         <v>Icon A5</v>
       </c>
     </row>
-    <row r="24" spans="1:137" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:141" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>88</v>
       </c>
@@ -17835,14 +18123,26 @@
         <v>88</v>
       </c>
       <c r="EF24" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EG24" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EH24" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EI24" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EJ24" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EG24" t="str">
+      <c r="EK24" t="str">
         <f>Tabelle1!AS24</f>
         <v>Mudry Cap 10 C</v>
       </c>
     </row>
-    <row r="25" spans="1:137" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:141" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>88</v>
       </c>
@@ -18284,14 +18584,26 @@
         <v>88</v>
       </c>
       <c r="EF25" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EG25" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EH25" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EI25" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EJ25" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EG25" t="str">
+      <c r="EK25" t="str">
         <f>Tabelle1!AS25</f>
         <v>Pilatus PC-6 Gauge</v>
       </c>
     </row>
-    <row r="26" spans="1:137" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:141" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>88</v>
       </c>
@@ -18733,14 +19045,26 @@
         <v>88</v>
       </c>
       <c r="EF26" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EG26" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EH26" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EI26" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EJ26" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EG26" t="str">
+      <c r="EK26" t="str">
         <f>Tabelle1!AS26</f>
         <v>Pilatus PC-6 G950</v>
       </c>
     </row>
-    <row r="27" spans="1:137" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:141" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>88</v>
       </c>
@@ -19182,14 +19506,26 @@
         <v>88</v>
       </c>
       <c r="EF27" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EG27" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EH27" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EI27" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EJ27" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EG27" t="str">
+      <c r="EK27" t="str">
         <f>Tabelle1!AS27</f>
         <v>Pipistrel Alpha Electro</v>
       </c>
     </row>
-    <row r="28" spans="1:137" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:141" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>88</v>
       </c>
@@ -19631,14 +19967,26 @@
         <v>88</v>
       </c>
       <c r="EF28" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EG28" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EH28" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EI28" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EJ28" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EG28" t="str">
+      <c r="EK28" t="str">
         <f>Tabelle1!AS28</f>
         <v>Pitts Special 1S</v>
       </c>
     </row>
-    <row r="29" spans="1:137" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:141" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>88</v>
       </c>
@@ -20080,14 +20428,26 @@
         <v>88</v>
       </c>
       <c r="EF29" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EG29" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EH29" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EI29" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EJ29" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EG29" t="str">
+      <c r="EK29" t="str">
         <f>Tabelle1!AS29</f>
         <v>Pitts Special S2S</v>
       </c>
     </row>
-    <row r="30" spans="1:137" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:141" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>88</v>
       </c>
@@ -20529,14 +20889,26 @@
         <v>88</v>
       </c>
       <c r="EF30" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EG30" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EH30" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EI30" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EJ30" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EG30" t="str">
+      <c r="EK30" t="str">
         <f>Tabelle1!AS30</f>
         <v>Savage Cub</v>
       </c>
     </row>
-    <row r="31" spans="1:137" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:141" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>88</v>
       </c>
@@ -20978,14 +21350,26 @@
         <v>88</v>
       </c>
       <c r="EF31" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EG31" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EH31" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EI31" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EJ31" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EG31" t="str">
+      <c r="EK31" t="str">
         <f>Tabelle1!AS31</f>
         <v>Savage Shock Ultra</v>
       </c>
     </row>
-    <row r="32" spans="1:137" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:141" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>88</v>
       </c>
@@ -21427,14 +21811,26 @@
         <v>88</v>
       </c>
       <c r="EF32" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EG32" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EH32" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EI32" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EJ32" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EG32" t="str">
+      <c r="EK32" t="str">
         <f>Tabelle1!AS32</f>
         <v>SR22</v>
       </c>
     </row>
-    <row r="33" spans="1:137" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:141" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>88</v>
       </c>
@@ -21876,14 +22272,26 @@
         <v>88</v>
       </c>
       <c r="EF33" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EG33" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EH33" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EI33" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EJ33" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EG33" t="str">
+      <c r="EK33" t="str">
         <f>Tabelle1!AS33</f>
         <v>TBM 930</v>
       </c>
     </row>
-    <row r="34" spans="1:137" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:141" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>88</v>
       </c>
@@ -22325,14 +22733,26 @@
         <v>88</v>
       </c>
       <c r="EF34" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EG34" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EH34" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EI34" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EJ34" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EG34" t="str">
+      <c r="EK34" t="str">
         <f>Tabelle1!AS34</f>
         <v>Vertigo</v>
       </c>
     </row>
-    <row r="35" spans="1:137" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:141" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
         <v>88</v>
       </c>
@@ -22774,14 +23194,26 @@
         <v>88</v>
       </c>
       <c r="EF35" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EG35" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EH35" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EI35" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EJ35" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EG35" t="str">
+      <c r="EK35" t="str">
         <f>Tabelle1!AS35</f>
         <v>VL3</v>
       </c>
     </row>
-    <row r="36" spans="1:137" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:141" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>88</v>
       </c>
@@ -23223,14 +23655,26 @@
         <v>88</v>
       </c>
       <c r="EF36" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EG36" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EH36" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EI36" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EJ36" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EG36" t="str">
+      <c r="EK36" t="str">
         <f>Tabelle1!AS36</f>
         <v>Volocity</v>
       </c>
     </row>
-    <row r="37" spans="1:137" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:141" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
         <v>88</v>
       </c>
@@ -23672,14 +24116,26 @@
         <v>88</v>
       </c>
       <c r="EF37" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EG37" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EH37" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EI37" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EJ37" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EG37" t="str">
+      <c r="EK37" t="str">
         <f>Tabelle1!AS37</f>
         <v>NXCub</v>
       </c>
     </row>
-    <row r="38" spans="1:137" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:141" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>88</v>
       </c>
@@ -24121,14 +24577,26 @@
         <v>88</v>
       </c>
       <c r="EF38" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EG38" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EH38" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EI38" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EJ38" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EG38" t="str">
+      <c r="EK38" t="str">
         <f>Tabelle1!AS38</f>
         <v>XCub</v>
       </c>
     </row>
-    <row r="39" spans="1:137" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:141" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>88</v>
       </c>
@@ -24570,14 +25038,26 @@
         <v>88</v>
       </c>
       <c r="EF39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EG39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EH39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EI39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EJ39" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EG39" t="str">
+      <c r="EK39" t="str">
         <f>Tabelle1!AS39</f>
         <v>SWS Kodiak 100 II</v>
       </c>
     </row>
-    <row r="40" spans="1:137" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:141" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
         <v>88</v>
       </c>
@@ -25019,9 +25499,21 @@
         <v>88</v>
       </c>
       <c r="EF40" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EG40" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EH40" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EI40" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EJ40" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EG40" t="str">
+      <c r="EK40" t="str">
         <f>Tabelle1!AS40</f>
         <v>Generic Glider</v>
       </c>

</xml_diff>